<commit_message>
updated .gitignore to include temp xl files
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\Ma'ayan Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EA31CA-15EC-451D-BA47-4BBDF6E9BA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882351F-3D25-47AE-AE4E-A648ADD79936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -553,7 +553,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,8 +610,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +645,12 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -648,15 +661,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -667,8 +681,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1010,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2103,7 @@
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F45">
@@ -2110,7 +2126,7 @@
       <c r="A46" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>56</v>
       </c>
       <c r="F46">
@@ -2133,7 +2149,7 @@
       <c r="A47" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>57</v>
       </c>
       <c r="F47">
@@ -2156,7 +2172,7 @@
       <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F48">

</xml_diff>

<commit_message>
added sparse jaccard functionality
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882351F-3D25-47AE-AE4E-A648ADD79936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840AB6FE-1B3E-45DA-99BA-671A8ACFFCC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -553,7 +553,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,13 +591,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -661,16 +654,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -678,21 +670,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+  <cellStyles count="6">
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -708,8 +731,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE186E64-132B-4E6F-BBD5-769A36DC41A2}" name="Table1" displayName="Table1" ref="A1:J120" totalsRowShown="0">
   <autoFilter ref="A1:J120" xr:uid="{5D1A7ADB-D789-4B9C-BF75-B396CFD6A519}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J120">
-    <sortCondition ref="A1:A120"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J77">
+    <sortCondition ref="B1:B120"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AFD3E64B-E874-4397-A348-505BB47ED81A}" name="Resource"/>
@@ -1024,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,10 +1062,11 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1098,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1087,7 +1111,7 @@
       <c r="D2">
         <v>216</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
         <v>131173</v>
       </c>
       <c r="F2">
@@ -1102,8 +1126,12 @@
       <c r="I2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>IF(COUNTA(E2),E2/H2,1)</f>
+        <v>4.9456992214952963E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1122,8 +1150,12 @@
       <c r="I3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="0">IF(COUNTA(E3),E3/H3,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1142,8 +1174,12 @@
       <c r="I4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1174,8 +1210,12 @@
       <c r="J5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1.1491851532773349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1206,37 +1246,36 @@
       <c r="J6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1.2597183797971199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>16632</v>
-      </c>
-      <c r="D7">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="F7">
-        <v>16827</v>
+        <v>18535</v>
       </c>
       <c r="G7">
-        <v>27</v>
+        <v>2826</v>
       </c>
       <c r="H7">
-        <v>27015</v>
+        <v>829693</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1264,131 +1303,165 @@
       <c r="I8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.98823356056177436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>16632</v>
+      </c>
+      <c r="D9">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>169</v>
       </c>
       <c r="F9">
         <v>16827</v>
       </c>
       <c r="G9">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9">
-        <v>33653</v>
+        <v>27015</v>
       </c>
       <c r="I9" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>22411</v>
+        <v>16827</v>
       </c>
       <c r="G10">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H10">
-        <v>44822</v>
+        <v>33653</v>
       </c>
       <c r="I10" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>22411</v>
       </c>
       <c r="G11">
-        <v>524</v>
+        <v>31</v>
       </c>
       <c r="H11">
-        <v>587286</v>
+        <v>44822</v>
       </c>
       <c r="I11" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <v>22411</v>
       </c>
       <c r="G12">
-        <v>26</v>
+        <v>524</v>
       </c>
       <c r="H12">
-        <v>44822</v>
+        <v>587286</v>
       </c>
       <c r="I12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F13">
-        <v>19281</v>
+        <v>22411</v>
       </c>
       <c r="G13">
-        <v>1198</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>1156878</v>
+        <v>44822</v>
       </c>
       <c r="I13" t="s">
         <v>147</v>
       </c>
-      <c r="J13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="F14">
-        <v>19281</v>
+        <v>13149</v>
       </c>
       <c r="G14">
-        <v>516</v>
+        <v>3679</v>
       </c>
       <c r="H14">
-        <v>501308</v>
+        <v>52079</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1407,8 +1480,12 @@
       <c r="I15" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1427,8 +1504,12 @@
       <c r="I16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1447,8 +1528,12 @@
       <c r="I17" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1467,8 +1552,12 @@
       <c r="I18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1487,8 +1576,12 @@
       <c r="I19" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1516,8 +1609,12 @@
       <c r="I20" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>1.1124590011722242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1545,13 +1642,26 @@
       <c r="I21" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>1.0990330203911971</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="C22">
+        <v>34500</v>
+      </c>
+      <c r="D22">
+        <v>1145</v>
+      </c>
+      <c r="E22">
+        <v>16703711</v>
       </c>
       <c r="F22">
         <v>34668</v>
@@ -1565,8 +1675,12 @@
       <c r="I22" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>1.114833657720123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1594,8 +1708,12 @@
       <c r="I23" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>1.3284207830720616</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1623,8 +1741,12 @@
       <c r="I24" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>1.5375814570097672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1655,8 +1777,12 @@
       <c r="J25" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>1.2280596203815786</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1684,8 +1810,12 @@
       <c r="I26" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>2.6712613392554672</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1713,8 +1843,12 @@
       <c r="I27" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>2.6848416289592758</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1742,8 +1876,12 @@
       <c r="I28" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>3.060516329346826</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1771,8 +1909,12 @@
       <c r="I29" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>0.25318885638449057</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1800,12 +1942,16 @@
       <c r="I30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0.19129584566160401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" t="s">
         <v>28</v>
       </c>
       <c r="F31">
@@ -1817,8 +1963,12 @@
       <c r="J31" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1846,8 +1996,12 @@
       <c r="I32" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>1.0505577739180261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1866,8 +2020,12 @@
       <c r="I33" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1886,8 +2044,12 @@
       <c r="I34" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1906,8 +2068,12 @@
       <c r="I35" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1926,8 +2092,12 @@
       <c r="I36" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1946,8 +2116,12 @@
       <c r="I37" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1966,8 +2140,12 @@
       <c r="I38" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1986,8 +2164,12 @@
       <c r="I39" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2006,8 +2188,12 @@
       <c r="I40" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2029,8 +2215,12 @@
       <c r="J41" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2052,8 +2242,12 @@
       <c r="J42" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2075,8 +2269,12 @@
       <c r="J43" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2098,12 +2296,16 @@
       <c r="J44" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F45">
@@ -2121,12 +2323,16 @@
       <c r="J45" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="8" t="s">
         <v>56</v>
       </c>
       <c r="F46">
@@ -2144,12 +2350,16 @@
       <c r="J46" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F47">
@@ -2167,12 +2377,16 @@
       <c r="J47" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F48">
@@ -2190,8 +2404,12 @@
       <c r="J48" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2210,11 +2428,15 @@
       <c r="I49" t="s">
         <v>148</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="J49" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -2233,11 +2455,15 @@
       <c r="I50" t="s">
         <v>148</v>
       </c>
-      <c r="J50" s="8" t="s">
+      <c r="J50" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2256,8 +2482,12 @@
       <c r="I51" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2285,8 +2515,12 @@
       <c r="I52" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>1.0052430405969</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -2314,8 +2548,12 @@
       <c r="I53" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>1.0036775901243822</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -2334,8 +2572,12 @@
       <c r="I54" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -2354,8 +2596,12 @@
       <c r="I55" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -2374,8 +2620,12 @@
       <c r="I56" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -2397,8 +2647,12 @@
       <c r="J57" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2420,8 +2674,12 @@
       <c r="J58" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -2443,8 +2701,12 @@
       <c r="J59" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -2454,8 +2716,12 @@
       <c r="I60" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -2474,8 +2740,12 @@
       <c r="I61" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -2494,8 +2764,12 @@
       <c r="I62" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -2523,8 +2797,12 @@
       <c r="I63" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <f t="shared" si="0"/>
+        <v>1.2855585434988008</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -2552,8 +2830,12 @@
       <c r="I64" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <f t="shared" si="0"/>
+        <v>2.0093676814988291</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2581,12 +2863,16 @@
       <c r="I65" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <f t="shared" si="0"/>
+        <v>5.7080381398817455</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" t="s">
         <v>81</v>
       </c>
       <c r="F66">
@@ -2604,12 +2890,16 @@
       <c r="J66" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" t="s">
         <v>82</v>
       </c>
       <c r="F67">
@@ -2627,8 +2917,12 @@
       <c r="J67" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <f t="shared" ref="L67:L120" si="1">IF(COUNTA(E67),E67/H67,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -2656,8 +2950,12 @@
       <c r="I68" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <f t="shared" si="1"/>
+        <v>1.3892684335957246</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -2676,68 +2974,87 @@
       <c r="I69" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F70">
-        <v>18535</v>
+        <v>11164</v>
       </c>
       <c r="G70">
-        <v>2826</v>
+        <v>51319</v>
       </c>
       <c r="H70">
-        <v>829693</v>
+        <v>1257932</v>
       </c>
       <c r="I70" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="F71">
-        <v>13149</v>
+        <v>19281</v>
       </c>
       <c r="G71">
-        <v>3679</v>
+        <v>1198</v>
       </c>
       <c r="H71">
-        <v>52079</v>
+        <v>1156878</v>
       </c>
       <c r="I71" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="J71" t="s">
+        <v>158</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="F72">
-        <v>18565</v>
+        <v>19281</v>
       </c>
       <c r="G72">
-        <v>4098</v>
+        <v>516</v>
       </c>
       <c r="H72">
-        <v>434311</v>
+        <v>501308</v>
       </c>
       <c r="I72" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>89</v>
       </c>
@@ -2765,8 +3082,12 @@
       <c r="I73" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <f t="shared" si="1"/>
+        <v>1.1916106184155706</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>159</v>
       </c>
@@ -2782,8 +3103,12 @@
       <c r="E74" s="5">
         <v>7641</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -2802,48 +3127,60 @@
       <c r="I75" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>92</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F76">
-        <v>11164</v>
+        <v>16291</v>
       </c>
       <c r="G76">
-        <v>51319</v>
+        <v>18511</v>
       </c>
       <c r="H76">
-        <v>1257932</v>
+        <v>1125042</v>
       </c>
       <c r="I76" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F77">
-        <v>16291</v>
+        <v>18565</v>
       </c>
       <c r="G77">
-        <v>18511</v>
+        <v>4098</v>
       </c>
       <c r="H77">
-        <v>1125042</v>
+        <v>434311</v>
       </c>
       <c r="I77" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>95</v>
       </c>
@@ -2856,8 +3193,12 @@
       <c r="I78" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>151</v>
       </c>
@@ -2867,8 +3208,12 @@
       <c r="I79" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>96</v>
       </c>
@@ -2896,8 +3241,12 @@
       <c r="I80" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <f t="shared" si="1"/>
+        <v>1.0779775664102467</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>97</v>
       </c>
@@ -2916,8 +3265,12 @@
       <c r="I81" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>99</v>
       </c>
@@ -2936,8 +3289,12 @@
       <c r="I82" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -2956,11 +3313,15 @@
       <c r="I83" t="s">
         <v>147</v>
       </c>
-      <c r="J83" s="8" t="s">
+      <c r="J83" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>100</v>
       </c>
@@ -2979,11 +3340,15 @@
       <c r="I84" t="s">
         <v>147</v>
       </c>
-      <c r="J84" s="8" t="s">
+      <c r="J84" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -3002,11 +3367,15 @@
       <c r="I85" t="s">
         <v>147</v>
       </c>
-      <c r="J85" s="8" t="s">
+      <c r="J85" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -3025,11 +3394,15 @@
       <c r="I86" t="s">
         <v>147</v>
       </c>
-      <c r="J86" s="8" t="s">
+      <c r="J86" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>100</v>
       </c>
@@ -3048,11 +3421,15 @@
       <c r="I87" t="s">
         <v>147</v>
       </c>
-      <c r="J87" s="8" t="s">
+      <c r="J87" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -3071,11 +3448,15 @@
       <c r="I88" t="s">
         <v>147</v>
       </c>
-      <c r="J88" s="8" t="s">
+      <c r="J88" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -3094,11 +3475,15 @@
       <c r="I89" t="s">
         <v>147</v>
       </c>
-      <c r="J89" s="8" t="s">
+      <c r="J89" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>100</v>
       </c>
@@ -3117,11 +3502,15 @@
       <c r="I90" t="s">
         <v>147</v>
       </c>
-      <c r="J90" s="8" t="s">
+      <c r="J90" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -3140,11 +3529,15 @@
       <c r="I91" t="s">
         <v>147</v>
       </c>
-      <c r="J91" s="8" t="s">
+      <c r="J91" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -3163,11 +3556,15 @@
       <c r="I92" t="s">
         <v>147</v>
       </c>
-      <c r="J92" s="8" t="s">
+      <c r="J92" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -3186,11 +3583,15 @@
       <c r="I93" t="s">
         <v>147</v>
       </c>
-      <c r="J93" s="8" t="s">
+      <c r="J93" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3209,11 +3610,15 @@
       <c r="I94" t="s">
         <v>147</v>
       </c>
-      <c r="J94" s="8" t="s">
+      <c r="J94" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L94">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -3232,11 +3637,15 @@
       <c r="I95" t="s">
         <v>147</v>
       </c>
-      <c r="J95" s="8" t="s">
+      <c r="J95" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3255,11 +3664,15 @@
       <c r="I96" t="s">
         <v>147</v>
       </c>
-      <c r="J96" s="8" t="s">
+      <c r="J96" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -3278,11 +3691,15 @@
       <c r="I97" t="s">
         <v>147</v>
       </c>
-      <c r="J97" s="8" t="s">
+      <c r="J97" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L97">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -3301,11 +3718,15 @@
       <c r="I98" t="s">
         <v>147</v>
       </c>
-      <c r="J98" s="8" t="s">
+      <c r="J98" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -3324,11 +3745,15 @@
       <c r="I99" t="s">
         <v>147</v>
       </c>
-      <c r="J99" s="8" t="s">
+      <c r="J99" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L99">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -3347,11 +3772,15 @@
       <c r="I100" t="s">
         <v>147</v>
       </c>
-      <c r="J100" s="8" t="s">
+      <c r="J100" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L100">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -3370,11 +3799,15 @@
       <c r="I101" t="s">
         <v>147</v>
       </c>
-      <c r="J101" s="8" t="s">
+      <c r="J101" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L101">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -3393,11 +3826,15 @@
       <c r="I102" t="s">
         <v>147</v>
       </c>
-      <c r="J102" s="8" t="s">
+      <c r="J102" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L102">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -3416,11 +3853,15 @@
       <c r="I103" t="s">
         <v>147</v>
       </c>
-      <c r="J103" s="8" t="s">
+      <c r="J103" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L103">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>100</v>
       </c>
@@ -3439,11 +3880,15 @@
       <c r="I104" t="s">
         <v>147</v>
       </c>
-      <c r="J104" s="8" t="s">
+      <c r="J104" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L104">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>100</v>
       </c>
@@ -3462,11 +3907,15 @@
       <c r="I105" t="s">
         <v>147</v>
       </c>
-      <c r="J105" s="8" t="s">
+      <c r="J105" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L105">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>100</v>
       </c>
@@ -3485,11 +3934,15 @@
       <c r="I106" t="s">
         <v>147</v>
       </c>
-      <c r="J106" s="8" t="s">
+      <c r="J106" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>100</v>
       </c>
@@ -3508,11 +3961,15 @@
       <c r="I107" t="s">
         <v>147</v>
       </c>
-      <c r="J107" s="8" t="s">
+      <c r="J107" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L107">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>100</v>
       </c>
@@ -3531,11 +3988,15 @@
       <c r="I108" t="s">
         <v>147</v>
       </c>
-      <c r="J108" s="8" t="s">
+      <c r="J108" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L108">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -3554,11 +4015,15 @@
       <c r="I109" t="s">
         <v>147</v>
       </c>
-      <c r="J109" s="8" t="s">
+      <c r="J109" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L109">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -3577,11 +4042,15 @@
       <c r="I110" t="s">
         <v>147</v>
       </c>
-      <c r="J110" s="8" t="s">
+      <c r="J110" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L110">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>100</v>
       </c>
@@ -3600,11 +4069,15 @@
       <c r="I111" t="s">
         <v>147</v>
       </c>
-      <c r="J111" s="8" t="s">
+      <c r="J111" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L111">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>100</v>
       </c>
@@ -3623,11 +4096,15 @@
       <c r="I112" t="s">
         <v>147</v>
       </c>
-      <c r="J112" s="8" t="s">
+      <c r="J112" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L112">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>100</v>
       </c>
@@ -3646,11 +4123,15 @@
       <c r="I113" t="s">
         <v>147</v>
       </c>
-      <c r="J113" s="8" t="s">
+      <c r="J113" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L113">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>100</v>
       </c>
@@ -3669,11 +4150,15 @@
       <c r="I114" t="s">
         <v>147</v>
       </c>
-      <c r="J114" s="8" t="s">
+      <c r="J114" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L114">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>133</v>
       </c>
@@ -3692,8 +4177,12 @@
       <c r="I115" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L115">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>135</v>
       </c>
@@ -3712,8 +4201,12 @@
       <c r="I116" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L116">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>135</v>
       </c>
@@ -3732,8 +4225,12 @@
       <c r="I117" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L117">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -3752,8 +4249,12 @@
       <c r="I118" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L118">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>139</v>
       </c>
@@ -3772,8 +4273,12 @@
       <c r="I119" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L119">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>141</v>
       </c>
@@ -3792,13 +4297,17 @@
       <c r="I120" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L120">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F121" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F122" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
converted DSigDB, sparse parameter added
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A2A6CE-D6FD-45D6-AA18-26FEAF42527E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA73093-20AB-43C7-86AA-186BC9CEAE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="169">
   <si>
     <t>Resource</t>
   </si>
@@ -520,9 +520,6 @@
   </si>
   <si>
     <t>Attributes</t>
-  </si>
-  <si>
-    <t>Site no longer accessible</t>
   </si>
   <si>
     <t>How was input file generated?</t>
@@ -553,7 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,15 +600,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,12 +628,6 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -654,15 +638,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -671,11 +654,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
+  <cellStyles count="5">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1016,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1059,7 @@
       <c r="D2">
         <v>216</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>131173</v>
       </c>
       <c r="F2">
@@ -1187,7 +1168,7 @@
         <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
@@ -1227,7 +1208,7 @@
         <v>147</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
@@ -1252,7 +1233,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F7">
         <v>16827</v>
@@ -1837,7 +1818,7 @@
         <v>148</v>
       </c>
       <c r="J25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
@@ -2047,7 +2028,7 @@
         <v>149</v>
       </c>
       <c r="J31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
@@ -2339,7 +2320,7 @@
         <v>148</v>
       </c>
       <c r="J41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
@@ -2370,7 +2351,7 @@
         <v>148</v>
       </c>
       <c r="J42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
@@ -2401,7 +2382,7 @@
         <v>148</v>
       </c>
       <c r="J43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
@@ -2432,7 +2413,7 @@
         <v>148</v>
       </c>
       <c r="J44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
@@ -2447,8 +2428,17 @@
       <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="3" t="s">
         <v>55</v>
+      </c>
+      <c r="C45">
+        <v>17903</v>
+      </c>
+      <c r="D45">
+        <v>15826</v>
+      </c>
+      <c r="E45">
+        <v>292610</v>
       </c>
       <c r="F45">
         <v>18215</v>
@@ -2462,12 +2452,9 @@
       <c r="I45" t="s">
         <v>148</v>
       </c>
-      <c r="J45" t="s">
-        <v>161</v>
-      </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9979911254813284</v>
       </c>
       <c r="M45">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2478,8 +2465,17 @@
       <c r="A46" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="C46">
+        <v>1271</v>
+      </c>
+      <c r="D46">
+        <v>1205</v>
+      </c>
+      <c r="E46">
+        <v>12543</v>
       </c>
       <c r="F46">
         <v>1279</v>
@@ -2493,12 +2489,9 @@
       <c r="I46" t="s">
         <v>148</v>
       </c>
-      <c r="J46" t="s">
-        <v>161</v>
-      </c>
       <c r="L46">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.99777265134038662</v>
       </c>
       <c r="M46">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2509,8 +2502,17 @@
       <c r="A47" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="C47">
+        <v>398</v>
+      </c>
+      <c r="D47">
+        <v>1153</v>
+      </c>
+      <c r="E47">
+        <v>16215</v>
       </c>
       <c r="F47">
         <v>404</v>
@@ -2524,12 +2526,9 @@
       <c r="I47" t="s">
         <v>148</v>
       </c>
-      <c r="J47" t="s">
-        <v>161</v>
-      </c>
       <c r="L47">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.99846059113300489</v>
       </c>
       <c r="M47">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2540,8 +2539,17 @@
       <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="3" t="s">
         <v>58</v>
+      </c>
+      <c r="C48">
+        <v>10792</v>
+      </c>
+      <c r="D48">
+        <v>1163</v>
+      </c>
+      <c r="E48">
+        <v>159229</v>
       </c>
       <c r="F48">
         <v>10933</v>
@@ -2555,12 +2563,9 @@
       <c r="I48" t="s">
         <v>148</v>
       </c>
-      <c r="J48" t="s">
-        <v>161</v>
-      </c>
       <c r="L48">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0023227999496411</v>
       </c>
       <c r="M48">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2587,7 +2592,7 @@
         <v>148</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
@@ -2618,7 +2623,7 @@
         <v>148</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
@@ -2835,7 +2840,7 @@
         <v>148</v>
       </c>
       <c r="J57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L57">
         <f t="shared" si="0"/>
@@ -2866,7 +2871,7 @@
         <v>148</v>
       </c>
       <c r="J58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L58">
         <f t="shared" si="0"/>
@@ -2897,7 +2902,7 @@
         <v>148</v>
       </c>
       <c r="J59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L59">
         <f t="shared" si="0"/>
@@ -3114,7 +3119,7 @@
         <v>148</v>
       </c>
       <c r="J66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L66">
         <f t="shared" si="0"/>
@@ -3145,7 +3150,7 @@
         <v>148</v>
       </c>
       <c r="J67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L67">
         <f t="shared" ref="L67:L120" si="1">IF(COUNTA(E67),E67/H67,1)</f>
@@ -3623,7 +3628,7 @@
         <v>147</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L83">
         <f t="shared" si="1"/>
@@ -3654,7 +3659,7 @@
         <v>147</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L84">
         <f t="shared" si="1"/>
@@ -3685,7 +3690,7 @@
         <v>147</v>
       </c>
       <c r="J85" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L85">
         <f t="shared" si="1"/>
@@ -3716,7 +3721,7 @@
         <v>147</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L86">
         <f t="shared" si="1"/>
@@ -3747,7 +3752,7 @@
         <v>147</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L87">
         <f t="shared" si="1"/>
@@ -3778,7 +3783,7 @@
         <v>147</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L88">
         <f t="shared" si="1"/>
@@ -3809,7 +3814,7 @@
         <v>147</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L89">
         <f t="shared" si="1"/>
@@ -3840,7 +3845,7 @@
         <v>147</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L90">
         <f t="shared" si="1"/>
@@ -3871,7 +3876,7 @@
         <v>147</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L91">
         <f t="shared" si="1"/>
@@ -3902,7 +3907,7 @@
         <v>147</v>
       </c>
       <c r="J92" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L92">
         <f t="shared" si="1"/>
@@ -3933,7 +3938,7 @@
         <v>147</v>
       </c>
       <c r="J93" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L93">
         <f t="shared" si="1"/>
@@ -3964,7 +3969,7 @@
         <v>147</v>
       </c>
       <c r="J94" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L94">
         <f t="shared" si="1"/>
@@ -3995,7 +4000,7 @@
         <v>147</v>
       </c>
       <c r="J95" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L95">
         <f t="shared" si="1"/>
@@ -4026,7 +4031,7 @@
         <v>147</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L96">
         <f t="shared" si="1"/>
@@ -4057,7 +4062,7 @@
         <v>147</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L97">
         <f t="shared" si="1"/>
@@ -4088,7 +4093,7 @@
         <v>147</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L98">
         <f t="shared" si="1"/>
@@ -4119,7 +4124,7 @@
         <v>147</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L99">
         <f t="shared" si="1"/>
@@ -4150,7 +4155,7 @@
         <v>147</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L100">
         <f t="shared" si="1"/>
@@ -4181,7 +4186,7 @@
         <v>147</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L101">
         <f t="shared" si="1"/>
@@ -4212,7 +4217,7 @@
         <v>147</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L102">
         <f t="shared" si="1"/>
@@ -4243,7 +4248,7 @@
         <v>147</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L103">
         <f t="shared" si="1"/>
@@ -4274,7 +4279,7 @@
         <v>147</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L104">
         <f t="shared" si="1"/>
@@ -4305,7 +4310,7 @@
         <v>147</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L105">
         <f t="shared" si="1"/>
@@ -4336,7 +4341,7 @@
         <v>147</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L106">
         <f t="shared" si="1"/>
@@ -4367,7 +4372,7 @@
         <v>147</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L107">
         <f t="shared" si="1"/>
@@ -4398,7 +4403,7 @@
         <v>147</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L108">
         <f t="shared" si="1"/>
@@ -4429,7 +4434,7 @@
         <v>147</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L109">
         <f t="shared" si="1"/>
@@ -4460,7 +4465,7 @@
         <v>147</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L110">
         <f t="shared" si="1"/>
@@ -4491,7 +4496,7 @@
         <v>147</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L111">
         <f t="shared" si="1"/>
@@ -4522,7 +4527,7 @@
         <v>147</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L112">
         <f t="shared" si="1"/>
@@ -4553,7 +4558,7 @@
         <v>147</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L113">
         <f t="shared" si="1"/>
@@ -4584,7 +4589,7 @@
         <v>147</v>
       </c>
       <c r="J114" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L114">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
fixed THPA RNA-seq, converted HMDB
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2E4E6-C675-4FC0-8BD4-F8B2562CBF36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5122964-4A3B-4F40-94E9-E79AB7A7229A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="169">
   <si>
     <t>Resource</t>
   </si>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,6 +1074,10 @@
       <c r="I2" t="s">
         <v>147</v>
       </c>
+      <c r="K2">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.0493257454677594E-2</v>
+      </c>
       <c r="L2">
         <f>IF(COUNTA(E2),E2/H2,1)</f>
         <v>4.9456992214952963E-2</v>
@@ -1102,6 +1106,10 @@
       <c r="I3" t="s">
         <v>147</v>
       </c>
+      <c r="K3" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L3">
         <f t="shared" ref="L3:L66" si="0">IF(COUNTA(E3),E3/H3,1)</f>
         <v>1</v>
@@ -1130,6 +1138,10 @@
       <c r="I4" t="s">
         <v>147</v>
       </c>
+      <c r="K4" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L4">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1170,6 +1182,10 @@
       <c r="J5" t="s">
         <v>167</v>
       </c>
+      <c r="K5">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.6242270069709915E-2</v>
+      </c>
       <c r="L5">
         <f t="shared" si="0"/>
         <v>1.1491851532773349</v>
@@ -1210,6 +1226,10 @@
       <c r="J6" t="s">
         <v>167</v>
       </c>
+      <c r="K6">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9951478158139009E-2</v>
+      </c>
       <c r="L6">
         <f t="shared" si="0"/>
         <v>1.2597183797971199</v>
@@ -1247,6 +1267,10 @@
       <c r="I7" t="s">
         <v>147</v>
       </c>
+      <c r="K7" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="L7" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -1284,6 +1308,10 @@
       <c r="I8" t="s">
         <v>147</v>
       </c>
+      <c r="K8">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9994598521021283E-2</v>
+      </c>
       <c r="L8">
         <f t="shared" si="0"/>
         <v>0.98823356056177436</v>
@@ -1312,6 +1340,10 @@
       <c r="I9" t="s">
         <v>147</v>
       </c>
+      <c r="K9" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L9">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1340,6 +1372,10 @@
       <c r="I10" t="s">
         <v>147</v>
       </c>
+      <c r="K10" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L10">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1368,6 +1404,10 @@
       <c r="I11" t="s">
         <v>147</v>
       </c>
+      <c r="K11" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L11">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1396,6 +1436,10 @@
       <c r="I12" t="s">
         <v>147</v>
       </c>
+      <c r="K12" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L12">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1427,6 +1471,10 @@
       <c r="J13" t="s">
         <v>158</v>
       </c>
+      <c r="K13" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L13">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1455,6 +1503,10 @@
       <c r="I14" t="s">
         <v>147</v>
       </c>
+      <c r="K14" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L14">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1483,6 +1535,10 @@
       <c r="I15" t="s">
         <v>147</v>
       </c>
+      <c r="K15" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L15">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1511,6 +1567,10 @@
       <c r="I16" t="s">
         <v>148</v>
       </c>
+      <c r="K16" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L16">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1539,6 +1599,10 @@
       <c r="I17" t="s">
         <v>147</v>
       </c>
+      <c r="K17" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1567,6 +1631,10 @@
       <c r="I18" t="s">
         <v>148</v>
       </c>
+      <c r="K18" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L18">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1595,6 +1663,10 @@
       <c r="I19" t="s">
         <v>148</v>
       </c>
+      <c r="K19" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L19">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1632,6 +1704,10 @@
       <c r="I20" t="s">
         <v>148</v>
       </c>
+      <c r="K20">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.43546672118486213</v>
+      </c>
       <c r="L20">
         <f t="shared" si="0"/>
         <v>1.1124590011722242</v>
@@ -1669,6 +1745,10 @@
       <c r="I21" t="s">
         <v>148</v>
       </c>
+      <c r="K21">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.58290645586297751</v>
+      </c>
       <c r="L21">
         <f t="shared" si="0"/>
         <v>1.0990330203911971</v>
@@ -1706,6 +1786,10 @@
       <c r="I22" t="s">
         <v>148</v>
       </c>
+      <c r="K22">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.42285199670906903</v>
+      </c>
       <c r="L22">
         <f t="shared" si="0"/>
         <v>1.114833657720123</v>
@@ -1743,6 +1827,10 @@
       <c r="I23" t="s">
         <v>148</v>
       </c>
+      <c r="K23">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>3.6521474902039934E-2</v>
+      </c>
       <c r="L23">
         <f t="shared" si="0"/>
         <v>1.3284207830720616</v>
@@ -1780,6 +1868,10 @@
       <c r="I24" t="s">
         <v>148</v>
       </c>
+      <c r="K24">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.48264840963548644</v>
+      </c>
       <c r="L24">
         <f t="shared" si="0"/>
         <v>1.5375814570097672</v>
@@ -1820,6 +1912,10 @@
       <c r="J25" t="s">
         <v>166</v>
       </c>
+      <c r="K25">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>2.8271890418803871E-2</v>
+      </c>
       <c r="L25">
         <f t="shared" si="0"/>
         <v>1.2280596203815786</v>
@@ -1857,6 +1953,10 @@
       <c r="I26" t="s">
         <v>148</v>
       </c>
+      <c r="K26">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.81467595441229146</v>
+      </c>
       <c r="L26">
         <f t="shared" si="0"/>
         <v>2.6712613392554672</v>
@@ -1894,6 +1994,10 @@
       <c r="I27" t="s">
         <v>148</v>
       </c>
+      <c r="K27">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.74925497525002527</v>
+      </c>
       <c r="L27">
         <f t="shared" si="0"/>
         <v>2.6848416289592758</v>
@@ -1931,6 +2035,10 @@
       <c r="I28" t="s">
         <v>148</v>
       </c>
+      <c r="K28">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.79661619392905381</v>
+      </c>
       <c r="L28">
         <f t="shared" si="0"/>
         <v>3.060516329346826</v>
@@ -1968,6 +2076,10 @@
       <c r="I29" t="s">
         <v>147</v>
       </c>
+      <c r="K29">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.0342960932276408E-2</v>
+      </c>
       <c r="L29">
         <f t="shared" si="0"/>
         <v>0.25318885638449057</v>
@@ -2005,6 +2117,10 @@
       <c r="I30" t="s">
         <v>147</v>
       </c>
+      <c r="K30">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.0474188219801548E-2</v>
+      </c>
       <c r="L30">
         <f t="shared" si="0"/>
         <v>0.19129584566160401</v>
@@ -2030,6 +2146,10 @@
       <c r="J31" t="s">
         <v>162</v>
       </c>
+      <c r="K31" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L31">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2067,6 +2187,10 @@
       <c r="I32" t="s">
         <v>148</v>
       </c>
+      <c r="K32">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.300654311996976E-3</v>
+      </c>
       <c r="L32">
         <f t="shared" si="0"/>
         <v>1.0505577739180261</v>
@@ -2095,6 +2219,10 @@
       <c r="I33" t="s">
         <v>147</v>
       </c>
+      <c r="K33" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L33">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2123,6 +2251,10 @@
       <c r="I34" t="s">
         <v>148</v>
       </c>
+      <c r="K34" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L34">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2151,6 +2283,10 @@
       <c r="I35" t="s">
         <v>148</v>
       </c>
+      <c r="K35" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L35">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2179,6 +2315,10 @@
       <c r="I36" t="s">
         <v>147</v>
       </c>
+      <c r="K36" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L36">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2207,6 +2347,10 @@
       <c r="I37" t="s">
         <v>148</v>
       </c>
+      <c r="K37" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L37">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2235,6 +2379,10 @@
       <c r="I38" t="s">
         <v>148</v>
       </c>
+      <c r="K38" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L38">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2263,6 +2411,10 @@
       <c r="I39" t="s">
         <v>147</v>
       </c>
+      <c r="K39" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L39">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2291,6 +2443,10 @@
       <c r="I40" t="s">
         <v>148</v>
       </c>
+      <c r="K40" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L40">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2322,6 +2478,10 @@
       <c r="J41" t="s">
         <v>164</v>
       </c>
+      <c r="K41" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L41">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2353,6 +2513,10 @@
       <c r="J42" t="s">
         <v>164</v>
       </c>
+      <c r="K42" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L42">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2384,6 +2548,10 @@
       <c r="J43" t="s">
         <v>164</v>
       </c>
+      <c r="K43" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L43">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2415,6 +2583,10 @@
       <c r="J44" t="s">
         <v>164</v>
       </c>
+      <c r="K44" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L44">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2452,6 +2624,10 @@
       <c r="I45" t="s">
         <v>148</v>
       </c>
+      <c r="K45">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.0327428361490754E-3</v>
+      </c>
       <c r="L45">
         <f t="shared" si="0"/>
         <v>0.9979911254813284</v>
@@ -2489,6 +2665,10 @@
       <c r="I46" t="s">
         <v>148</v>
       </c>
+      <c r="K46">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>8.1897156811214754E-3</v>
+      </c>
       <c r="L46">
         <f t="shared" si="0"/>
         <v>0.99777265134038662</v>
@@ -2526,6 +2706,10 @@
       <c r="I47" t="s">
         <v>148</v>
       </c>
+      <c r="K47">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>3.5334957528318091E-2</v>
+      </c>
       <c r="L47">
         <f t="shared" si="0"/>
         <v>0.99846059113300489</v>
@@ -2563,6 +2747,10 @@
       <c r="I48" t="s">
         <v>148</v>
       </c>
+      <c r="K48">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.2686461803813788E-2</v>
+      </c>
       <c r="L48">
         <f t="shared" si="0"/>
         <v>1.0023227999496411</v>
@@ -2594,6 +2782,10 @@
       <c r="J49" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K49" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L49">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2625,6 +2817,10 @@
       <c r="J50" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K50" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L50">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2653,6 +2849,10 @@
       <c r="I51" t="s">
         <v>148</v>
       </c>
+      <c r="K51" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L51">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2690,6 +2890,10 @@
       <c r="I52" t="s">
         <v>148</v>
       </c>
+      <c r="K52">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.0091512505704263E-4</v>
+      </c>
       <c r="L52">
         <f t="shared" si="0"/>
         <v>1.0052430405969</v>
@@ -2727,6 +2931,10 @@
       <c r="I53" t="s">
         <v>148</v>
       </c>
+      <c r="K53">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.16013334479420877</v>
+      </c>
       <c r="L53">
         <f t="shared" si="0"/>
         <v>1.0036775901243822</v>
@@ -2755,6 +2963,10 @@
       <c r="I54" t="s">
         <v>147</v>
       </c>
+      <c r="K54" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L54">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2783,6 +2995,10 @@
       <c r="I55" t="s">
         <v>148</v>
       </c>
+      <c r="K55" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L55">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2811,6 +3027,10 @@
       <c r="I56" t="s">
         <v>148</v>
       </c>
+      <c r="K56" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L56">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2842,6 +3062,10 @@
       <c r="J57" t="s">
         <v>163</v>
       </c>
+      <c r="K57" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L57">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2873,6 +3097,10 @@
       <c r="J58" t="s">
         <v>163</v>
       </c>
+      <c r="K58" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2904,6 +3132,10 @@
       <c r="J59" t="s">
         <v>163</v>
       </c>
+      <c r="K59" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L59">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2923,6 +3155,10 @@
       <c r="I60" t="s">
         <v>147</v>
       </c>
+      <c r="K60" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L60">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2951,6 +3187,10 @@
       <c r="I61" t="s">
         <v>147</v>
       </c>
+      <c r="K61" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L61">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2979,6 +3219,10 @@
       <c r="I62" t="s">
         <v>147</v>
       </c>
+      <c r="K62" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L62">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3016,6 +3260,10 @@
       <c r="I63" t="s">
         <v>148</v>
       </c>
+      <c r="K63">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.0086581624526999E-3</v>
+      </c>
       <c r="L63">
         <f t="shared" si="0"/>
         <v>1.2855585434988008</v>
@@ -3053,6 +3301,10 @@
       <c r="I64" t="s">
         <v>148</v>
       </c>
+      <c r="K64">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>7.7219382244942038E-3</v>
+      </c>
       <c r="L64">
         <f t="shared" si="0"/>
         <v>2.0093676814988291</v>
@@ -3090,6 +3342,10 @@
       <c r="I65" t="s">
         <v>148</v>
       </c>
+      <c r="K65">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.4553570577299918E-3</v>
+      </c>
       <c r="L65">
         <f t="shared" si="0"/>
         <v>5.7080381398817455</v>
@@ -3121,6 +3377,10 @@
       <c r="J66" t="s">
         <v>165</v>
       </c>
+      <c r="K66" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L66">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3152,6 +3412,10 @@
       <c r="J67" t="s">
         <v>165</v>
       </c>
+      <c r="K67" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L67">
         <f t="shared" ref="L67:L120" si="1">IF(COUNTA(E67),E67/H67,1)</f>
         <v>1</v>
@@ -3189,6 +3453,10 @@
       <c r="I68" t="s">
         <v>148</v>
       </c>
+      <c r="K68">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.4986207799680335E-2</v>
+      </c>
       <c r="L68">
         <f t="shared" si="1"/>
         <v>1.3892684335957246</v>
@@ -3217,6 +3485,10 @@
       <c r="I69" t="s">
         <v>148</v>
       </c>
+      <c r="K69" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L69">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3254,6 +3526,10 @@
       <c r="I70" t="s">
         <v>148</v>
       </c>
+      <c r="K70">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>6.3270385115103078E-2</v>
+      </c>
       <c r="L70">
         <f t="shared" si="1"/>
         <v>5.1171843079307644</v>
@@ -3291,6 +3567,10 @@
       <c r="I71" t="s">
         <v>148</v>
       </c>
+      <c r="K71">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>2.0450501673110744E-3</v>
+      </c>
       <c r="L71">
         <f t="shared" si="1"/>
         <v>3.5024098004954012</v>
@@ -3328,6 +3608,10 @@
       <c r="I72" t="s">
         <v>148</v>
       </c>
+      <c r="K72">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.7222059355583242E-2</v>
+      </c>
       <c r="L72">
         <f t="shared" si="1"/>
         <v>18.120848884785328</v>
@@ -3365,6 +3649,10 @@
       <c r="I73" t="s">
         <v>148</v>
       </c>
+      <c r="K73">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.7047801145843595E-3</v>
+      </c>
       <c r="L73">
         <f t="shared" si="1"/>
         <v>1.1916106184155706</v>
@@ -3393,6 +3681,10 @@
       <c r="I74" t="s">
         <v>148</v>
       </c>
+      <c r="K74" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L74">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3418,6 +3710,10 @@
       <c r="E75" s="5">
         <v>7641</v>
       </c>
+      <c r="K75">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9144138839492127E-4</v>
+      </c>
       <c r="L75" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3455,6 +3751,10 @@
       <c r="I76" t="s">
         <v>148</v>
       </c>
+      <c r="K76">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.6376285458378361E-4</v>
+      </c>
       <c r="L76" s="1">
         <f t="shared" si="1"/>
         <v>0.11656194452482328</v>
@@ -3492,6 +3792,10 @@
       <c r="I77" t="s">
         <v>148</v>
       </c>
+      <c r="K77">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>3.6669036505992633E-3</v>
+      </c>
       <c r="L77">
         <f t="shared" si="1"/>
         <v>0.97154417346196853</v>
@@ -3514,6 +3818,10 @@
       <c r="I78" t="s">
         <v>149</v>
       </c>
+      <c r="K78" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L78">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3533,6 +3841,10 @@
       <c r="I79" t="s">
         <v>148</v>
       </c>
+      <c r="K79" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L79">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3570,6 +3882,10 @@
       <c r="I80" t="s">
         <v>148</v>
       </c>
+      <c r="K80">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.6007758408868329E-3</v>
+      </c>
       <c r="L80">
         <f t="shared" si="1"/>
         <v>1.0779775664102467</v>
@@ -3598,6 +3914,10 @@
       <c r="I81" t="s">
         <v>147</v>
       </c>
+      <c r="K81" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L81">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3626,6 +3946,10 @@
       <c r="I82" t="s">
         <v>148</v>
       </c>
+      <c r="K82" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L82">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3657,6 +3981,10 @@
       <c r="J83" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K83" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L83">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3688,6 +4016,10 @@
       <c r="J84" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K84" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L84">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3719,6 +4051,10 @@
       <c r="J85" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K85" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L85">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3750,6 +4086,10 @@
       <c r="J86" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K86" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L86">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3781,6 +4121,10 @@
       <c r="J87" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K87" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L87">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3812,6 +4156,10 @@
       <c r="J88" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K88" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L88">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3843,6 +4191,10 @@
       <c r="J89" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K89" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L89">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3874,6 +4226,10 @@
       <c r="J90" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K90" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L90">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3905,6 +4261,10 @@
       <c r="J91" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K91" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L91">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3936,6 +4296,10 @@
       <c r="J92" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K92" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L92">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3967,6 +4331,10 @@
       <c r="J93" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K93" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L93">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3998,6 +4366,10 @@
       <c r="J94" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K94" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L94">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4029,6 +4401,10 @@
       <c r="J95" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K95" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L95">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4060,6 +4436,10 @@
       <c r="J96" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K96" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L96">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4091,6 +4471,10 @@
       <c r="J97" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K97" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L97">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4122,6 +4506,10 @@
       <c r="J98" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K98" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L98">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4153,6 +4541,10 @@
       <c r="J99" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K99" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L99">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4184,6 +4576,10 @@
       <c r="J100" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K100" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L100">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4215,6 +4611,10 @@
       <c r="J101" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K101" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L101">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4246,6 +4646,10 @@
       <c r="J102" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K102" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L102">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4277,6 +4681,10 @@
       <c r="J103" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K103" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L103">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4308,6 +4716,10 @@
       <c r="J104" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K104" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L104">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4339,6 +4751,10 @@
       <c r="J105" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K105" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L105">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4370,6 +4786,10 @@
       <c r="J106" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K106" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L106">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4401,6 +4821,10 @@
       <c r="J107" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K107" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L107">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4432,6 +4856,10 @@
       <c r="J108" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K108" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L108">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4463,6 +4891,10 @@
       <c r="J109" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K109" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L109">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4494,6 +4926,10 @@
       <c r="J110" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K110" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L110">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4525,6 +4961,10 @@
       <c r="J111" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K111" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L111">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4556,6 +4996,10 @@
       <c r="J112" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K112" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L112">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4587,6 +5031,10 @@
       <c r="J113" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K113" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L113">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4618,6 +5066,10 @@
       <c r="J114" s="7" t="s">
         <v>161</v>
       </c>
+      <c r="K114" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L114">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4631,7 +5083,7 @@
       <c r="A115" t="s">
         <v>133</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F115">
@@ -4645,6 +5097,10 @@
       </c>
       <c r="I115" t="s">
         <v>148</v>
+      </c>
+      <c r="K115" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L115">
         <f t="shared" si="1"/>
@@ -4659,8 +5115,17 @@
       <c r="A116" t="s">
         <v>135</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="3" t="s">
         <v>136</v>
+      </c>
+      <c r="C116">
+        <v>18025</v>
+      </c>
+      <c r="D116">
+        <v>64</v>
+      </c>
+      <c r="E116">
+        <v>58693</v>
       </c>
       <c r="F116">
         <v>17661</v>
@@ -4674,9 +5139,13 @@
       <c r="I116" t="s">
         <v>147</v>
       </c>
+      <c r="K116">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.0878120665742023E-2</v>
+      </c>
       <c r="L116">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.29665702963891472</v>
       </c>
       <c r="M116">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -4711,6 +5180,10 @@
       <c r="I117" t="s">
         <v>148</v>
       </c>
+      <c r="K117">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>8.9651769798828621E-2</v>
+      </c>
       <c r="L117">
         <f t="shared" si="1"/>
         <v>1.0049699255785502</v>
@@ -4724,8 +5197,17 @@
       <c r="A118" t="s">
         <v>135</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="3" t="s">
         <v>138</v>
+      </c>
+      <c r="C118">
+        <v>18362</v>
+      </c>
+      <c r="D118">
+        <v>62</v>
+      </c>
+      <c r="E118">
+        <v>56832</v>
       </c>
       <c r="F118">
         <v>18200</v>
@@ -4739,9 +5221,13 @@
       <c r="I118" t="s">
         <v>147</v>
       </c>
+      <c r="K118">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9920769049685364E-2</v>
+      </c>
       <c r="L118">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.42186212578961824</v>
       </c>
       <c r="M118">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -4752,7 +5238,7 @@
       <c r="A119" t="s">
         <v>139</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>140</v>
       </c>
       <c r="F119">
@@ -4766,6 +5252,13 @@
       </c>
       <c r="I119" t="s">
         <v>153</v>
+      </c>
+      <c r="J119" t="s">
+        <v>162</v>
+      </c>
+      <c r="K119" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L119">
         <f t="shared" si="1"/>
@@ -4794,6 +5287,10 @@
       </c>
       <c r="I120" t="s">
         <v>148</v>
+      </c>
+      <c r="K120" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L120">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
converted huMAP, updated requirements)
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC68034-CD75-49C8-BB32-3D09B5DC4FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD1BDC9-D9A3-4721-81E8-139F02087FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="170">
   <si>
     <t>Resource</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Original does not take probability into account</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,6 +1016,7 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3471,8 +3475,17 @@
       <c r="A69" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>83</v>
+      </c>
+      <c r="C69">
+        <v>1991</v>
+      </c>
+      <c r="D69">
+        <v>1991</v>
+      </c>
+      <c r="E69">
+        <v>9764</v>
       </c>
       <c r="F69">
         <v>7669</v>
@@ -3486,13 +3499,16 @@
       <c r="I69" t="s">
         <v>148</v>
       </c>
-      <c r="K69" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L69">
+      <c r="J69" t="s">
+        <v>169</v>
+      </c>
+      <c r="K69">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>2.4631181855264811E-3</v>
+      </c>
+      <c r="L69" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7.7383971595232054E-2</v>
       </c>
       <c r="M69">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>

</xml_diff>

<commit_message>
converted cle, clinvar, generif, go, gtex. Fixed utility_functions imputeandremove function
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD1BDC9-D9A3-4721-81E8-139F02087FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CEBC34-8E99-4815-BA67-89BA68CCDF11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="170">
   <si>
     <t>Resource</t>
   </si>
@@ -522,15 +522,9 @@
     <t>Attributes</t>
   </si>
   <si>
-    <t>How was input file generated?</t>
-  </si>
-  <si>
     <t>No analysis in original document</t>
   </si>
   <si>
-    <t>Need to read Owl file</t>
-  </si>
-  <si>
     <t>Need access to site</t>
   </si>
   <si>
@@ -547,6 +541,12 @@
   </si>
   <si>
     <t>Original does not take probability into account</t>
+  </si>
+  <si>
+    <t>Website no longer live</t>
+  </si>
+  <si>
+    <t>Original Input File?</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -658,6 +658,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
@@ -1000,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1186,7 @@
         <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K5">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1229,7 +1230,7 @@
         <v>147</v>
       </c>
       <c r="J6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K6">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1258,7 +1259,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F7">
         <v>16827</v>
@@ -1915,7 +1916,7 @@
         <v>148</v>
       </c>
       <c r="J25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K25">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2149,7 +2150,7 @@
         <v>149</v>
       </c>
       <c r="J31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K31" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2209,7 +2210,7 @@
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F33">
@@ -2273,7 +2274,7 @@
       <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>42</v>
       </c>
       <c r="F35">
@@ -2465,8 +2466,17 @@
       <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="C41">
+        <v>86</v>
+      </c>
+      <c r="D41">
+        <v>550</v>
+      </c>
+      <c r="E41">
+        <v>833</v>
       </c>
       <c r="F41">
         <v>61</v>
@@ -2481,15 +2491,15 @@
         <v>148</v>
       </c>
       <c r="J41" t="s">
-        <v>164</v>
-      </c>
-      <c r="K41" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>162</v>
+      </c>
+      <c r="K41">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.7610993657505285E-2</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.3664772727272729</v>
       </c>
       <c r="M41">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2500,8 +2510,17 @@
       <c r="A42" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>51</v>
+      </c>
+      <c r="C42">
+        <v>384</v>
+      </c>
+      <c r="D42">
+        <v>1677</v>
+      </c>
+      <c r="E42">
+        <v>5170</v>
       </c>
       <c r="F42">
         <v>261</v>
@@ -2516,15 +2535,15 @@
         <v>148</v>
       </c>
       <c r="J42" t="s">
-        <v>164</v>
-      </c>
-      <c r="K42" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>162</v>
+      </c>
+      <c r="K42">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>8.0283492347445837E-3</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.1284479209551255</v>
       </c>
       <c r="M42">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2535,8 +2554,17 @@
       <c r="A43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="C43">
+        <v>2774</v>
+      </c>
+      <c r="D43">
+        <v>5660</v>
+      </c>
+      <c r="E43">
+        <v>16123</v>
       </c>
       <c r="F43">
         <v>2532</v>
@@ -2551,15 +2579,15 @@
         <v>148</v>
       </c>
       <c r="J43" t="s">
-        <v>164</v>
-      </c>
-      <c r="K43" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>162</v>
+      </c>
+      <c r="K43">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.026887733395156E-3</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.2072631973043804</v>
       </c>
       <c r="M43">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2570,8 +2598,17 @@
       <c r="A44" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="C44">
+        <v>261</v>
+      </c>
+      <c r="D44">
+        <v>972</v>
+      </c>
+      <c r="E44">
+        <v>3003</v>
       </c>
       <c r="F44">
         <v>154</v>
@@ -2586,15 +2623,15 @@
         <v>148</v>
       </c>
       <c r="J44" t="s">
-        <v>164</v>
-      </c>
-      <c r="K44" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>162</v>
+      </c>
+      <c r="K44">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.1837188401683933E-2</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.6832959641255605</v>
       </c>
       <c r="M44">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2784,9 +2821,7 @@
       <c r="I49" t="s">
         <v>148</v>
       </c>
-      <c r="J49" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J49" s="7"/>
       <c r="K49" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -2819,9 +2854,7 @@
       <c r="I50" t="s">
         <v>148</v>
       </c>
-      <c r="J50" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J50" s="7"/>
       <c r="K50" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -2968,6 +3001,9 @@
       <c r="I54" t="s">
         <v>147</v>
       </c>
+      <c r="J54" s="7" t="s">
+        <v>169</v>
+      </c>
       <c r="K54" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -2985,8 +3021,17 @@
       <c r="A55" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>68</v>
+      </c>
+      <c r="C55" s="9">
+        <v>4457</v>
+      </c>
+      <c r="D55">
+        <v>661</v>
+      </c>
+      <c r="E55">
+        <v>13374</v>
       </c>
       <c r="F55">
         <v>4368</v>
@@ -3000,13 +3045,13 @@
       <c r="I55" t="s">
         <v>148</v>
       </c>
-      <c r="K55" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K55">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.5395962155775288E-3</v>
       </c>
       <c r="L55">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.4149386373254338</v>
       </c>
       <c r="M55">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -3017,7 +3062,7 @@
       <c r="A56" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>69</v>
       </c>
       <c r="F56">
@@ -3031,6 +3076,9 @@
       </c>
       <c r="I56" t="s">
         <v>148</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="K56" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3049,8 +3097,17 @@
       <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="3" t="s">
         <v>71</v>
+      </c>
+      <c r="C57">
+        <v>3082</v>
+      </c>
+      <c r="D57">
+        <v>3152</v>
+      </c>
+      <c r="E57">
+        <v>25272</v>
       </c>
       <c r="F57">
         <v>14481</v>
@@ -3064,16 +3121,13 @@
       <c r="I57" t="s">
         <v>148</v>
       </c>
-      <c r="J57" t="s">
-        <v>163</v>
-      </c>
-      <c r="K57" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K57">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>2.6014816669247013E-3</v>
       </c>
       <c r="L57">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.12925994690890119</v>
       </c>
       <c r="M57">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -3084,8 +3138,17 @@
       <c r="A58" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="C58">
+        <v>3789</v>
+      </c>
+      <c r="D58">
+        <v>1249</v>
+      </c>
+      <c r="E58">
+        <v>20753</v>
       </c>
       <c r="F58">
         <v>12400</v>
@@ -3099,16 +3162,13 @@
       <c r="I58" t="s">
         <v>148</v>
       </c>
-      <c r="J58" t="s">
-        <v>163</v>
-      </c>
-      <c r="K58" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K58">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.3852448018060798E-3</v>
       </c>
       <c r="L58">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.47754153435500946</v>
       </c>
       <c r="M58">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -3119,8 +3179,17 @@
       <c r="A59" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="3" t="s">
         <v>73</v>
+      </c>
+      <c r="C59">
+        <v>3794</v>
+      </c>
+      <c r="D59">
+        <v>2552</v>
+      </c>
+      <c r="E59">
+        <v>16903</v>
       </c>
       <c r="F59">
         <v>11739</v>
@@ -3134,16 +3203,13 @@
       <c r="I59" t="s">
         <v>148</v>
       </c>
-      <c r="J59" t="s">
-        <v>163</v>
-      </c>
-      <c r="K59" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K59">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.7457650505748228E-3</v>
       </c>
       <c r="L59">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.34992961245445514</v>
       </c>
       <c r="M59">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -3154,7 +3220,7 @@
       <c r="A60" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>150</v>
       </c>
       <c r="I60" t="s">
@@ -3177,7 +3243,7 @@
       <c r="A61" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F61">
@@ -3209,7 +3275,7 @@
       <c r="A62" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F62">
@@ -3380,7 +3446,7 @@
         <v>148</v>
       </c>
       <c r="J66" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K66" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3415,7 +3481,7 @@
         <v>148</v>
       </c>
       <c r="J67" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K67" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3500,7 +3566,7 @@
         <v>148</v>
       </c>
       <c r="J69" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K69">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3845,7 +3911,7 @@
         <v>149</v>
       </c>
       <c r="J78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K78" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3940,9 +4006,6 @@
       <c r="B81" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D81">
-        <v>4543</v>
-      </c>
       <c r="F81">
         <v>18375</v>
       </c>
@@ -4028,9 +4091,7 @@
       <c r="I83" t="s">
         <v>147</v>
       </c>
-      <c r="J83" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J83" s="7"/>
       <c r="K83" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4063,9 +4124,7 @@
       <c r="I84" t="s">
         <v>147</v>
       </c>
-      <c r="J84" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J84" s="7"/>
       <c r="K84" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4098,9 +4157,7 @@
       <c r="I85" t="s">
         <v>147</v>
       </c>
-      <c r="J85" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J85" s="7"/>
       <c r="K85" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4133,9 +4190,7 @@
       <c r="I86" t="s">
         <v>147</v>
       </c>
-      <c r="J86" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J86" s="7"/>
       <c r="K86" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4168,9 +4223,7 @@
       <c r="I87" t="s">
         <v>147</v>
       </c>
-      <c r="J87" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J87" s="7"/>
       <c r="K87" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4203,9 +4256,7 @@
       <c r="I88" t="s">
         <v>147</v>
       </c>
-      <c r="J88" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J88" s="7"/>
       <c r="K88" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4238,9 +4289,7 @@
       <c r="I89" t="s">
         <v>147</v>
       </c>
-      <c r="J89" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J89" s="7"/>
       <c r="K89" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4273,9 +4322,7 @@
       <c r="I90" t="s">
         <v>147</v>
       </c>
-      <c r="J90" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J90" s="7"/>
       <c r="K90" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4308,9 +4355,7 @@
       <c r="I91" t="s">
         <v>147</v>
       </c>
-      <c r="J91" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J91" s="7"/>
       <c r="K91" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4343,9 +4388,7 @@
       <c r="I92" t="s">
         <v>147</v>
       </c>
-      <c r="J92" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J92" s="7"/>
       <c r="K92" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4378,9 +4421,7 @@
       <c r="I93" t="s">
         <v>147</v>
       </c>
-      <c r="J93" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J93" s="7"/>
       <c r="K93" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4413,9 +4454,7 @@
       <c r="I94" t="s">
         <v>147</v>
       </c>
-      <c r="J94" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J94" s="7"/>
       <c r="K94" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4448,9 +4487,7 @@
       <c r="I95" t="s">
         <v>147</v>
       </c>
-      <c r="J95" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J95" s="7"/>
       <c r="K95" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4483,9 +4520,7 @@
       <c r="I96" t="s">
         <v>147</v>
       </c>
-      <c r="J96" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J96" s="7"/>
       <c r="K96" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4518,9 +4553,7 @@
       <c r="I97" t="s">
         <v>147</v>
       </c>
-      <c r="J97" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J97" s="7"/>
       <c r="K97" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4553,9 +4586,7 @@
       <c r="I98" t="s">
         <v>147</v>
       </c>
-      <c r="J98" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J98" s="7"/>
       <c r="K98" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4588,9 +4619,7 @@
       <c r="I99" t="s">
         <v>147</v>
       </c>
-      <c r="J99" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J99" s="7"/>
       <c r="K99" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4623,9 +4652,7 @@
       <c r="I100" t="s">
         <v>147</v>
       </c>
-      <c r="J100" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J100" s="7"/>
       <c r="K100" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4658,9 +4685,7 @@
       <c r="I101" t="s">
         <v>147</v>
       </c>
-      <c r="J101" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J101" s="7"/>
       <c r="K101" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4693,9 +4718,7 @@
       <c r="I102" t="s">
         <v>147</v>
       </c>
-      <c r="J102" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J102" s="7"/>
       <c r="K102" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4728,9 +4751,7 @@
       <c r="I103" t="s">
         <v>147</v>
       </c>
-      <c r="J103" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J103" s="7"/>
       <c r="K103" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4763,9 +4784,7 @@
       <c r="I104" t="s">
         <v>147</v>
       </c>
-      <c r="J104" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J104" s="7"/>
       <c r="K104" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4798,9 +4817,7 @@
       <c r="I105" t="s">
         <v>147</v>
       </c>
-      <c r="J105" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J105" s="7"/>
       <c r="K105" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4833,9 +4850,7 @@
       <c r="I106" t="s">
         <v>147</v>
       </c>
-      <c r="J106" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J106" s="7"/>
       <c r="K106" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4868,9 +4883,7 @@
       <c r="I107" t="s">
         <v>147</v>
       </c>
-      <c r="J107" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J107" s="7"/>
       <c r="K107" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4903,9 +4916,7 @@
       <c r="I108" t="s">
         <v>147</v>
       </c>
-      <c r="J108" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J108" s="7"/>
       <c r="K108" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4938,9 +4949,7 @@
       <c r="I109" t="s">
         <v>147</v>
       </c>
-      <c r="J109" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J109" s="7"/>
       <c r="K109" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4973,9 +4982,7 @@
       <c r="I110" t="s">
         <v>147</v>
       </c>
-      <c r="J110" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J110" s="7"/>
       <c r="K110" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5008,9 +5015,7 @@
       <c r="I111" t="s">
         <v>147</v>
       </c>
-      <c r="J111" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J111" s="7"/>
       <c r="K111" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5043,9 +5048,7 @@
       <c r="I112" t="s">
         <v>147</v>
       </c>
-      <c r="J112" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J112" s="7"/>
       <c r="K112" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5078,9 +5081,7 @@
       <c r="I113" t="s">
         <v>147</v>
       </c>
-      <c r="J113" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J113" s="7"/>
       <c r="K113" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5113,9 +5114,7 @@
       <c r="I114" t="s">
         <v>147</v>
       </c>
-      <c r="J114" s="7" t="s">
-        <v>161</v>
-      </c>
+      <c r="J114" s="7"/>
       <c r="K114" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5313,7 +5312,7 @@
         <v>153</v>
       </c>
       <c r="J119" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K119" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>

</xml_diff>

<commit_message>
converted corum, ctd, generif, gtex. Updated requirements and utility_functions
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CEBC34-8E99-4815-BA67-89BA68CCDF11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B31982-10F5-4798-B16F-BD8F1D31E5D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="173">
   <si>
     <t>Resource</t>
   </si>
@@ -525,9 +525,6 @@
     <t>No analysis in original document</t>
   </si>
   <si>
-    <t>Need access to site</t>
-  </si>
-  <si>
     <t>Files not downloadable</t>
   </si>
   <si>
@@ -547,13 +544,25 @@
   </si>
   <si>
     <t>Original Input File?</t>
+  </si>
+  <si>
+    <t>How was input file generated?</t>
+  </si>
+  <si>
+    <t>Propose new method (ratiomatrix -&gt; map instances at top, U133A probe names on left)</t>
+  </si>
+  <si>
+    <t>No longer maintained</t>
+  </si>
+  <si>
+    <t>Some sites down, cannot find input file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,8 +612,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +647,12 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -641,14 +663,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -659,15 +682,38 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1001,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1232,7 @@
         <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K5">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1230,7 +1276,7 @@
         <v>147</v>
       </c>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K6">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1259,7 +1305,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7">
         <v>16827</v>
@@ -1916,7 +1962,7 @@
         <v>148</v>
       </c>
       <c r="J25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K25">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2210,8 +2256,17 @@
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="C33">
+        <v>27399</v>
+      </c>
+      <c r="D33">
+        <v>984</v>
+      </c>
+      <c r="E33">
+        <v>1347887</v>
       </c>
       <c r="F33">
         <v>17337</v>
@@ -2225,13 +2280,13 @@
       <c r="I33" t="s">
         <v>147</v>
       </c>
-      <c r="K33" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K33">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9994666293974886E-2</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.500215924546614</v>
       </c>
       <c r="M33">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2274,8 +2329,17 @@
       <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>42</v>
+      </c>
+      <c r="C35">
+        <v>43</v>
+      </c>
+      <c r="D35">
+        <v>403</v>
+      </c>
+      <c r="E35">
+        <v>694</v>
       </c>
       <c r="F35">
         <v>1952</v>
@@ -2289,13 +2353,13 @@
       <c r="I35" t="s">
         <v>148</v>
       </c>
-      <c r="K35" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K35">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.0048473656875756E-2</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.10415728650757917</v>
       </c>
       <c r="M35">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2306,7 +2370,7 @@
       <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F36">
@@ -2320,6 +2384,9 @@
       </c>
       <c r="I36" t="s">
         <v>147</v>
+      </c>
+      <c r="J36" t="s">
+        <v>170</v>
       </c>
       <c r="K36" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2338,8 +2405,17 @@
       <c r="A37" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="C37">
+        <v>5257</v>
+      </c>
+      <c r="D37">
+        <v>3719</v>
+      </c>
+      <c r="E37">
+        <v>14531</v>
       </c>
       <c r="F37">
         <v>3753</v>
@@ -2353,13 +2429,13 @@
       <c r="I37" t="s">
         <v>148</v>
       </c>
-      <c r="K37" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K37">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>7.4324388951583164E-4</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.2882092198581561</v>
       </c>
       <c r="M37">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2370,8 +2446,17 @@
       <c r="A38" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="C38">
+        <v>17905</v>
+      </c>
+      <c r="D38">
+        <v>11746</v>
+      </c>
+      <c r="E38">
+        <v>214780</v>
       </c>
       <c r="F38">
         <v>15676</v>
@@ -2385,13 +2470,13 @@
       <c r="I38" t="s">
         <v>148</v>
       </c>
-      <c r="K38" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K38">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.0212439957695259E-3</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.3395953396701843</v>
       </c>
       <c r="M38">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2402,8 +2487,17 @@
       <c r="A39" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="C39">
+        <v>18974</v>
+      </c>
+      <c r="D39">
+        <v>7213</v>
+      </c>
+      <c r="E39">
+        <v>6839499</v>
       </c>
       <c r="F39">
         <v>17487</v>
@@ -2417,13 +2511,13 @@
       <c r="I39" t="s">
         <v>147</v>
       </c>
-      <c r="K39" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+      <c r="K39">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9974615565856896E-2</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.30635843794665146</v>
       </c>
       <c r="M39">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2434,7 +2528,7 @@
       <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>48</v>
       </c>
       <c r="F40">
@@ -2448,6 +2542,9 @@
       </c>
       <c r="I40" t="s">
         <v>148</v>
+      </c>
+      <c r="J40" t="s">
+        <v>169</v>
       </c>
       <c r="K40" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2490,9 +2587,6 @@
       <c r="I41" t="s">
         <v>148</v>
       </c>
-      <c r="J41" t="s">
-        <v>162</v>
-      </c>
       <c r="K41">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7610993657505285E-2</v>
@@ -2534,9 +2628,6 @@
       <c r="I42" t="s">
         <v>148</v>
       </c>
-      <c r="J42" t="s">
-        <v>162</v>
-      </c>
       <c r="K42">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>8.0283492347445837E-3</v>
@@ -2578,9 +2669,6 @@
       <c r="I43" t="s">
         <v>148</v>
       </c>
-      <c r="J43" t="s">
-        <v>162</v>
-      </c>
       <c r="K43">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.026887733395156E-3</v>
@@ -2622,9 +2710,6 @@
       <c r="I44" t="s">
         <v>148</v>
       </c>
-      <c r="J44" t="s">
-        <v>162</v>
-      </c>
       <c r="K44">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.1837188401683933E-2</v>
@@ -2872,7 +2957,7 @@
       <c r="A51" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>62</v>
       </c>
       <c r="F51">
@@ -2886,6 +2971,9 @@
       </c>
       <c r="I51" t="s">
         <v>148</v>
+      </c>
+      <c r="J51" t="s">
+        <v>171</v>
       </c>
       <c r="K51" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2986,7 +3074,7 @@
       <c r="A54" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="10" t="s">
         <v>67</v>
       </c>
       <c r="F54">
@@ -3002,7 +3090,7 @@
         <v>147</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K54" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3078,7 +3166,7 @@
         <v>148</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K56" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3446,7 +3534,7 @@
         <v>148</v>
       </c>
       <c r="J66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K66" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3481,7 +3569,7 @@
         <v>148</v>
       </c>
       <c r="J67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K67" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3566,7 +3654,7 @@
         <v>148</v>
       </c>
       <c r="J69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K69">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4003,7 +4091,7 @@
       <c r="A81" t="s">
         <v>97</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>98</v>
       </c>
       <c r="F81">
@@ -4017,6 +4105,9 @@
       </c>
       <c r="I81" t="s">
         <v>147</v>
+      </c>
+      <c r="J81" t="s">
+        <v>172</v>
       </c>
       <c r="K81" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5370,6 +5461,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="L2:L120">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0.95</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
revised Bgee, changed order of removeandimpute in Achilles and bgee
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B31982-10F5-4798-B16F-BD8F1D31E5D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD44AD-D299-41CE-893E-9755C2FBFD40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="176">
   <si>
     <t>Resource</t>
   </si>
@@ -465,18 +465,6 @@
     <t>WikiPathways</t>
   </si>
   <si>
-    <t>Gene - Attribute associations</t>
-  </si>
-  <si>
-    <t>Binary Matrix</t>
-  </si>
-  <si>
-    <t>Tertiary Matrix</t>
-  </si>
-  <si>
-    <t>RNA-Seq (numeric data)</t>
-  </si>
-  <si>
     <t>Type of Matrix</t>
   </si>
   <si>
@@ -556,6 +544,27 @@
   </si>
   <si>
     <t>Some sites down, cannot find input file</t>
+  </si>
+  <si>
+    <t>Appyter</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Appyter Checked/Uploaded</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>" (dev)</t>
+  </si>
+  <si>
+    <t>bgee (ana)</t>
+  </si>
+  <si>
+    <t>" (ana + dev)</t>
   </si>
 </sst>
 </file>
@@ -692,7 +701,17 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -705,11 +724,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -745,6 +784,19 @@
     <tableColumn id="7" xr3:uid="{FC31696F-B15D-4C63-941B-6D259049B49F}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E6570D1-E748-4481-A019-4350A6937CEB}" name="Table5" displayName="Table5" ref="A1:D83" totalsRowShown="0">
+  <autoFilter ref="A1:D83" xr:uid="{7167200E-1BC9-4E25-B3DC-B97A94FBAA82}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{036140A4-066F-4FFE-A3A7-383BDD6ED976}" name="Resource"/>
+    <tableColumn id="3" xr3:uid="{D5872A27-B44F-41FC-992C-B9DBAB0D8D74}" name="Data Set"/>
+    <tableColumn id="2" xr3:uid="{88160321-3BFB-4A18-ACAC-9A03438F8691}" name="Appyter"/>
+    <tableColumn id="4" xr3:uid="{3C29EDB3-5D2B-4B80-91AC-48AF2314FD99}" name="Appyter Checked/Uploaded"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1047,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView topLeftCell="A106" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,13 +1126,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1092,14 +1144,14 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1124,7 +1176,7 @@
         <v>2652264</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K2">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1144,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F3">
         <v>18822</v>
@@ -1156,7 +1208,7 @@
         <v>377048</v>
       </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K3" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1188,7 +1240,7 @@
         <v>92925</v>
       </c>
       <c r="I4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K4" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1229,10 +1281,10 @@
         <v>55716</v>
       </c>
       <c r="I5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K5">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1273,10 +1325,10 @@
         <v>56388</v>
       </c>
       <c r="I6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K6">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1305,7 +1357,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F7">
         <v>16827</v>
@@ -1317,7 +1369,7 @@
         <v>27015</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K7" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1358,7 +1410,7 @@
         <v>413974</v>
       </c>
       <c r="I8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K8">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1390,7 +1442,7 @@
         <v>33653</v>
       </c>
       <c r="I9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K9" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1422,7 +1474,7 @@
         <v>44822</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K10" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1454,7 +1506,7 @@
         <v>587286</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K11" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1486,7 +1538,7 @@
         <v>44822</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K12" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1518,10 +1570,10 @@
         <v>1156878</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K13" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1553,7 +1605,7 @@
         <v>501308</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K14" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1585,7 +1637,7 @@
         <v>608457</v>
       </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K15" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1617,7 +1669,7 @@
         <v>140739</v>
       </c>
       <c r="I16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K16" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1649,7 +1701,7 @@
         <v>500364</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K17" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1681,7 +1733,7 @@
         <v>470861</v>
       </c>
       <c r="I18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K18" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1713,7 +1765,7 @@
         <v>95958</v>
       </c>
       <c r="I19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K19" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1754,7 +1806,7 @@
         <v>4308050</v>
       </c>
       <c r="I20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K20">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1795,7 +1847,7 @@
         <v>603839</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K21">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1836,7 +1888,7 @@
         <v>14983142</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K22">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1877,7 +1929,7 @@
         <v>3163055</v>
       </c>
       <c r="I23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K23">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1918,7 +1970,7 @@
         <v>660778</v>
       </c>
       <c r="I24" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K24">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1959,10 +2011,10 @@
         <v>9141706</v>
       </c>
       <c r="I25" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="K25">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2003,7 +2055,7 @@
         <v>132835</v>
       </c>
       <c r="I26" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K26">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2044,7 +2096,7 @@
         <v>22100</v>
       </c>
       <c r="I27" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K27">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2085,7 +2137,7 @@
         <v>139136</v>
       </c>
       <c r="I28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K28">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2126,7 +2178,7 @@
         <v>228687</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K29">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2167,7 +2219,7 @@
         <v>274099</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K30">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2193,10 +2245,10 @@
         <v>9819</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J31" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K31" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2237,7 +2289,7 @@
         <v>111694</v>
       </c>
       <c r="I32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K32">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2278,7 +2330,7 @@
         <v>898462</v>
       </c>
       <c r="I33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K33">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2310,7 +2362,7 @@
         <v>1361218</v>
       </c>
       <c r="I34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K34" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2351,7 +2403,7 @@
         <v>6663</v>
       </c>
       <c r="I35" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K35">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2383,10 +2435,10 @@
         <v>142745</v>
       </c>
       <c r="I36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K36" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2427,7 +2479,7 @@
         <v>11280</v>
       </c>
       <c r="I37" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K37">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2468,7 +2520,7 @@
         <v>160332</v>
       </c>
       <c r="I38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K38">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2509,7 +2561,7 @@
         <v>22325153</v>
       </c>
       <c r="I39" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K39">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2541,10 +2593,10 @@
         <v>6088</v>
       </c>
       <c r="I40" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="K40" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2585,7 +2637,7 @@
         <v>352</v>
       </c>
       <c r="I41" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K41">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2626,7 +2678,7 @@
         <v>2429</v>
       </c>
       <c r="I42" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K42">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2667,7 +2719,7 @@
         <v>13355</v>
       </c>
       <c r="I43" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K43">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2708,7 +2760,7 @@
         <v>1784</v>
       </c>
       <c r="I44" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K44">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2749,7 +2801,7 @@
         <v>293199</v>
       </c>
       <c r="I45" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K45">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2790,7 +2842,7 @@
         <v>12571</v>
       </c>
       <c r="I46" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K46">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2831,7 +2883,7 @@
         <v>16240</v>
       </c>
       <c r="I47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K47">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2872,7 +2924,7 @@
         <v>158860</v>
       </c>
       <c r="I48" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K48">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2904,7 +2956,7 @@
         <v>1530489</v>
       </c>
       <c r="I49" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J49" s="7"/>
       <c r="K49" t="e">
@@ -2937,7 +2989,7 @@
         <v>2220608</v>
       </c>
       <c r="I50" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J50" s="7"/>
       <c r="K50" t="e">
@@ -2970,10 +3022,10 @@
         <v>81427</v>
       </c>
       <c r="I51" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J51" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K51" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3014,7 +3066,7 @@
         <v>109097</v>
       </c>
       <c r="I52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K52">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3055,7 +3107,7 @@
         <v>42691</v>
       </c>
       <c r="I53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K53">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3087,10 +3139,10 @@
         <v>1787693</v>
       </c>
       <c r="I54" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K54" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3131,7 +3183,7 @@
         <v>9452</v>
       </c>
       <c r="I55" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K55">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3163,10 +3215,10 @@
         <v>404516</v>
       </c>
       <c r="I56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K56" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3207,7 +3259,7 @@
         <v>195513</v>
       </c>
       <c r="I57" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K57">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3248,7 +3300,7 @@
         <v>43458</v>
       </c>
       <c r="I58" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K58">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3289,7 +3341,7 @@
         <v>48304</v>
       </c>
       <c r="I59" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K59">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3309,10 +3361,10 @@
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I60" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K60" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3344,7 +3396,7 @@
         <v>10940561</v>
       </c>
       <c r="I61" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K61" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3376,7 +3428,7 @@
         <v>64221</v>
       </c>
       <c r="I62" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K62" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3417,7 +3469,7 @@
         <v>13759</v>
       </c>
       <c r="I63" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K63">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3458,7 +3510,7 @@
         <v>427</v>
       </c>
       <c r="I64" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K64">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3499,7 +3551,7 @@
         <v>18773</v>
       </c>
       <c r="I65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K65">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3531,10 +3583,10 @@
         <v>60246</v>
       </c>
       <c r="I66" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J66" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K66" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3566,10 +3618,10 @@
         <v>70482</v>
       </c>
       <c r="I67" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J67" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K67" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3610,7 +3662,7 @@
         <v>415410</v>
       </c>
       <c r="I68" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K68">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3651,10 +3703,10 @@
         <v>126176</v>
       </c>
       <c r="I69" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J69" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K69">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3695,7 +3747,7 @@
         <v>829693</v>
       </c>
       <c r="I70" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K70">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3736,7 +3788,7 @@
         <v>52079</v>
       </c>
       <c r="I71" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K71">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3777,7 +3829,7 @@
         <v>434311</v>
       </c>
       <c r="I72" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K72">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3818,7 +3870,7 @@
         <v>134408</v>
       </c>
       <c r="I73" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K73">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3859,7 +3911,7 @@
         <v>417884</v>
       </c>
       <c r="I74" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K74">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3876,10 +3928,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C75" s="5">
         <v>4067</v>
@@ -3929,7 +3981,7 @@
         <v>1257932</v>
       </c>
       <c r="I76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K76">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3970,7 +4022,7 @@
         <v>1125042</v>
       </c>
       <c r="I77" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K77">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3996,10 +4048,10 @@
         <v>2716</v>
       </c>
       <c r="I78" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J78" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K78" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4016,10 +4068,10 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C79">
         <v>13894</v>
@@ -4031,7 +4083,7 @@
         <v>188518</v>
       </c>
       <c r="I79" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K79">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4072,7 +4124,7 @@
         <v>105556</v>
       </c>
       <c r="I80" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K80">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4104,10 +4156,10 @@
         <v>209475</v>
       </c>
       <c r="I81" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J81" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K81" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4148,7 +4200,7 @@
         <v>5898446</v>
       </c>
       <c r="I82" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K82">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4180,7 +4232,7 @@
         <v>72970</v>
       </c>
       <c r="I83" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J83" s="7"/>
       <c r="K83" t="e">
@@ -4213,7 +4265,7 @@
         <v>398197</v>
       </c>
       <c r="I84" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J84" s="7"/>
       <c r="K84" t="e">
@@ -4246,7 +4298,7 @@
         <v>489769</v>
       </c>
       <c r="I85" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J85" s="7"/>
       <c r="K85" t="e">
@@ -4279,7 +4331,7 @@
         <v>1124480</v>
       </c>
       <c r="I86" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J86" s="7"/>
       <c r="K86" t="e">
@@ -4312,7 +4364,7 @@
         <v>284538</v>
       </c>
       <c r="I87" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J87" s="7"/>
       <c r="K87" t="e">
@@ -4345,7 +4397,7 @@
         <v>41743</v>
       </c>
       <c r="I88" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" t="e">
@@ -4378,7 +4430,7 @@
         <v>459393</v>
       </c>
       <c r="I89" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J89" s="7"/>
       <c r="K89" t="e">
@@ -4411,7 +4463,7 @@
         <v>186087</v>
       </c>
       <c r="I90" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J90" s="7"/>
       <c r="K90" t="e">
@@ -4444,7 +4496,7 @@
         <v>159910</v>
       </c>
       <c r="I91" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J91" s="7"/>
       <c r="K91" t="e">
@@ -4477,7 +4529,7 @@
         <v>527943</v>
       </c>
       <c r="I92" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J92" s="7"/>
       <c r="K92" t="e">
@@ -4510,7 +4562,7 @@
         <v>84676</v>
       </c>
       <c r="I93" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J93" s="7"/>
       <c r="K93" t="e">
@@ -4543,7 +4595,7 @@
         <v>565628</v>
       </c>
       <c r="I94" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J94" s="7"/>
       <c r="K94" t="e">
@@ -4576,7 +4628,7 @@
         <v>299781</v>
       </c>
       <c r="I95" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J95" s="7"/>
       <c r="K95" t="e">
@@ -4609,7 +4661,7 @@
         <v>387737</v>
       </c>
       <c r="I96" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J96" s="7"/>
       <c r="K96" t="e">
@@ -4642,7 +4694,7 @@
         <v>533911</v>
       </c>
       <c r="I97" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J97" s="7"/>
       <c r="K97" t="e">
@@ -4675,7 +4727,7 @@
         <v>513287</v>
       </c>
       <c r="I98" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J98" s="7"/>
       <c r="K98" t="e">
@@ -4708,7 +4760,7 @@
         <v>42973</v>
       </c>
       <c r="I99" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J99" s="7"/>
       <c r="K99" t="e">
@@ -4741,7 +4793,7 @@
         <v>81072</v>
       </c>
       <c r="I100" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J100" s="7"/>
       <c r="K100" t="e">
@@ -4774,7 +4826,7 @@
         <v>399505</v>
       </c>
       <c r="I101" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J101" s="7"/>
       <c r="K101" t="e">
@@ -4807,7 +4859,7 @@
         <v>169642</v>
       </c>
       <c r="I102" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J102" s="7"/>
       <c r="K102" t="e">
@@ -4840,7 +4892,7 @@
         <v>172133</v>
       </c>
       <c r="I103" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J103" s="7"/>
       <c r="K103" t="e">
@@ -4873,7 +4925,7 @@
         <v>509464</v>
       </c>
       <c r="I104" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J104" s="7"/>
       <c r="K104" t="e">
@@ -4906,7 +4958,7 @@
         <v>162528</v>
       </c>
       <c r="I105" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J105" s="7"/>
       <c r="K105" t="e">
@@ -4939,7 +4991,7 @@
         <v>245886</v>
       </c>
       <c r="I106" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J106" s="7"/>
       <c r="K106" t="e">
@@ -4972,7 +5024,7 @@
         <v>439949</v>
       </c>
       <c r="I107" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J107" s="7"/>
       <c r="K107" t="e">
@@ -5005,7 +5057,7 @@
         <v>428467</v>
       </c>
       <c r="I108" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J108" s="7"/>
       <c r="K108" t="e">
@@ -5038,7 +5090,7 @@
         <v>145048</v>
       </c>
       <c r="I109" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J109" s="7"/>
       <c r="K109" t="e">
@@ -5071,7 +5123,7 @@
         <v>112695</v>
       </c>
       <c r="I110" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J110" s="7"/>
       <c r="K110" t="e">
@@ -5104,7 +5156,7 @@
         <v>525419</v>
       </c>
       <c r="I111" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J111" s="7"/>
       <c r="K111" t="e">
@@ -5137,7 +5189,7 @@
         <v>56384</v>
       </c>
       <c r="I112" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J112" s="7"/>
       <c r="K112" t="e">
@@ -5170,7 +5222,7 @@
         <v>542785</v>
       </c>
       <c r="I113" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J113" s="7"/>
       <c r="K113" t="e">
@@ -5203,7 +5255,7 @@
         <v>73121</v>
       </c>
       <c r="I114" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J114" s="7"/>
       <c r="K114" t="e">
@@ -5245,7 +5297,7 @@
         <v>848829</v>
       </c>
       <c r="I115" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K115">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5286,7 +5338,7 @@
         <v>197848</v>
       </c>
       <c r="I116" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K116">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5327,7 +5379,7 @@
         <v>117708</v>
       </c>
       <c r="I117" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K117">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5368,7 +5420,7 @@
         <v>134717</v>
       </c>
       <c r="I118" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K118">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5400,10 +5452,10 @@
         <v>2338</v>
       </c>
       <c r="I119" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J119" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K119" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5444,7 +5496,7 @@
         <v>15503</v>
       </c>
       <c r="I120" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K120">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5462,11 +5514,11 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="L2:L120">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>1.05</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
       <formula>0.95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5478,48 +5530,736 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269FE0F6-69DC-44D9-8AD6-854C38438A66}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558B39D-DF60-4E54-8F48-AB6C60277695}">
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <f>C1+C2</f>
-        <v>117</v>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>86</v>
+      </c>
+      <c r="B66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>133</v>
+      </c>
+      <c r="B78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>135</v>
+      </c>
+      <c r="B80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>135</v>
+      </c>
+      <c r="B81" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D83">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Checked"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Uploaded"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised GO, added comments to others
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493C4C6-7341-4326-9AD0-D385B89BABCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E660B9A-B02E-4AC3-952F-F9C2D67A8DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="1060" windowWidth="18000" windowHeight="9180" activeTab="1" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="178">
   <si>
     <t>Resource</t>
   </si>
@@ -565,6 +565,12 @@
   </si>
   <si>
     <t>" (ana + dev)</t>
+  </si>
+  <si>
+    <t>Reviewed and corrected</t>
+  </si>
+  <si>
+    <t>Probably GO ID retained in original</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,6 +1224,9 @@
       <c r="I2" t="s">
         <v>144</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="K2">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.0048473656875756E-2</v>
@@ -1259,6 +1268,7 @@
       <c r="I3" t="s">
         <v>144</v>
       </c>
+      <c r="J3" s="7"/>
       <c r="K3">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7610993657505285E-2</v>
@@ -1452,7 +1462,7 @@
       <c r="I8" t="s">
         <v>144</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="7" t="s">
         <v>162</v>
       </c>
       <c r="K8">
@@ -1701,6 +1711,9 @@
       <c r="I14" t="s">
         <v>144</v>
       </c>
+      <c r="J14" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="K14">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7457650505748228E-3</v>
@@ -1783,6 +1796,9 @@
       <c r="I16" t="s">
         <v>144</v>
       </c>
+      <c r="J16" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="K16">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.3852448018060798E-3</v>
@@ -1823,6 +1839,9 @@
       </c>
       <c r="I17" t="s">
         <v>144</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="K17">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -5573,8 +5592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558B39D-DF60-4E54-8F48-AB6C60277695}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
revised humap, jensen lab, mgi, mirtarbase
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A497801-A3C6-44A2-8E00-E29C35018EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A87126-5C91-45BF-B839-9F83F1027D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
revised orphanet, pathway commons, phgkb, reactome. Roadmap epigenomics needs more work
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A87126-5C91-45BF-B839-9F83F1027D62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28631F20-25A6-4412-AEFB-EEB93D43293C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="179">
   <si>
     <t>Resource</t>
   </si>
@@ -1148,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B74" sqref="B74:E74"/>
     </sheetView>
   </sheetViews>
@@ -5598,8 +5598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558B39D-DF60-4E54-8F48-AB6C60277695}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5955,6 +5955,9 @@
       <c r="B35" t="s">
         <v>48</v>
       </c>
+      <c r="D35" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -5963,6 +5966,9 @@
       <c r="B36" t="s">
         <v>50</v>
       </c>
+      <c r="D36" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -5995,6 +6001,9 @@
       <c r="B40" t="s">
         <v>55</v>
       </c>
+      <c r="D40" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -6027,6 +6036,9 @@
       <c r="B44" t="s">
         <v>60</v>
       </c>
+      <c r="D44" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -6035,6 +6047,9 @@
       <c r="B45" t="s">
         <v>61</v>
       </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -6043,6 +6058,9 @@
       <c r="B46" t="s">
         <v>62</v>
       </c>
+      <c r="D46" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -6051,6 +6069,9 @@
       <c r="B47" t="s">
         <v>64</v>
       </c>
+      <c r="D47" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -6060,39 +6081,51 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>66</v>
       </c>
       <c r="B49" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>68</v>
       </c>
       <c r="B50" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>69</v>
       </c>
       <c r="B51" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
       <c r="B52" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -6100,7 +6133,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -6108,7 +6141,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -6116,7 +6149,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -6124,7 +6157,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -6132,15 +6165,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
       <c r="B58" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -6148,23 +6184,29 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
       <c r="B60" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>80</v>
       </c>
       <c r="B61" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -6172,31 +6214,40 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
       <c r="B63" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>83</v>
       </c>
       <c r="B64" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>86</v>
       </c>
       <c r="B65" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -6204,7 +6255,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -6212,23 +6263,29 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>89</v>
       </c>
       <c r="B68" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>91</v>
       </c>
       <c r="B69" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -6236,7 +6293,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -6244,7 +6301,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>92</v>
       </c>
@@ -6252,7 +6309,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>95</v>
       </c>
@@ -6260,7 +6317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -6268,7 +6325,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -6276,7 +6333,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -6284,7 +6341,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>99</v>
       </c>
@@ -6292,7 +6349,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>133</v>
       </c>
@@ -6300,7 +6357,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>135</v>
       </c>
@@ -6308,7 +6365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
changed similarity to standardized matrix
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28631F20-25A6-4412-AEFB-EEB93D43293C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEB1389-5B4C-46B0-817E-45E5C66DA080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="173">
   <si>
     <t>Resource</t>
   </si>
@@ -546,27 +545,6 @@
     <t>Some sites down, cannot find input file</t>
   </si>
   <si>
-    <t>Appyter</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>Appyter Checked/Uploaded</t>
-  </si>
-  <si>
-    <t>Checked</t>
-  </si>
-  <si>
-    <t>" (dev)</t>
-  </si>
-  <si>
-    <t>bgee (ana)</t>
-  </si>
-  <si>
-    <t>" (ana + dev)</t>
-  </si>
-  <si>
     <t>Reviewed and corrected</t>
   </si>
   <si>
@@ -574,6 +552,9 @@
   </si>
   <si>
     <t>Original number is clearly wrong</t>
+  </si>
+  <si>
+    <t>Standard matrix for attribute matrix</t>
   </si>
 </sst>
 </file>
@@ -638,7 +619,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +652,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -681,15 +668,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -701,8 +689,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -710,77 +700,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -833,19 +753,6 @@
     <tableColumn id="7" xr3:uid="{FC31696F-B15D-4C63-941B-6D259049B49F}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E6570D1-E748-4481-A019-4350A6937CEB}" name="Table5" displayName="Table5" ref="A1:D83" totalsRowShown="0">
-  <autoFilter ref="A1:D83" xr:uid="{7167200E-1BC9-4E25-B3DC-B97A94FBAA82}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{036140A4-066F-4FFE-A3A7-383BDD6ED976}" name="Resource"/>
-    <tableColumn id="3" xr3:uid="{D5872A27-B44F-41FC-992C-B9DBAB0D8D74}" name="Data Set"/>
-    <tableColumn id="2" xr3:uid="{88160321-3BFB-4A18-ACAC-9A03438F8691}" name="Appyter"/>
-    <tableColumn id="4" xr3:uid="{3C29EDB3-5D2B-4B80-91AC-48AF2314FD99}" name="Appyter Checked/Uploaded"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1148,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74:E74"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1107,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1228,7 +1135,7 @@
         <v>143</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K2">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1311,7 +1218,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5">
@@ -1355,7 +1262,7 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6">
@@ -1440,7 +1347,7 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C8">
@@ -1833,7 +1740,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1874,7 +1781,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1915,10 +1822,10 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C22">
@@ -1956,10 +1863,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C23">
@@ -1997,10 +1904,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C24">
@@ -2038,10 +1945,10 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C25">
@@ -2082,7 +1989,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2123,7 +2030,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2164,7 +2071,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2205,7 +2112,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2246,7 +2153,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2316,7 +2223,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2357,10 +2264,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C33">
@@ -2383,6 +2290,9 @@
       </c>
       <c r="I33" t="s">
         <v>143</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="K33">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2430,7 +2340,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2458,7 +2368,7 @@
         <v>144</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="K35">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2509,10 +2419,10 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C37">
@@ -2550,10 +2460,10 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C38">
@@ -2591,10 +2501,10 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C39">
@@ -2667,10 +2577,10 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C41">
@@ -2709,10 +2619,10 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C42">
@@ -2750,10 +2660,10 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C43">
@@ -2791,10 +2701,10 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C44">
@@ -2832,10 +2742,10 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C45">
@@ -2873,10 +2783,10 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C46">
@@ -2914,10 +2824,10 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C47">
@@ -2955,10 +2865,10 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C48">
@@ -3097,10 +3007,10 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C52">
@@ -3138,10 +3048,10 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C53">
@@ -3214,10 +3124,10 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C55" s="9">
@@ -3290,10 +3200,10 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C57">
@@ -3318,7 +3228,7 @@
         <v>144</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K57">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3334,10 +3244,10 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C58">
@@ -3362,7 +3272,7 @@
         <v>144</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K58">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3378,10 +3288,10 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C59">
@@ -3406,7 +3316,7 @@
         <v>144</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K59">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3509,10 +3419,10 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>77</v>
       </c>
       <c r="C63">
@@ -3550,10 +3460,10 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C64">
@@ -3591,10 +3501,10 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>79</v>
       </c>
       <c r="C65">
@@ -3702,10 +3612,10 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C68">
@@ -3743,10 +3653,10 @@
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C69">
@@ -3787,10 +3697,10 @@
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C70">
@@ -3828,10 +3738,10 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C71">
@@ -3869,10 +3779,10 @@
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C72">
@@ -3910,10 +3820,10 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C73">
@@ -3951,10 +3861,10 @@
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C74">
@@ -3992,10 +3902,10 @@
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>155</v>
       </c>
       <c r="C75" s="5">
@@ -4021,10 +3931,10 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C76">
@@ -4062,10 +3972,10 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C77">
@@ -4132,10 +4042,10 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C79">
@@ -4164,10 +4074,10 @@
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C80">
@@ -4240,10 +4150,10 @@
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C82">
@@ -5337,10 +5247,10 @@
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C115">
@@ -5378,10 +5288,10 @@
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C116">
@@ -5419,10 +5329,10 @@
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C117">
@@ -5460,10 +5370,10 @@
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C118">
@@ -5536,10 +5446,10 @@
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C120">
@@ -5579,10 +5489,10 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="L2:L120">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5592,845 +5502,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558B39D-DF60-4E54-8F48-AB6C60277695}">
-  <dimension ref="A1:D83"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>66</v>
-      </c>
-      <c r="B49" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>74</v>
-      </c>
-      <c r="B55" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" t="s">
-        <v>79</v>
-      </c>
-      <c r="D60" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>80</v>
-      </c>
-      <c r="B61" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>83</v>
-      </c>
-      <c r="B64" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>86</v>
-      </c>
-      <c r="B66" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>89</v>
-      </c>
-      <c r="B68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D68" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>91</v>
-      </c>
-      <c r="B69" t="s">
-        <v>91</v>
-      </c>
-      <c r="D69" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>155</v>
-      </c>
-      <c r="B70" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>92</v>
-      </c>
-      <c r="B71" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>92</v>
-      </c>
-      <c r="B72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>95</v>
-      </c>
-      <c r="B73" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>147</v>
-      </c>
-      <c r="B74" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>96</v>
-      </c>
-      <c r="B75" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>99</v>
-      </c>
-      <c r="B77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>133</v>
-      </c>
-      <c r="B78" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>135</v>
-      </c>
-      <c r="B79" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>135</v>
-      </c>
-      <c r="B80" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>135</v>
-      </c>
-      <c r="B81" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>139</v>
-      </c>
-      <c r="B82" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D2:D83">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Checked"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"Uploaded"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"Run"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D83">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Uploaded"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Run"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Uploaded"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
removed sparse keyword bgee
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEB1389-5B4C-46B0-817E-45E5C66DA080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB9E83-B62A-4ADC-ADFC-CEB703810C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -536,9 +536,6 @@
     <t>How was input file generated?</t>
   </si>
   <si>
-    <t>Propose new method (ratiomatrix -&gt; map instances at top, U133A probe names on left)</t>
-  </si>
-  <si>
     <t>No longer maintained</t>
   </si>
   <si>
@@ -555,6 +552,9 @@
   </si>
   <si>
     <t>Standard matrix for attribute matrix</t>
+  </si>
+  <si>
+    <t>Unable to find original file</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
         <v>143</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K2">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1825,7 +1825,7 @@
       <c r="A22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C22">
@@ -2267,17 +2267,17 @@
       <c r="A33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C33">
-        <v>27399</v>
+        <v>31981</v>
       </c>
       <c r="D33">
         <v>984</v>
       </c>
       <c r="E33">
-        <v>1347887</v>
+        <v>1573497</v>
       </c>
       <c r="F33">
         <v>17337</v>
@@ -2292,15 +2292,15 @@
         <v>143</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K33">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.9994666293974886E-2</v>
+        <v>5.0001010508526025E-2</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
-        <v>1.500215924546614</v>
+        <v>1.751322816101293</v>
       </c>
       <c r="M33">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2343,17 +2343,17 @@
       <c r="A35" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C35">
-        <v>43</v>
+        <v>1644</v>
       </c>
       <c r="D35">
-        <v>403</v>
+        <v>4371</v>
       </c>
       <c r="E35">
-        <v>694</v>
+        <v>8962</v>
       </c>
       <c r="F35">
         <v>1952</v>
@@ -2368,15 +2368,15 @@
         <v>144</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K35">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.0048473656875756E-2</v>
+        <v>1.2471604208449741E-3</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>0.10415728650757917</v>
+        <v>1.3450397718745311</v>
       </c>
       <c r="M35">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -2384,10 +2384,10 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" t="s">
         <v>43</v>
       </c>
       <c r="F36">
@@ -2403,7 +2403,7 @@
         <v>143</v>
       </c>
       <c r="J36" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="K36" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2422,7 +2422,7 @@
       <c r="A37" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C37">
@@ -2463,7 +2463,7 @@
       <c r="A38" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C38">
@@ -2991,7 +2991,7 @@
         <v>144</v>
       </c>
       <c r="J51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K51" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3228,7 +3228,7 @@
         <v>144</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K57">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3272,7 +3272,7 @@
         <v>144</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K58">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -3316,7 +3316,7 @@
         <v>144</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K59">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -4134,7 +4134,7 @@
         <v>143</v>
       </c>
       <c r="J81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K81" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>

</xml_diff>

<commit_message>
changes ot drugbank, created cosmic cnv, tcga
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB9E83-B62A-4ADC-ADFC-CEB703810C85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837174E-68F1-4521-A8A9-1A5C3D59F17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$121</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="170">
   <si>
     <t>Resource</t>
   </si>
@@ -527,34 +527,25 @@
     <t>Original does not take probability into account</t>
   </si>
   <si>
-    <t>Website no longer live</t>
-  </si>
-  <si>
-    <t>Original Input File?</t>
-  </si>
-  <si>
-    <t>How was input file generated?</t>
-  </si>
-  <si>
-    <t>No longer maintained</t>
-  </si>
-  <si>
-    <t>Some sites down, cannot find input file</t>
-  </si>
-  <si>
-    <t>Reviewed and corrected</t>
-  </si>
-  <si>
     <t>Probably GO ID retained in original</t>
   </si>
   <si>
     <t>Original number is clearly wrong</t>
   </si>
   <si>
-    <t>Standard matrix for attribute matrix</t>
-  </si>
-  <si>
     <t>Unable to find original file</t>
+  </si>
+  <si>
+    <t>Unable to find original file (Original uses GWASCatalog file)</t>
+  </si>
+  <si>
+    <t>Website dead</t>
+  </si>
+  <si>
+    <t>COSMIC</t>
+  </si>
+  <si>
+    <t>Removed sparse attributes</t>
   </si>
 </sst>
 </file>
@@ -619,7 +610,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,12 +639,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -668,16 +653,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -689,11 +673,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
-    <cellStyle name="60% - Accent2" xfId="5" builtinId="36"/>
+  <cellStyles count="6">
+    <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -735,10 +717,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE186E64-132B-4E6F-BBD5-769A36DC41A2}" name="Table1" displayName="Table1" ref="A1:J120" totalsRowShown="0">
-  <autoFilter ref="A1:J120" xr:uid="{5D1A7ADB-D789-4B9C-BF75-B396CFD6A519}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J120">
-    <sortCondition ref="A1:A120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE186E64-132B-4E6F-BBD5-769A36DC41A2}" name="Table1" displayName="Table1" ref="A1:J121" totalsRowShown="0">
+  <autoFilter ref="A1:J121" xr:uid="{5D1A7ADB-D789-4B9C-BF75-B396CFD6A519}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J121">
+    <sortCondition ref="A1:A121"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AFD3E64B-E874-4397-A348-505BB47ED81A}" name="Resource"/>
@@ -1053,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1089,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1135,7 +1117,7 @@
         <v>143</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="K2">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -1174,7 +1156,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L66" si="0">IF(COUNTA(E3),E3/H3,1)</f>
+        <f t="shared" ref="L3:L67" si="0">IF(COUNTA(E3),E3/H3,1)</f>
         <v>1</v>
       </c>
       <c r="M3">
@@ -1740,7 +1722,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1781,7 +1763,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1822,7 +1804,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1863,10 +1845,10 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C23">
@@ -1904,10 +1886,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C24">
@@ -1945,20 +1927,20 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>36294</v>
+        <v>36299</v>
       </c>
       <c r="D25">
         <v>10941</v>
       </c>
       <c r="E25">
-        <v>11226560</v>
+        <v>11227184</v>
       </c>
       <c r="F25">
         <v>16289</v>
@@ -1977,11 +1959,11 @@
       </c>
       <c r="K25">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>2.8271890418803871E-2</v>
+        <v>2.8269567316951488E-2</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>1.2280596203815786</v>
+        <v>1.2281278789757624</v>
       </c>
       <c r="M25">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
@@ -1989,7 +1971,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2030,7 +2012,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2071,7 +2053,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2112,7 +2094,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2153,7 +2135,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2206,9 +2188,6 @@
       <c r="I31" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J31" t="s">
-        <v>157</v>
-      </c>
       <c r="K31" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -2223,7 +2202,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2264,7 +2243,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2291,9 +2270,7 @@
       <c r="I33" t="s">
         <v>143</v>
       </c>
-      <c r="J33" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="J33" s="7"/>
       <c r="K33">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.0001010508526025E-2</v>
@@ -2311,7 +2288,7 @@
       <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>41</v>
       </c>
       <c r="F34">
@@ -2340,7 +2317,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2367,9 +2344,7 @@
       <c r="I35" t="s">
         <v>144</v>
       </c>
-      <c r="J35" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="J35" s="7"/>
       <c r="K35">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.2471604208449741E-3</v>
@@ -2384,7 +2359,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B36" t="s">
@@ -2403,7 +2378,7 @@
         <v>143</v>
       </c>
       <c r="J36" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="K36" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
@@ -2419,7 +2394,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2460,482 +2435,462 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>17905</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>11746</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>214780</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>15676</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>10366</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>160332</v>
       </c>
-      <c r="I38" t="s">
-        <v>144</v>
-      </c>
-      <c r="K38">
+      <c r="I39" t="s">
+        <v>144</v>
+      </c>
+      <c r="K39">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0212439957695259E-3</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <f t="shared" si="0"/>
         <v>1.3395953396701843</v>
       </c>
-      <c r="M38">
+      <c r="M39">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>9.8667415117542536E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C39">
-        <v>18974</v>
-      </c>
-      <c r="D39">
-        <v>7213</v>
-      </c>
-      <c r="E39">
-        <v>6839499</v>
-      </c>
-      <c r="F39">
+      <c r="C40">
+        <v>24343</v>
+      </c>
+      <c r="D40">
+        <v>3197</v>
+      </c>
+      <c r="E40">
+        <v>3886596</v>
+      </c>
+      <c r="F40">
         <v>17487</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>6384</v>
       </c>
-      <c r="H39">
+      <c r="H40">
         <v>22325153</v>
       </c>
-      <c r="I39" t="s">
-        <v>143</v>
-      </c>
-      <c r="K39">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.9974615565856896E-2</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>0.30635843794665146</v>
-      </c>
-      <c r="M39">
+      <c r="I40" t="s">
+        <v>143</v>
+      </c>
+      <c r="J40" t="s">
+        <v>169</v>
+      </c>
+      <c r="K40">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9940474455040684E-2</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>0.17409045304191195</v>
+      </c>
+      <c r="M40">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.19997985793384931</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>48</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>3616</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>591</v>
       </c>
-      <c r="H40">
+      <c r="H41">
         <v>6088</v>
       </c>
-      <c r="I40" t="s">
-        <v>144</v>
-      </c>
-      <c r="J40" t="s">
-        <v>165</v>
-      </c>
-      <c r="K40" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M40">
+      <c r="I41" t="s">
+        <v>144</v>
+      </c>
+      <c r="J41" t="s">
+        <v>166</v>
+      </c>
+      <c r="K41" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M41">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.8487788808529116E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>86</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>550</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>833</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>61</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>270</v>
       </c>
-      <c r="H41">
+      <c r="H42">
         <v>352</v>
       </c>
-      <c r="I41" t="s">
-        <v>144</v>
-      </c>
-      <c r="J41" s="7"/>
-      <c r="K41">
+      <c r="I42" t="s">
+        <v>144</v>
+      </c>
+      <c r="J42" s="7"/>
+      <c r="K42">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7610993657505285E-2</v>
       </c>
-      <c r="L41">
+      <c r="L42">
         <f t="shared" si="0"/>
         <v>2.3664772727272729</v>
       </c>
-      <c r="M41">
+      <c r="M42">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.1372191863995142E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>384</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <v>1677</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <v>5170</v>
       </c>
-      <c r="F42">
+      <c r="F43">
         <v>261</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <v>869</v>
       </c>
-      <c r="H42">
+      <c r="H43">
         <v>2429</v>
       </c>
-      <c r="I42" t="s">
-        <v>144</v>
-      </c>
-      <c r="K42">
+      <c r="I43" t="s">
+        <v>144</v>
+      </c>
+      <c r="K43">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>8.0283492347445837E-3</v>
       </c>
-      <c r="L42">
+      <c r="L43">
         <f t="shared" si="0"/>
         <v>2.1284479209551255</v>
       </c>
-      <c r="M42">
+      <c r="M43">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0709451564973171E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>2774</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>5660</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>16123</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>2532</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>5108</v>
       </c>
-      <c r="H43">
+      <c r="H44">
         <v>13355</v>
       </c>
-      <c r="I43" t="s">
-        <v>144</v>
-      </c>
-      <c r="K43">
+      <c r="I44" t="s">
+        <v>144</v>
+      </c>
+      <c r="K44">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.026887733395156E-3</v>
       </c>
-      <c r="L43">
+      <c r="L44">
         <f t="shared" si="0"/>
         <v>1.2072631973043804</v>
       </c>
-      <c r="M43">
+      <c r="M44">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0325932991151012E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>261</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>972</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>3003</v>
       </c>
-      <c r="F44">
+      <c r="F45">
         <v>154</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>609</v>
       </c>
-      <c r="H44">
+      <c r="H45">
         <v>1784</v>
       </c>
-      <c r="I44" t="s">
-        <v>144</v>
-      </c>
-      <c r="K44">
+      <c r="I45" t="s">
+        <v>144</v>
+      </c>
+      <c r="K45">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.1837188401683933E-2</v>
       </c>
-      <c r="L44">
+      <c r="L45">
         <f t="shared" si="0"/>
         <v>1.6832959641255605</v>
       </c>
-      <c r="M44">
+      <c r="M45">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.9022028874245624E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>17903</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>15826</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>292610</v>
       </c>
-      <c r="F45">
+      <c r="F46">
         <v>18215</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>15819</v>
       </c>
-      <c r="H45">
+      <c r="H46">
         <v>293199</v>
       </c>
-      <c r="I45" t="s">
-        <v>144</v>
-      </c>
-      <c r="K45">
+      <c r="I46" t="s">
+        <v>144</v>
+      </c>
+      <c r="K46">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0327428361490754E-3</v>
       </c>
-      <c r="L45">
+      <c r="L46">
         <f t="shared" si="0"/>
         <v>0.9979911254813284</v>
       </c>
-      <c r="M45">
+      <c r="M46">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0175465428920497E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>1271</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>1205</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <v>12543</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>1279</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>1205</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>12571</v>
       </c>
-      <c r="I46" t="s">
-        <v>144</v>
-      </c>
-      <c r="K46">
+      <c r="I47" t="s">
+        <v>144</v>
+      </c>
+      <c r="K47">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>8.1897156811214754E-3</v>
       </c>
-      <c r="L46">
+      <c r="L47">
         <f t="shared" si="0"/>
         <v>0.99777265134038662</v>
       </c>
-      <c r="M46">
+      <c r="M47">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>8.1566576585052515E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>398</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>1153</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <v>16215</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <v>404</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <v>1150</v>
       </c>
-      <c r="H47">
+      <c r="H48">
         <v>16240</v>
       </c>
-      <c r="I47" t="s">
-        <v>144</v>
-      </c>
-      <c r="K47">
+      <c r="I48" t="s">
+        <v>144</v>
+      </c>
+      <c r="K48">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>3.5334957528318091E-2</v>
       </c>
-      <c r="L47">
+      <c r="L48">
         <f t="shared" si="0"/>
         <v>0.99846059113300489</v>
       </c>
-      <c r="M47">
+      <c r="M48">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>3.4954799827808865E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>10792</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>1163</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <v>159229</v>
       </c>
-      <c r="F48">
+      <c r="F49">
         <v>10933</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>1163</v>
       </c>
-      <c r="H48">
+      <c r="H49">
         <v>158860</v>
       </c>
-      <c r="I48" t="s">
-        <v>144</v>
-      </c>
-      <c r="K48">
+      <c r="I49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K49">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.2686461803813788E-2</v>
       </c>
-      <c r="L48">
+      <c r="L49">
         <f t="shared" si="0"/>
         <v>1.0023227999496411</v>
       </c>
-      <c r="M48">
+      <c r="M49">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.2493827210983117E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49">
-        <v>24656</v>
-      </c>
-      <c r="G49">
-        <v>456</v>
-      </c>
-      <c r="H49">
-        <v>1530489</v>
-      </c>
-      <c r="I49" t="s">
-        <v>144</v>
-      </c>
-      <c r="J49" s="7"/>
-      <c r="K49" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M49">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.13612652199528671</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -2943,16 +2898,16 @@
         <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F50">
         <v>24656</v>
       </c>
       <c r="G50">
-        <v>1129</v>
+        <v>456</v>
       </c>
       <c r="H50">
-        <v>2220608</v>
+        <v>1530489</v>
       </c>
       <c r="I50" t="s">
         <v>144</v>
@@ -2968,390 +2923,397 @@
       </c>
       <c r="M50">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>7.9772892000121859E-2</v>
+        <v>0.13612652199528671</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51">
+        <v>24656</v>
+      </c>
+      <c r="G51">
+        <v>1129</v>
+      </c>
+      <c r="H51">
+        <v>2220608</v>
+      </c>
+      <c r="I51" t="s">
+        <v>144</v>
+      </c>
+      <c r="J51" s="7"/>
+      <c r="K51" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>7.9772892000121859E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>62</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>62</v>
       </c>
-      <c r="F51">
+      <c r="F52">
         <v>13514</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>44</v>
       </c>
-      <c r="H51">
+      <c r="H52">
         <v>81427</v>
       </c>
-      <c r="I51" t="s">
-        <v>144</v>
-      </c>
-      <c r="J51" t="s">
-        <v>166</v>
-      </c>
-      <c r="K51" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M51">
+      <c r="I52" t="s">
+        <v>144</v>
+      </c>
+      <c r="K52" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M52">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.13694047923365668</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>14066</v>
       </c>
-      <c r="D52">
+      <c r="D53">
         <v>15565</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <v>109669</v>
       </c>
-      <c r="F52">
+      <c r="F53">
         <v>14107</v>
       </c>
-      <c r="G52">
+      <c r="G53">
         <v>15522</v>
       </c>
-      <c r="H52">
+      <c r="H53">
         <v>109097</v>
       </c>
-      <c r="I52" t="s">
-        <v>144</v>
-      </c>
-      <c r="K52">
+      <c r="I53" t="s">
+        <v>144</v>
+      </c>
+      <c r="K53">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.0091512505704263E-4</v>
       </c>
-      <c r="L52">
+      <c r="L53">
         <f t="shared" si="0"/>
         <v>1.0052430405969</v>
       </c>
-      <c r="M52">
+      <c r="M53">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>4.9823067530873591E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>14083</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>19</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>42848</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>14120</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>19</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>42691</v>
       </c>
-      <c r="I53" t="s">
-        <v>144</v>
-      </c>
-      <c r="K53">
+      <c r="I54" t="s">
+        <v>144</v>
+      </c>
+      <c r="K54">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>0.16013334479420877</v>
       </c>
-      <c r="L53">
+      <c r="L54">
         <f t="shared" si="0"/>
         <v>1.0036775901243822</v>
       </c>
-      <c r="M53">
+      <c r="M54">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.15912852243924258</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B55" t="s">
         <v>67</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>12296</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>727</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>1787693</v>
       </c>
-      <c r="I54" t="s">
-        <v>143</v>
-      </c>
-      <c r="J54" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="K54" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M54">
+      <c r="I55" t="s">
+        <v>143</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="K55" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M55">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.19998373454782042</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C56" s="9">
         <v>4457</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>661</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>13374</v>
       </c>
-      <c r="F55">
+      <c r="F56">
         <v>4368</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>125</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <v>9452</v>
       </c>
-      <c r="I55" t="s">
-        <v>144</v>
-      </c>
-      <c r="K55">
+      <c r="I56" t="s">
+        <v>144</v>
+      </c>
+      <c r="K56">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.5395962155775288E-3</v>
       </c>
-      <c r="L55">
+      <c r="L56">
         <f t="shared" si="0"/>
         <v>1.4149386373254338</v>
       </c>
-      <c r="M55">
+      <c r="M56">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.731135531135531E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>69</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>69</v>
       </c>
-      <c r="F56">
+      <c r="F57">
         <v>18534</v>
       </c>
-      <c r="G56">
+      <c r="G57">
         <v>3508</v>
       </c>
-      <c r="H56">
+      <c r="H57">
         <v>404516</v>
       </c>
-      <c r="I56" t="s">
-        <v>144</v>
-      </c>
-      <c r="J56" s="9" t="s">
+      <c r="I57" t="s">
+        <v>144</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K57" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>6.2216698356707427E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58">
+        <v>3082</v>
+      </c>
+      <c r="D58">
+        <v>3152</v>
+      </c>
+      <c r="E58">
+        <v>25272</v>
+      </c>
+      <c r="F58">
+        <v>14481</v>
+      </c>
+      <c r="G58">
+        <v>11947</v>
+      </c>
+      <c r="H58">
+        <v>195513</v>
+      </c>
+      <c r="I58" t="s">
+        <v>144</v>
+      </c>
+      <c r="J58" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="K56" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M56">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>6.2216698356707427E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="K58">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>2.6014816669247013E-3</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>0.12925994690890119</v>
+      </c>
+      <c r="M58">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>1.1301035064941979E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57">
-        <v>3082</v>
-      </c>
-      <c r="D57">
-        <v>3152</v>
-      </c>
-      <c r="E57">
-        <v>25272</v>
-      </c>
-      <c r="F57">
-        <v>14481</v>
-      </c>
-      <c r="G57">
-        <v>11947</v>
-      </c>
-      <c r="H57">
-        <v>195513</v>
-      </c>
-      <c r="I57" t="s">
-        <v>144</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K57">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>2.6014816669247013E-3</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>0.12925994690890119</v>
-      </c>
-      <c r="M57">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>1.1301035064941979E-3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="B59" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59">
+        <v>3789</v>
+      </c>
+      <c r="D59">
+        <v>1249</v>
+      </c>
+      <c r="E59">
+        <v>20753</v>
+      </c>
+      <c r="F59">
+        <v>12400</v>
+      </c>
+      <c r="G59">
+        <v>962</v>
+      </c>
+      <c r="H59">
+        <v>43458</v>
+      </c>
+      <c r="I59" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K59">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.3852448018060798E-3</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="0"/>
+        <v>0.47754153435500946</v>
+      </c>
+      <c r="M59">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>3.6431158205351756E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58">
-        <v>3789</v>
-      </c>
-      <c r="D58">
-        <v>1249</v>
-      </c>
-      <c r="E58">
-        <v>20753</v>
-      </c>
-      <c r="F58">
-        <v>12400</v>
-      </c>
-      <c r="G58">
-        <v>962</v>
-      </c>
-      <c r="H58">
-        <v>43458</v>
-      </c>
-      <c r="I58" t="s">
-        <v>144</v>
-      </c>
-      <c r="J58" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K58">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.3852448018060798E-3</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>0.47754153435500946</v>
-      </c>
-      <c r="M58">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>3.6431158205351756E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>3794</v>
       </c>
-      <c r="D59">
+      <c r="D60">
         <v>2552</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <v>16903</v>
       </c>
-      <c r="F59">
+      <c r="F60">
         <v>11739</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <v>3618</v>
       </c>
-      <c r="H59">
+      <c r="H60">
         <v>48304</v>
       </c>
-      <c r="I59" t="s">
-        <v>144</v>
-      </c>
-      <c r="J59" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="K59">
+      <c r="I60" t="s">
+        <v>144</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K60">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7457650505748228E-3</v>
       </c>
-      <c r="L59">
+      <c r="L60">
         <f t="shared" si="0"/>
         <v>0.34992961245445514</v>
       </c>
-      <c r="M59">
+      <c r="M60">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.1373219749940796E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I60" t="s">
-        <v>143</v>
-      </c>
-      <c r="K60" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M60" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3359,16 +3321,7 @@
         <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F61">
-        <v>25577</v>
-      </c>
-      <c r="G61">
-        <v>8555</v>
-      </c>
-      <c r="H61">
-        <v>10940561</v>
+        <v>146</v>
       </c>
       <c r="I61" t="s">
         <v>143</v>
@@ -3381,9 +3334,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M61">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9999996572388065E-2</v>
+      <c r="M61" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3391,189 +3344,186 @@
         <v>74</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="F62">
         <v>25577</v>
       </c>
       <c r="G62">
+        <v>8555</v>
+      </c>
+      <c r="H62">
+        <v>10940561</v>
+      </c>
+      <c r="I62" t="s">
+        <v>143</v>
+      </c>
+      <c r="K62" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M62">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>4.9999996572388065E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63">
+        <v>25577</v>
+      </c>
+      <c r="G63">
         <v>53</v>
       </c>
-      <c r="H62">
+      <c r="H63">
         <v>64221</v>
       </c>
-      <c r="I62" t="s">
-        <v>143</v>
-      </c>
-      <c r="K62" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M62">
+      <c r="I63" t="s">
+        <v>143</v>
+      </c>
+      <c r="K63" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M63">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>4.7375258284086307E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>2143</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>8183</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <v>17688</v>
       </c>
-      <c r="F63">
+      <c r="F64">
         <v>1577</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>7087</v>
       </c>
-      <c r="H63">
+      <c r="H64">
         <v>13759</v>
       </c>
-      <c r="I63" t="s">
-        <v>144</v>
-      </c>
-      <c r="K63">
+      <c r="I64" t="s">
+        <v>144</v>
+      </c>
+      <c r="K64">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0086581624526999E-3</v>
       </c>
-      <c r="L63">
+      <c r="L64">
         <f t="shared" si="0"/>
         <v>1.2855585434988008</v>
       </c>
-      <c r="M63">
+      <c r="M64">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.2310983367422143E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C64">
-        <v>323</v>
-      </c>
-      <c r="D64">
-        <v>344</v>
-      </c>
-      <c r="E64">
-        <v>858</v>
-      </c>
-      <c r="F64">
+      <c r="C65">
+        <v>322</v>
+      </c>
+      <c r="D65">
+        <v>340</v>
+      </c>
+      <c r="E65">
+        <v>850</v>
+      </c>
+      <c r="F65">
         <v>224</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>196</v>
       </c>
-      <c r="H64">
+      <c r="H65">
         <v>427</v>
       </c>
-      <c r="I64" t="s">
-        <v>144</v>
-      </c>
-      <c r="K64">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>7.7219382244942038E-3</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
-        <v>2.0093676814988291</v>
-      </c>
-      <c r="M64">
+      <c r="I65" t="s">
+        <v>144</v>
+      </c>
+      <c r="K65">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>7.763975155279503E-3</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="0"/>
+        <v>1.9906323185011709</v>
+      </c>
+      <c r="M65">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>9.7257653061224494E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>17954</v>
       </c>
-      <c r="D65">
+      <c r="D66">
         <v>4101</v>
       </c>
-      <c r="E65">
+      <c r="E66">
         <v>107157</v>
       </c>
-      <c r="F65">
+      <c r="F66">
         <v>6990</v>
       </c>
-      <c r="G65">
+      <c r="G66">
         <v>1978</v>
       </c>
-      <c r="H65">
+      <c r="H66">
         <v>18773</v>
       </c>
-      <c r="I65" t="s">
-        <v>144</v>
-      </c>
-      <c r="K65">
+      <c r="I66" t="s">
+        <v>144</v>
+      </c>
+      <c r="K66">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.4553570577299918E-3</v>
       </c>
-      <c r="L65">
+      <c r="L66">
         <f t="shared" si="0"/>
         <v>5.7080381398817455</v>
       </c>
-      <c r="M65">
+      <c r="M66">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.3577825320297233E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>80</v>
-      </c>
-      <c r="B66" t="s">
-        <v>81</v>
-      </c>
-      <c r="F66">
-        <v>12091</v>
-      </c>
-      <c r="G66">
-        <v>225</v>
-      </c>
-      <c r="H66">
-        <v>60246</v>
-      </c>
-      <c r="I66" t="s">
-        <v>144</v>
-      </c>
-      <c r="J66" t="s">
-        <v>158</v>
-      </c>
-      <c r="K66" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M66">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>2.2145397403027046E-2</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3581,16 +3531,16 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F67">
-        <v>12652</v>
+        <v>12091</v>
       </c>
       <c r="G67">
-        <v>487</v>
+        <v>225</v>
       </c>
       <c r="H67">
-        <v>70482</v>
+        <v>60246</v>
       </c>
       <c r="I67" t="s">
         <v>144</v>
@@ -3603,624 +3553,620 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L67">
-        <f t="shared" ref="L67:L120" si="1">IF(COUNTA(E67),E67/H67,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M67">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>2.2145397403027046E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="F68">
+        <v>12652</v>
+      </c>
+      <c r="G68">
+        <v>487</v>
+      </c>
+      <c r="H68">
+        <v>70482</v>
+      </c>
+      <c r="I68" t="s">
+        <v>144</v>
+      </c>
+      <c r="J68" t="s">
+        <v>158</v>
+      </c>
+      <c r="K68" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L121" si="1">IF(COUNTA(E68),E68/H68,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.14390530654429E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>4251</v>
       </c>
-      <c r="D68">
+      <c r="D69">
         <v>9059</v>
       </c>
-      <c r="E68">
+      <c r="E69">
         <v>577116</v>
       </c>
-      <c r="F68">
+      <c r="F69">
         <v>3644</v>
       </c>
-      <c r="G68">
+      <c r="G69">
         <v>7841</v>
       </c>
-      <c r="H68">
+      <c r="H69">
         <v>415410</v>
       </c>
-      <c r="I68" t="s">
-        <v>144</v>
-      </c>
-      <c r="K68">
+      <c r="I69" t="s">
+        <v>144</v>
+      </c>
+      <c r="K69">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.4986207799680335E-2</v>
       </c>
-      <c r="L68">
+      <c r="L69">
         <f t="shared" si="1"/>
         <v>1.3892684335957246</v>
       </c>
-      <c r="M68">
+      <c r="M69">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.4538751875747831E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>1991</v>
       </c>
-      <c r="D69">
+      <c r="D70">
         <v>1991</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <v>9764</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <v>7669</v>
       </c>
-      <c r="G69">
+      <c r="G70">
         <v>7669</v>
       </c>
-      <c r="H69">
+      <c r="H70">
         <v>126176</v>
       </c>
-      <c r="I69" t="s">
-        <v>144</v>
-      </c>
-      <c r="J69" s="7" t="s">
+      <c r="I70" t="s">
+        <v>144</v>
+      </c>
+      <c r="J70" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="K69">
+      <c r="K70">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>2.4631181855264811E-3</v>
       </c>
-      <c r="L69" s="1">
+      <c r="L70" s="1">
         <f t="shared" si="1"/>
         <v>7.7383971595232054E-2</v>
       </c>
-      <c r="M69">
+      <c r="M70">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.1453555583889911E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>20471</v>
       </c>
-      <c r="D70">
+      <c r="D71">
         <v>3278</v>
       </c>
-      <c r="E70">
+      <c r="E71">
         <v>4245692</v>
       </c>
-      <c r="F70">
+      <c r="F71">
         <v>18535</v>
       </c>
-      <c r="G70">
+      <c r="G71">
         <v>2826</v>
       </c>
-      <c r="H70">
+      <c r="H71">
         <v>829693</v>
       </c>
-      <c r="I70" t="s">
-        <v>144</v>
-      </c>
-      <c r="K70">
+      <c r="I71" t="s">
+        <v>144</v>
+      </c>
+      <c r="K71">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>6.3270385115103078E-2</v>
       </c>
-      <c r="L70">
+      <c r="L71">
         <f t="shared" si="1"/>
         <v>5.1171843079307644</v>
       </c>
-      <c r="M70">
+      <c r="M71">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.5839908850549762E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>16712</v>
       </c>
-      <c r="D71">
+      <c r="D72">
         <v>5337</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <v>182402</v>
       </c>
-      <c r="F71">
+      <c r="F72">
         <v>13149</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>3679</v>
       </c>
-      <c r="H71">
+      <c r="H72">
         <v>52079</v>
       </c>
-      <c r="I71" t="s">
-        <v>144</v>
-      </c>
-      <c r="K71">
+      <c r="I72" t="s">
+        <v>144</v>
+      </c>
+      <c r="K72">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>2.0450501673110744E-3</v>
       </c>
-      <c r="L71">
+      <c r="L72">
         <f t="shared" si="1"/>
         <v>3.5024098004954012</v>
       </c>
-      <c r="M71">
+      <c r="M72">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0765646699212701E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>20540</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <v>6696</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <v>7870084</v>
       </c>
-      <c r="F72">
+      <c r="F73">
         <v>18565</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>4098</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <v>434311</v>
       </c>
-      <c r="I72" t="s">
-        <v>144</v>
-      </c>
-      <c r="K72">
+      <c r="I73" t="s">
+        <v>144</v>
+      </c>
+      <c r="K73">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.7222059355583242E-2</v>
       </c>
-      <c r="L72">
+      <c r="L73">
         <f t="shared" si="1"/>
         <v>18.120848884785328</v>
       </c>
-      <c r="M72">
+      <c r="M73">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>5.7086566305688388E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>9767</v>
       </c>
-      <c r="D73">
+      <c r="D74">
         <v>9619</v>
       </c>
-      <c r="E73">
+      <c r="E74">
         <v>160162</v>
       </c>
-      <c r="F73">
+      <c r="F74">
         <v>7758</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <v>8639</v>
       </c>
-      <c r="H73">
+      <c r="H74">
         <v>134408</v>
       </c>
-      <c r="I73" t="s">
-        <v>144</v>
-      </c>
-      <c r="K73">
+      <c r="I74" t="s">
+        <v>144</v>
+      </c>
+      <c r="K74">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7047801145843595E-3</v>
       </c>
-      <c r="L73">
+      <c r="L74">
         <f t="shared" si="1"/>
         <v>1.1916106184155706</v>
       </c>
-      <c r="M73">
+      <c r="M74">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.0054501428962306E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>21859</v>
       </c>
-      <c r="D74">
+      <c r="D75">
         <v>3737</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>421067</v>
       </c>
-      <c r="F74">
+      <c r="F75">
         <v>15575</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <v>3551</v>
       </c>
-      <c r="H74">
+      <c r="H75">
         <v>417884</v>
       </c>
-      <c r="I74" t="s">
-        <v>144</v>
-      </c>
-      <c r="K74">
+      <c r="I75" t="s">
+        <v>144</v>
+      </c>
+      <c r="K75">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.1546338115660223E-3</v>
       </c>
-      <c r="L74">
+      <c r="L75">
         <f t="shared" si="1"/>
         <v>1.0076169463296034</v>
       </c>
-      <c r="M74">
+      <c r="M75">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>7.5557401821565425E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>4067</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D76" s="5">
         <v>3823</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E76" s="5">
         <v>7641</v>
       </c>
-      <c r="K75">
+      <c r="K76">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.9144138839492127E-4</v>
       </c>
-      <c r="L75" t="e">
+      <c r="L76" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M75" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="M76" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>10957</v>
       </c>
-      <c r="D76">
+      <c r="D77">
         <v>23737</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E77" s="5">
         <v>146627</v>
       </c>
-      <c r="F76">
+      <c r="F77">
         <v>11164</v>
       </c>
-      <c r="G76">
+      <c r="G77">
         <v>51319</v>
       </c>
-      <c r="H76">
+      <c r="H77">
         <v>1257932</v>
       </c>
-      <c r="I76" t="s">
-        <v>144</v>
-      </c>
-      <c r="K76">
+      <c r="I77" t="s">
+        <v>144</v>
+      </c>
+      <c r="K77">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.6376285458378361E-4</v>
       </c>
-      <c r="L76" s="1">
+      <c r="L77" s="1">
         <f t="shared" si="1"/>
         <v>0.11656194452482328</v>
       </c>
-      <c r="M76">
+      <c r="M77">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.1956299798070017E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>16396</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>18180</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>1093028</v>
       </c>
-      <c r="F77">
+      <c r="F78">
         <v>16291</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>18511</v>
       </c>
-      <c r="H77">
+      <c r="H78">
         <v>1125042</v>
       </c>
-      <c r="I77" t="s">
-        <v>144</v>
-      </c>
-      <c r="K77">
+      <c r="I78" t="s">
+        <v>144</v>
+      </c>
+      <c r="K78">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>3.6669036505992633E-3</v>
       </c>
-      <c r="L77">
+      <c r="L78">
         <f t="shared" si="1"/>
         <v>0.97154417346196853</v>
       </c>
-      <c r="M77">
+      <c r="M78">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>3.7307067361755722E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>95</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>95</v>
       </c>
-      <c r="F78">
+      <c r="F79">
         <v>2716</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I79" t="s">
         <v>145</v>
       </c>
-      <c r="J78" t="s">
-        <v>157</v>
-      </c>
-      <c r="K78" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L78">
+      <c r="K79" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L79">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M78" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="M79" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>13894</v>
       </c>
-      <c r="D79">
+      <c r="D80">
         <v>3000</v>
       </c>
-      <c r="E79">
+      <c r="E80">
         <v>188518</v>
       </c>
-      <c r="I79" t="s">
-        <v>144</v>
-      </c>
-      <c r="K79">
+      <c r="I80" t="s">
+        <v>144</v>
+      </c>
+      <c r="K80">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.5227676215152824E-3</v>
       </c>
-      <c r="L79" t="e">
+      <c r="L80" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M79" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="M80" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>10601</v>
       </c>
-      <c r="D80">
+      <c r="D81">
         <v>2333</v>
       </c>
-      <c r="E80">
+      <c r="E81">
         <v>113787</v>
       </c>
-      <c r="F80">
+      <c r="F81">
         <v>10237</v>
       </c>
-      <c r="G80">
+      <c r="G81">
         <v>1887</v>
       </c>
-      <c r="H80">
+      <c r="H81">
         <v>105556</v>
       </c>
-      <c r="I80" t="s">
-        <v>144</v>
-      </c>
-      <c r="K80">
+      <c r="I81" t="s">
+        <v>144</v>
+      </c>
+      <c r="K81">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.6007758408868329E-3</v>
       </c>
-      <c r="L80">
+      <c r="L81">
         <f t="shared" si="1"/>
         <v>1.0779775664102467</v>
       </c>
-      <c r="M80">
+      <c r="M81">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>5.4643476372038856E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>97</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F81">
+      <c r="F82">
         <v>18375</v>
       </c>
-      <c r="G81">
+      <c r="G82">
         <v>57</v>
       </c>
-      <c r="H81">
+      <c r="H82">
         <v>209475</v>
       </c>
-      <c r="I81" t="s">
-        <v>143</v>
-      </c>
-      <c r="J81" t="s">
-        <v>167</v>
-      </c>
-      <c r="K81" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L81">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M81">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C82">
-        <v>18218</v>
-      </c>
-      <c r="D82">
-        <v>4543</v>
-      </c>
-      <c r="E82">
-        <v>15151173</v>
-      </c>
-      <c r="F82">
-        <v>18028</v>
-      </c>
-      <c r="G82">
-        <v>2318</v>
-      </c>
-      <c r="H82">
-        <v>5898446</v>
-      </c>
       <c r="I82" t="s">
-        <v>144</v>
-      </c>
-      <c r="K82">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>0.1830639472969372</v>
+        <v>143</v>
+      </c>
+      <c r="K82" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L82">
         <f t="shared" si="1"/>
-        <v>2.5686719858077876</v>
+        <v>1</v>
       </c>
       <c r="M82">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.14114861686729088</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>100</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>101</v>
+      <c r="A83" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C83">
+        <v>18218</v>
+      </c>
+      <c r="D83">
+        <v>4543</v>
+      </c>
+      <c r="E83">
+        <v>15151173</v>
       </c>
       <c r="F83">
-        <v>18423</v>
+        <v>18028</v>
       </c>
       <c r="G83">
-        <v>79</v>
+        <v>2318</v>
       </c>
       <c r="H83">
-        <v>72970</v>
+        <v>5898446</v>
       </c>
       <c r="I83" t="s">
-        <v>143</v>
-      </c>
-      <c r="J83" s="7"/>
-      <c r="K83" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>144</v>
+      </c>
+      <c r="K83">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.1830639472969372</v>
       </c>
       <c r="L83">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5686719858077876</v>
       </c>
       <c r="M83">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0136833635995734E-2</v>
+        <v>0.14114861686729088</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4228,16 +4174,16 @@
         <v>100</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F84">
-        <v>18549</v>
+        <v>18423</v>
       </c>
       <c r="G84">
-        <v>430</v>
+        <v>79</v>
       </c>
       <c r="H84">
-        <v>398197</v>
+        <v>72970</v>
       </c>
       <c r="I84" t="s">
         <v>143</v>
@@ -4253,7 +4199,7 @@
       </c>
       <c r="M84">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9923960045486063E-2</v>
+        <v>5.0136833635995734E-2</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4261,16 +4207,16 @@
         <v>100</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F85">
-        <v>18480</v>
+        <v>18549</v>
       </c>
       <c r="G85">
-        <v>530</v>
+        <v>430</v>
       </c>
       <c r="H85">
-        <v>489769</v>
+        <v>398197</v>
       </c>
       <c r="I85" t="s">
         <v>143</v>
@@ -4286,7 +4232,7 @@
       </c>
       <c r="M85">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0005002858776446E-2</v>
+        <v>4.9923960045486063E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4294,16 +4240,16 @@
         <v>100</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F86">
-        <v>18511</v>
+        <v>18480</v>
       </c>
       <c r="G86">
-        <v>1215</v>
+        <v>530</v>
       </c>
       <c r="H86">
-        <v>1124480</v>
+        <v>489769</v>
       </c>
       <c r="I86" t="s">
         <v>143</v>
@@ -4319,7 +4265,7 @@
       </c>
       <c r="M86">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9997187747114216E-2</v>
+        <v>5.0005002858776446E-2</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -4327,16 +4273,16 @@
         <v>100</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F87">
-        <v>18478</v>
+        <v>18511</v>
       </c>
       <c r="G87">
-        <v>309</v>
+        <v>1215</v>
       </c>
       <c r="H87">
-        <v>284538</v>
+        <v>1124480</v>
       </c>
       <c r="I87" t="s">
         <v>143</v>
@@ -4352,7 +4298,7 @@
       </c>
       <c r="M87">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9834124442921887E-2</v>
+        <v>4.9997187747114216E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4360,16 +4306,16 @@
         <v>100</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F88">
-        <v>18589</v>
+        <v>18478</v>
       </c>
       <c r="G88">
-        <v>45</v>
+        <v>309</v>
       </c>
       <c r="H88">
-        <v>41743</v>
+        <v>284538</v>
       </c>
       <c r="I88" t="s">
         <v>143</v>
@@ -4385,7 +4331,7 @@
       </c>
       <c r="M88">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9901674227888652E-2</v>
+        <v>4.9834124442921887E-2</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4393,16 +4339,16 @@
         <v>100</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F89">
-        <v>18340</v>
+        <v>18589</v>
       </c>
       <c r="G89">
-        <v>501</v>
+        <v>45</v>
       </c>
       <c r="H89">
-        <v>459393</v>
+        <v>41743</v>
       </c>
       <c r="I89" t="s">
         <v>143</v>
@@ -4418,7 +4364,7 @@
       </c>
       <c r="M89">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9997387993914025E-2</v>
+        <v>4.9901674227888652E-2</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4426,16 +4372,16 @@
         <v>100</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F90">
-        <v>18875</v>
+        <v>18340</v>
       </c>
       <c r="G90">
-        <v>198</v>
+        <v>501</v>
       </c>
       <c r="H90">
-        <v>186087</v>
+        <v>459393</v>
       </c>
       <c r="I90" t="s">
         <v>143</v>
@@ -4451,7 +4397,7 @@
       </c>
       <c r="M90">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9792494481236203E-2</v>
+        <v>4.9997387993914025E-2</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4459,16 +4405,16 @@
         <v>100</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F91">
-        <v>18471</v>
+        <v>18875</v>
       </c>
       <c r="G91">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="H91">
-        <v>159910</v>
+        <v>186087</v>
       </c>
       <c r="I91" t="s">
         <v>143</v>
@@ -4484,7 +4430,7 @@
       </c>
       <c r="M91">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.004251313494705E-2</v>
+        <v>4.9792494481236203E-2</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4492,16 +4438,16 @@
         <v>100</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F92">
-        <v>18648</v>
+        <v>18471</v>
       </c>
       <c r="G92">
-        <v>566</v>
+        <v>173</v>
       </c>
       <c r="H92">
-        <v>527943</v>
+        <v>159910</v>
       </c>
       <c r="I92" t="s">
         <v>143</v>
@@ -4517,7 +4463,7 @@
       </c>
       <c r="M92">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.001938460419026E-2</v>
+        <v>5.004251313494705E-2</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -4525,16 +4471,16 @@
         <v>100</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F93">
-        <v>18540</v>
+        <v>18648</v>
       </c>
       <c r="G93">
-        <v>91</v>
+        <v>566</v>
       </c>
       <c r="H93">
-        <v>84676</v>
+        <v>527943</v>
       </c>
       <c r="I93" t="s">
         <v>143</v>
@@ -4550,7 +4496,7 @@
       </c>
       <c r="M93">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0189077373543396E-2</v>
+        <v>5.001938460419026E-2</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -4558,16 +4504,16 @@
         <v>100</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F94">
-        <v>18665</v>
+        <v>18540</v>
       </c>
       <c r="G94">
-        <v>606</v>
+        <v>91</v>
       </c>
       <c r="H94">
-        <v>565628</v>
+        <v>84676</v>
       </c>
       <c r="I94" t="s">
         <v>143</v>
@@ -4583,7 +4529,7 @@
       </c>
       <c r="M94">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.000694015289555E-2</v>
+        <v>5.0189077373543396E-2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -4591,16 +4537,16 @@
         <v>100</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F95">
-        <v>18546</v>
+        <v>18665</v>
       </c>
       <c r="G95">
-        <v>323</v>
+        <v>606</v>
       </c>
       <c r="H95">
-        <v>299781</v>
+        <v>565628</v>
       </c>
       <c r="I95" t="s">
         <v>143</v>
@@ -4616,7 +4562,7 @@
       </c>
       <c r="M95">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0043920580372658E-2</v>
+        <v>5.000694015289555E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4624,16 +4570,16 @@
         <v>100</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F96">
-        <v>18339</v>
+        <v>18546</v>
       </c>
       <c r="G96">
-        <v>423</v>
+        <v>323</v>
       </c>
       <c r="H96">
-        <v>387737</v>
+        <v>299781</v>
       </c>
       <c r="I96" t="s">
         <v>143</v>
@@ -4649,7 +4595,7 @@
       </c>
       <c r="M96">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9982874410063063E-2</v>
+        <v>5.0043920580372658E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -4657,16 +4603,16 @@
         <v>100</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F97">
-        <v>18508</v>
+        <v>18339</v>
       </c>
       <c r="G97">
-        <v>577</v>
+        <v>423</v>
       </c>
       <c r="H97">
-        <v>533911</v>
+        <v>387737</v>
       </c>
       <c r="I97" t="s">
         <v>143</v>
@@ -4682,7 +4628,7 @@
       </c>
       <c r="M97">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9995804896210513E-2</v>
+        <v>4.9982874410063063E-2</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4690,16 +4636,16 @@
         <v>100</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F98">
-        <v>18608</v>
+        <v>18508</v>
       </c>
       <c r="G98">
-        <v>552</v>
+        <v>577</v>
       </c>
       <c r="H98">
-        <v>513287</v>
+        <v>533911</v>
       </c>
       <c r="I98" t="s">
         <v>143</v>
@@ -4715,7 +4661,7 @@
       </c>
       <c r="M98">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9971396905803329E-2</v>
+        <v>4.9995804896210513E-2</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -4723,16 +4669,16 @@
         <v>100</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F99">
-        <v>18967</v>
+        <v>18608</v>
       </c>
       <c r="G99">
-        <v>48</v>
+        <v>552</v>
       </c>
       <c r="H99">
-        <v>42973</v>
+        <v>513287</v>
       </c>
       <c r="I99" t="s">
         <v>143</v>
@@ -4748,7 +4694,7 @@
       </c>
       <c r="M99">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.7201499094919247E-2</v>
+        <v>4.9971396905803329E-2</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -4756,16 +4702,16 @@
         <v>100</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F100">
-        <v>18545</v>
+        <v>18967</v>
       </c>
       <c r="G100">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H100">
-        <v>81072</v>
+        <v>42973</v>
       </c>
       <c r="I100" t="s">
         <v>143</v>
@@ -4781,7 +4727,7 @@
       </c>
       <c r="M100">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0248696088731046E-2</v>
+        <v>4.7201499094919247E-2</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -4789,16 +4735,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F101">
-        <v>18621</v>
+        <v>18545</v>
       </c>
       <c r="G101">
-        <v>429</v>
+        <v>87</v>
       </c>
       <c r="H101">
-        <v>399505</v>
+        <v>81072</v>
       </c>
       <c r="I101" t="s">
         <v>143</v>
@@ -4814,7 +4760,7 @@
       </c>
       <c r="M101">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0010584085016178E-2</v>
+        <v>5.0248696088731046E-2</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -4822,16 +4768,16 @@
         <v>100</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F102">
-        <v>18493</v>
+        <v>18621</v>
       </c>
       <c r="G102">
-        <v>183</v>
+        <v>429</v>
       </c>
       <c r="H102">
-        <v>169642</v>
+        <v>399505</v>
       </c>
       <c r="I102" t="s">
         <v>143</v>
@@ -4847,7 +4793,7 @@
       </c>
       <c r="M102">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0127370598652153E-2</v>
+        <v>5.0010584085016178E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -4855,16 +4801,16 @@
         <v>100</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F103">
-        <v>18370</v>
+        <v>18493</v>
       </c>
       <c r="G103">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H103">
-        <v>172133</v>
+        <v>169642</v>
       </c>
       <c r="I103" t="s">
         <v>143</v>
@@ -4880,7 +4826,7 @@
       </c>
       <c r="M103">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0108727610408743E-2</v>
+        <v>5.0127370598652153E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -4888,16 +4834,16 @@
         <v>100</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F104">
-        <v>18528</v>
+        <v>18370</v>
       </c>
       <c r="G104">
-        <v>550</v>
+        <v>187</v>
       </c>
       <c r="H104">
-        <v>509464</v>
+        <v>172133</v>
       </c>
       <c r="I104" t="s">
         <v>143</v>
@@ -4913,7 +4859,7 @@
       </c>
       <c r="M104">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9994504631810328E-2</v>
+        <v>5.0108727610408743E-2</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -4921,16 +4867,16 @@
         <v>100</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F105">
-        <v>18335</v>
+        <v>18528</v>
       </c>
       <c r="G105">
-        <v>177</v>
+        <v>550</v>
       </c>
       <c r="H105">
-        <v>162528</v>
+        <v>509464</v>
       </c>
       <c r="I105" t="s">
         <v>143</v>
@@ -4946,7 +4892,7 @@
       </c>
       <c r="M105">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0081117433083897E-2</v>
+        <v>4.9994504631810328E-2</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -4954,16 +4900,16 @@
         <v>100</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F106">
-        <v>18584</v>
+        <v>18335</v>
       </c>
       <c r="G106">
-        <v>265</v>
+        <v>177</v>
       </c>
       <c r="H106">
-        <v>245886</v>
+        <v>162528</v>
       </c>
       <c r="I106" t="s">
         <v>143</v>
@@ -4979,7 +4925,7 @@
       </c>
       <c r="M106">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9928524435708541E-2</v>
+        <v>5.0081117433083897E-2</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4987,16 +4933,16 @@
         <v>100</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F107">
-        <v>18612</v>
+        <v>18584</v>
       </c>
       <c r="G107">
-        <v>473</v>
+        <v>265</v>
       </c>
       <c r="H107">
-        <v>439949</v>
+        <v>245886</v>
       </c>
       <c r="I107" t="s">
         <v>143</v>
@@ -5012,7 +4958,7 @@
       </c>
       <c r="M107">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9974464631924932E-2</v>
+        <v>4.9928524435708541E-2</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -5020,16 +4966,16 @@
         <v>100</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F108">
-        <v>18917</v>
+        <v>18612</v>
       </c>
       <c r="G108">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="H108">
-        <v>428467</v>
+        <v>439949</v>
       </c>
       <c r="I108" t="s">
         <v>143</v>
@@ -5045,7 +4991,7 @@
       </c>
       <c r="M108">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9999644082474377E-2</v>
+        <v>4.9974464631924932E-2</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -5053,16 +4999,16 @@
         <v>100</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F109">
-        <v>18742</v>
+        <v>18917</v>
       </c>
       <c r="G109">
-        <v>156</v>
+        <v>453</v>
       </c>
       <c r="H109">
-        <v>145048</v>
+        <v>428467</v>
       </c>
       <c r="I109" t="s">
         <v>143</v>
@@ -5078,7 +5024,7 @@
       </c>
       <c r="M109">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9610226859186417E-2</v>
+        <v>4.9999644082474377E-2</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -5086,16 +5032,16 @@
         <v>100</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F110">
-        <v>18514</v>
+        <v>18742</v>
       </c>
       <c r="G110">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="H110">
-        <v>112695</v>
+        <v>145048</v>
       </c>
       <c r="I110" t="s">
         <v>143</v>
@@ -5111,7 +5057,7 @@
       </c>
       <c r="M110">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9893567473086382E-2</v>
+        <v>4.9610226859186417E-2</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -5119,16 +5065,16 @@
         <v>100</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F111">
-        <v>18371</v>
+        <v>18514</v>
       </c>
       <c r="G111">
-        <v>572</v>
+        <v>122</v>
       </c>
       <c r="H111">
-        <v>525419</v>
+        <v>112695</v>
       </c>
       <c r="I111" t="s">
         <v>143</v>
@@ -5144,7 +5090,7 @@
       </c>
       <c r="M111">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0000799374812763E-2</v>
+        <v>4.9893567473086382E-2</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -5152,16 +5098,16 @@
         <v>100</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F112">
-        <v>18821</v>
+        <v>18371</v>
       </c>
       <c r="G112">
-        <v>57</v>
+        <v>572</v>
       </c>
       <c r="H112">
-        <v>56384</v>
+        <v>525419</v>
       </c>
       <c r="I112" t="s">
         <v>143</v>
@@ -5177,7 +5123,7 @@
       </c>
       <c r="M112">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.2557939666125091E-2</v>
+        <v>5.0000799374812763E-2</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -5185,16 +5131,16 @@
         <v>100</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F113">
-        <v>18689</v>
+        <v>18821</v>
       </c>
       <c r="G113">
-        <v>581</v>
+        <v>57</v>
       </c>
       <c r="H113">
-        <v>542785</v>
+        <v>56384</v>
       </c>
       <c r="I113" t="s">
         <v>143</v>
@@ -5210,7 +5156,7 @@
       </c>
       <c r="M113">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9987986158802442E-2</v>
+        <v>5.2557939666125091E-2</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -5218,16 +5164,16 @@
         <v>100</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F114">
-        <v>18136</v>
+        <v>18689</v>
       </c>
       <c r="G114">
-        <v>80</v>
+        <v>581</v>
       </c>
       <c r="H114">
-        <v>73121</v>
+        <v>542785</v>
       </c>
       <c r="I114" t="s">
         <v>143</v>
@@ -5243,252 +5189,285 @@
       </c>
       <c r="M114">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0397689677988529E-2</v>
+        <v>4.9987986158802442E-2</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C115">
-        <v>5213</v>
-      </c>
-      <c r="D115">
-        <v>24504</v>
-      </c>
-      <c r="E115">
-        <v>850425</v>
+      <c r="A115" t="s">
+        <v>100</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="F115">
-        <v>5309</v>
+        <v>18136</v>
       </c>
       <c r="G115">
-        <v>22128</v>
+        <v>80</v>
       </c>
       <c r="H115">
-        <v>848829</v>
+        <v>73121</v>
       </c>
       <c r="I115" t="s">
-        <v>144</v>
-      </c>
-      <c r="K115">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>6.657502067178171E-3</v>
+        <v>143</v>
+      </c>
+      <c r="J115" s="7"/>
+      <c r="K115" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L115">
         <f t="shared" si="1"/>
-        <v>1.0018802373622955</v>
+        <v>1</v>
       </c>
       <c r="M115">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>7.2254569962438443E-3</v>
+        <v>5.0397689677988529E-2</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>136</v>
+      <c r="A116" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C116">
-        <v>18025</v>
+        <v>5213</v>
       </c>
       <c r="D116">
-        <v>64</v>
+        <v>24504</v>
       </c>
       <c r="E116">
-        <v>58693</v>
+        <v>850425</v>
       </c>
       <c r="F116">
-        <v>17661</v>
+        <v>5309</v>
       </c>
       <c r="G116">
-        <v>56</v>
+        <v>22128</v>
       </c>
       <c r="H116">
-        <v>197848</v>
+        <v>848829</v>
       </c>
       <c r="I116" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K116">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>5.0878120665742023E-2</v>
+        <v>6.657502067178171E-3</v>
       </c>
       <c r="L116">
         <f t="shared" si="1"/>
-        <v>0.29665702963891472</v>
+        <v>1.0018802373622955</v>
       </c>
       <c r="M116">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.20004529754827019</v>
+        <v>7.2254569962438443E-3</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117" s="11" t="s">
+      <c r="A117" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C117">
-        <v>9702</v>
+        <v>18025</v>
       </c>
       <c r="D117">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="E117">
-        <v>118293</v>
+        <v>58693</v>
       </c>
       <c r="F117">
-        <v>9490</v>
+        <v>17661</v>
       </c>
       <c r="G117">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="H117">
-        <v>117708</v>
+        <v>197848</v>
       </c>
       <c r="I117" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K117">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>8.9651769798828621E-2</v>
+        <v>5.0878120665742023E-2</v>
       </c>
       <c r="L117">
         <f t="shared" si="1"/>
-        <v>1.0049699255785502</v>
+        <v>0.29665702963891472</v>
       </c>
       <c r="M117">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.11484603676384499</v>
+        <v>0.20004529754827019</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
+      <c r="A118" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C118">
-        <v>18362</v>
+        <v>9702</v>
       </c>
       <c r="D118">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="E118">
-        <v>56832</v>
+        <v>118293</v>
       </c>
       <c r="F118">
-        <v>18200</v>
+        <v>9490</v>
       </c>
       <c r="G118">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="H118">
-        <v>134717</v>
+        <v>117708</v>
       </c>
       <c r="I118" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K118">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.9920769049685364E-2</v>
+        <v>8.9651769798828621E-2</v>
       </c>
       <c r="L118">
         <f t="shared" si="1"/>
-        <v>0.42186212578961824</v>
+        <v>1.0049699255785502</v>
       </c>
       <c r="M118">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.20005494505494506</v>
+        <v>0.11484603676384499</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>139</v>
-      </c>
-      <c r="B119" t="s">
-        <v>140</v>
+      <c r="A119" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C119">
+        <v>18362</v>
+      </c>
+      <c r="D119">
+        <v>62</v>
+      </c>
+      <c r="E119">
+        <v>56832</v>
       </c>
       <c r="F119">
-        <v>1212</v>
+        <v>18200</v>
       </c>
       <c r="G119">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H119">
-        <v>2338</v>
+        <v>134717</v>
       </c>
       <c r="I119" t="s">
-        <v>149</v>
-      </c>
-      <c r="J119" t="s">
-        <v>157</v>
-      </c>
-      <c r="K119" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>143</v>
+      </c>
+      <c r="K119">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9920769049685364E-2</v>
       </c>
       <c r="L119">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.42186212578961824</v>
       </c>
       <c r="M119">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>9.6452145214521445E-2</v>
+        <v>0.20005494505494506</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C120">
-        <v>7183</v>
-      </c>
-      <c r="D120">
-        <v>621</v>
-      </c>
-      <c r="E120">
-        <v>26332</v>
+      <c r="A120" t="s">
+        <v>139</v>
+      </c>
+      <c r="B120" t="s">
+        <v>140</v>
       </c>
       <c r="F120">
-        <v>5388</v>
+        <v>1212</v>
       </c>
       <c r="G120">
-        <v>372</v>
+        <v>20</v>
       </c>
       <c r="H120">
-        <v>15503</v>
+        <v>2338</v>
       </c>
       <c r="I120" t="s">
-        <v>144</v>
-      </c>
-      <c r="K120">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>5.9031848099029673E-3</v>
+        <v>149</v>
+      </c>
+      <c r="J120" t="s">
+        <v>157</v>
+      </c>
+      <c r="K120" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L120">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M120">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>9.6452145214521445E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C121">
+        <v>7183</v>
+      </c>
+      <c r="D121">
+        <v>621</v>
+      </c>
+      <c r="E121">
+        <v>26332</v>
+      </c>
+      <c r="F121">
+        <v>5388</v>
+      </c>
+      <c r="G121">
+        <v>372</v>
+      </c>
+      <c r="H121">
+        <v>15503</v>
+      </c>
+      <c r="I121" t="s">
+        <v>144</v>
+      </c>
+      <c r="K121">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.9031848099029673E-3</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="1"/>
         <v>1.6985099658130685</v>
       </c>
-      <c r="M120">
+      <c r="M121">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>7.7347311029687636E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="L2:L120">
+  <conditionalFormatting sqref="L2:L121">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1.05</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated ABA-CCLE with examples, sections
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5724E29-6C4F-4EEF-AD1D-A6796ADFD79C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059E7BDF-6E1E-474F-BC3F-91C188D17B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="172">
   <si>
     <t>Resource</t>
   </si>
@@ -546,13 +546,19 @@
   </si>
   <si>
     <t>Removed sparse attributes</t>
+  </si>
+  <si>
+    <t>CNV</t>
+  </si>
+  <si>
+    <t>Mutations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,13 +594,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,7 +609,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,11 +633,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -653,30 +647,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
-    <cellStyle name="Accent3" xfId="4" builtinId="37"/>
+  <cellStyles count="5">
+    <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -717,10 +708,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE186E64-132B-4E6F-BBD5-769A36DC41A2}" name="Table1" displayName="Table1" ref="A1:J121" totalsRowShown="0">
-  <autoFilter ref="A1:J121" xr:uid="{5D1A7ADB-D789-4B9C-BF75-B396CFD6A519}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J121">
-    <sortCondition ref="A1:A121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE186E64-132B-4E6F-BBD5-769A36DC41A2}" name="Table1" displayName="Table1" ref="A1:J122" totalsRowShown="0">
+  <autoFilter ref="A1:J122" xr:uid="{5D1A7ADB-D789-4B9C-BF75-B396CFD6A519}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J122">
+    <sortCondition ref="A1:A122"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{AFD3E64B-E874-4397-A348-505BB47ED81A}" name="Resource"/>
@@ -1035,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1080,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1101,7 +1092,7 @@
       <c r="D2">
         <v>216</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>131670</v>
       </c>
       <c r="F2">
@@ -1116,7 +1107,7 @@
       <c r="I2" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>164</v>
       </c>
       <c r="K2">
@@ -1133,7 +1124,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1156,7 +1147,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L67" si="0">IF(COUNTA(E3),E3/H3,1)</f>
+        <f t="shared" ref="L3:L68" si="0">IF(COUNTA(E3),E3/H3,1)</f>
         <v>1</v>
       </c>
       <c r="M3">
@@ -1165,7 +1156,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1197,10 +1188,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C5">
@@ -1241,10 +1232,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C6">
@@ -1285,7 +1276,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1326,7 +1317,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1367,7 +1358,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1399,7 +1390,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1431,7 +1422,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1463,7 +1454,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1495,7 +1486,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1530,7 +1521,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1722,7 +1713,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1763,7 +1754,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1804,7 +1795,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1845,7 +1836,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1886,7 +1877,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1927,7 +1918,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1971,7 +1962,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2012,7 +2003,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2053,7 +2044,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2094,7 +2085,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2135,7 +2126,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2202,7 +2193,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2243,10 +2234,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C33">
@@ -2270,7 +2261,7 @@
       <c r="I33" t="s">
         <v>143</v>
       </c>
-      <c r="J33" s="7"/>
+      <c r="J33" s="6"/>
       <c r="K33">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.0001010508526025E-2</v>
@@ -2317,7 +2308,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2344,7 +2335,7 @@
       <c r="I35" t="s">
         <v>144</v>
       </c>
-      <c r="J35" s="7"/>
+      <c r="J35" s="6"/>
       <c r="K35">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.2471604208449741E-3</v>
@@ -2359,7 +2350,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B36" t="s">
@@ -2394,7 +2385,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2435,175 +2426,143 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>168</v>
+      <c r="B38" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="C38" s="5"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>17905</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>11746</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>214780</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>15676</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>10366</v>
       </c>
-      <c r="H39">
+      <c r="H40">
         <v>160332</v>
       </c>
-      <c r="I39" t="s">
-        <v>144</v>
-      </c>
-      <c r="K39">
+      <c r="I40" t="s">
+        <v>144</v>
+      </c>
+      <c r="K40">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0212439957695259E-3</v>
       </c>
-      <c r="L39">
+      <c r="L40">
         <f t="shared" si="0"/>
         <v>1.3395953396701843</v>
       </c>
-      <c r="M39">
+      <c r="M40">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>9.8667415117542536E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>24343</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <v>3197</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>3886596</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>17487</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>6384</v>
       </c>
-      <c r="H40">
+      <c r="H41">
         <v>22325153</v>
       </c>
-      <c r="I40" t="s">
-        <v>143</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="I41" t="s">
+        <v>143</v>
+      </c>
+      <c r="J41" t="s">
         <v>169</v>
       </c>
-      <c r="K40">
+      <c r="K41">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.9940474455040684E-2</v>
       </c>
-      <c r="L40">
+      <c r="L41">
         <f t="shared" si="0"/>
         <v>0.17409045304191195</v>
       </c>
-      <c r="M40">
+      <c r="M41">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.19997985793384931</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>48</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>3616</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>591</v>
       </c>
-      <c r="H41">
+      <c r="H42">
         <v>6088</v>
       </c>
-      <c r="I41" t="s">
-        <v>144</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="I42" t="s">
+        <v>144</v>
+      </c>
+      <c r="J42" t="s">
         <v>166</v>
       </c>
-      <c r="K41" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M41">
+      <c r="K42" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M42">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.8487788808529116E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42">
-        <v>86</v>
-      </c>
-      <c r="D42">
-        <v>550</v>
-      </c>
-      <c r="E42">
-        <v>833</v>
-      </c>
-      <c r="F42">
-        <v>61</v>
-      </c>
-      <c r="G42">
-        <v>270</v>
-      </c>
-      <c r="H42">
-        <v>352</v>
-      </c>
-      <c r="I42" t="s">
-        <v>144</v>
-      </c>
-      <c r="J42" s="7"/>
-      <c r="K42">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>1.7610993657505285E-2</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
-        <v>2.3664772727272729</v>
-      </c>
-      <c r="M42">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>2.1372191863995142E-2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2611,40 +2570,41 @@
         <v>49</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43">
-        <v>384</v>
+        <v>86</v>
       </c>
       <c r="D43">
-        <v>1677</v>
+        <v>550</v>
       </c>
       <c r="E43">
-        <v>5170</v>
+        <v>833</v>
       </c>
       <c r="F43">
-        <v>261</v>
+        <v>61</v>
       </c>
       <c r="G43">
-        <v>869</v>
+        <v>270</v>
       </c>
       <c r="H43">
-        <v>2429</v>
+        <v>352</v>
       </c>
       <c r="I43" t="s">
         <v>144</v>
       </c>
+      <c r="J43" s="6"/>
       <c r="K43">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>8.0283492347445837E-3</v>
+        <v>1.7610993657505285E-2</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>2.1284479209551255</v>
+        <v>2.3664772727272729</v>
       </c>
       <c r="M43">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>1.0709451564973171E-2</v>
+        <v>2.1372191863995142E-2</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -2652,40 +2612,40 @@
         <v>49</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44">
-        <v>2774</v>
+        <v>384</v>
       </c>
       <c r="D44">
-        <v>5660</v>
+        <v>1677</v>
       </c>
       <c r="E44">
-        <v>16123</v>
+        <v>5170</v>
       </c>
       <c r="F44">
-        <v>2532</v>
+        <v>261</v>
       </c>
       <c r="G44">
-        <v>5108</v>
+        <v>869</v>
       </c>
       <c r="H44">
-        <v>13355</v>
+        <v>2429</v>
       </c>
       <c r="I44" t="s">
         <v>144</v>
       </c>
       <c r="K44">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>1.026887733395156E-3</v>
+        <v>8.0283492347445837E-3</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>1.2072631973043804</v>
+        <v>2.1284479209551255</v>
       </c>
       <c r="M44">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>1.0325932991151012E-3</v>
+        <v>1.0709451564973171E-2</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2693,237 +2653,245 @@
         <v>49</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45">
+        <v>2774</v>
+      </c>
+      <c r="D45">
+        <v>5660</v>
+      </c>
+      <c r="E45">
+        <v>16123</v>
+      </c>
+      <c r="F45">
+        <v>2532</v>
+      </c>
+      <c r="G45">
+        <v>5108</v>
+      </c>
+      <c r="H45">
+        <v>13355</v>
+      </c>
+      <c r="I45" t="s">
+        <v>144</v>
+      </c>
+      <c r="K45">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>1.026887733395156E-3</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>1.2072631973043804</v>
+      </c>
+      <c r="M45">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>1.0325932991151012E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>261</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <v>972</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <v>3003</v>
       </c>
-      <c r="F45">
+      <c r="F46">
         <v>154</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>609</v>
       </c>
-      <c r="H45">
+      <c r="H46">
         <v>1784</v>
       </c>
-      <c r="I45" t="s">
-        <v>144</v>
-      </c>
-      <c r="K45">
+      <c r="I46" t="s">
+        <v>144</v>
+      </c>
+      <c r="K46">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.1837188401683933E-2</v>
       </c>
-      <c r="L45">
+      <c r="L46">
         <f t="shared" si="0"/>
         <v>1.6832959641255605</v>
       </c>
-      <c r="M45">
+      <c r="M46">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.9022028874245624E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>17903</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>15826</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <v>292610</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>18215</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>15819</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>293199</v>
       </c>
-      <c r="I46" t="s">
-        <v>144</v>
-      </c>
-      <c r="K46">
+      <c r="I47" t="s">
+        <v>144</v>
+      </c>
+      <c r="K47">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0327428361490754E-3</v>
       </c>
-      <c r="L46">
+      <c r="L47">
         <f t="shared" si="0"/>
         <v>0.9979911254813284</v>
       </c>
-      <c r="M46">
+      <c r="M47">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0175465428920497E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>1271</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <v>1205</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <v>12543</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <v>1279</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <v>1205</v>
       </c>
-      <c r="H47">
+      <c r="H48">
         <v>12571</v>
       </c>
-      <c r="I47" t="s">
-        <v>144</v>
-      </c>
-      <c r="K47">
+      <c r="I48" t="s">
+        <v>144</v>
+      </c>
+      <c r="K48">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>8.1897156811214754E-3</v>
       </c>
-      <c r="L47">
+      <c r="L48">
         <f t="shared" si="0"/>
         <v>0.99777265134038662</v>
       </c>
-      <c r="M47">
+      <c r="M48">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>8.1566576585052515E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>398</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <v>1153</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <v>16215</v>
       </c>
-      <c r="F48">
+      <c r="F49">
         <v>404</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>1150</v>
       </c>
-      <c r="H48">
+      <c r="H49">
         <v>16240</v>
       </c>
-      <c r="I48" t="s">
-        <v>144</v>
-      </c>
-      <c r="K48">
+      <c r="I49" t="s">
+        <v>144</v>
+      </c>
+      <c r="K49">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>3.5334957528318091E-2</v>
       </c>
-      <c r="L48">
+      <c r="L49">
         <f t="shared" si="0"/>
         <v>0.99846059113300489</v>
       </c>
-      <c r="M48">
+      <c r="M49">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>3.4954799827808865E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>10792</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>1163</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>159229</v>
       </c>
-      <c r="F49">
+      <c r="F50">
         <v>10933</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>1163</v>
       </c>
-      <c r="H49">
+      <c r="H50">
         <v>158860</v>
       </c>
-      <c r="I49" t="s">
-        <v>144</v>
-      </c>
-      <c r="K49">
+      <c r="I50" t="s">
+        <v>144</v>
+      </c>
+      <c r="K50">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.2686461803813788E-2</v>
       </c>
-      <c r="L49">
+      <c r="L50">
         <f t="shared" si="0"/>
         <v>1.0023227999496411</v>
       </c>
-      <c r="M49">
+      <c r="M50">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.2493827210983117E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>59</v>
-      </c>
-      <c r="B50" t="s">
-        <v>60</v>
-      </c>
-      <c r="F50">
-        <v>24656</v>
-      </c>
-      <c r="G50">
-        <v>456</v>
-      </c>
-      <c r="H50">
-        <v>1530489</v>
-      </c>
-      <c r="I50" t="s">
-        <v>144</v>
-      </c>
-      <c r="J50" s="7"/>
-      <c r="K50" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M50">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.13612652199528671</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2931,21 +2899,21 @@
         <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F51">
         <v>24656</v>
       </c>
       <c r="G51">
-        <v>1129</v>
+        <v>456</v>
       </c>
       <c r="H51">
-        <v>2220608</v>
+        <v>1530489</v>
       </c>
       <c r="I51" t="s">
         <v>144</v>
       </c>
-      <c r="J51" s="7"/>
+      <c r="J51" s="6"/>
       <c r="K51" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -2956,609 +2924,607 @@
       </c>
       <c r="M51">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>7.9772892000121859E-2</v>
+        <v>0.13612652199528671</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="F52">
+        <v>24656</v>
+      </c>
+      <c r="G52">
+        <v>1129</v>
+      </c>
+      <c r="H52">
+        <v>2220608</v>
+      </c>
+      <c r="I52" t="s">
+        <v>144</v>
+      </c>
+      <c r="J52" s="6"/>
+      <c r="K52" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>7.9772892000121859E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>62</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>62</v>
       </c>
-      <c r="F52">
+      <c r="F53">
         <v>13514</v>
       </c>
-      <c r="G52">
+      <c r="G53">
         <v>44</v>
       </c>
-      <c r="H52">
+      <c r="H53">
         <v>81427</v>
       </c>
-      <c r="I52" t="s">
-        <v>144</v>
-      </c>
-      <c r="K52" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M52">
+      <c r="I53" t="s">
+        <v>144</v>
+      </c>
+      <c r="K53" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M53">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.13694047923365668</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>14066</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>15565</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>109669</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>14107</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>15522</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>109097</v>
       </c>
-      <c r="I53" t="s">
-        <v>144</v>
-      </c>
-      <c r="K53">
+      <c r="I54" t="s">
+        <v>144</v>
+      </c>
+      <c r="K54">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.0091512505704263E-4</v>
       </c>
-      <c r="L53">
+      <c r="L54">
         <f t="shared" si="0"/>
         <v>1.0052430405969</v>
       </c>
-      <c r="M53">
+      <c r="M54">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>4.9823067530873591E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>14083</v>
       </c>
-      <c r="D54">
+      <c r="D55">
         <v>19</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>42848</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>14120</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>19</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>42691</v>
       </c>
-      <c r="I54" t="s">
-        <v>144</v>
-      </c>
-      <c r="K54">
+      <c r="I55" t="s">
+        <v>144</v>
+      </c>
+      <c r="K55">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>0.16013334479420877</v>
       </c>
-      <c r="L54">
+      <c r="L55">
         <f t="shared" si="0"/>
         <v>1.0036775901243822</v>
       </c>
-      <c r="M54">
+      <c r="M55">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.15912852243924258</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>66</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>67</v>
       </c>
-      <c r="F55">
+      <c r="F56">
         <v>12296</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>727</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <v>1787693</v>
       </c>
-      <c r="I55" t="s">
-        <v>143</v>
-      </c>
-      <c r="J55" s="9" t="s">
+      <c r="I56" t="s">
+        <v>143</v>
+      </c>
+      <c r="J56" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K55" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M55">
+      <c r="K56" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M56">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>0.19998373454782042</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C57" s="8">
         <v>4457</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>661</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>13374</v>
       </c>
-      <c r="F56">
+      <c r="F57">
         <v>4368</v>
       </c>
-      <c r="G56">
+      <c r="G57">
         <v>125</v>
       </c>
-      <c r="H56">
+      <c r="H57">
         <v>9452</v>
       </c>
-      <c r="I56" t="s">
-        <v>144</v>
-      </c>
-      <c r="K56">
+      <c r="I57" t="s">
+        <v>144</v>
+      </c>
+      <c r="K57">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.5395962155775288E-3</v>
       </c>
-      <c r="L56">
+      <c r="L57">
         <f t="shared" si="0"/>
         <v>1.4149386373254338</v>
       </c>
-      <c r="M56">
+      <c r="M57">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.731135531135531E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>69</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>69</v>
       </c>
-      <c r="F57">
+      <c r="F58">
         <v>18534</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>3508</v>
       </c>
-      <c r="H57">
+      <c r="H58">
         <v>404516</v>
       </c>
-      <c r="I57" t="s">
-        <v>144</v>
-      </c>
-      <c r="J57" s="9" t="s">
+      <c r="I58" t="s">
+        <v>144</v>
+      </c>
+      <c r="J58" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="K57" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M57">
+      <c r="K58" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M58">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>6.2216698356707427E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>3082</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <v>3152</v>
       </c>
-      <c r="E58">
+      <c r="E59">
         <v>25272</v>
       </c>
-      <c r="F58">
+      <c r="F59">
         <v>14481</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <v>11947</v>
       </c>
-      <c r="H58">
+      <c r="H59">
         <v>195513</v>
       </c>
-      <c r="I58" t="s">
-        <v>144</v>
-      </c>
-      <c r="J58" s="9" t="s">
+      <c r="I59" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K58">
+      <c r="K59">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>2.6014816669247013E-3</v>
       </c>
-      <c r="L58">
+      <c r="L59">
         <f t="shared" si="0"/>
         <v>0.12925994690890119</v>
       </c>
-      <c r="M58">
+      <c r="M59">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.1301035064941979E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>3789</v>
       </c>
-      <c r="D59">
+      <c r="D60">
         <v>1249</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <v>20753</v>
       </c>
-      <c r="F59">
+      <c r="F60">
         <v>12400</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <v>962</v>
       </c>
-      <c r="H59">
+      <c r="H60">
         <v>43458</v>
       </c>
-      <c r="I59" t="s">
-        <v>144</v>
-      </c>
-      <c r="J59" s="9" t="s">
+      <c r="I60" t="s">
+        <v>144</v>
+      </c>
+      <c r="J60" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K59">
+      <c r="K60">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.3852448018060798E-3</v>
       </c>
-      <c r="L59">
+      <c r="L60">
         <f t="shared" si="0"/>
         <v>0.47754153435500946</v>
       </c>
-      <c r="M59">
+      <c r="M60">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>3.6431158205351756E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>3794</v>
       </c>
-      <c r="D60">
+      <c r="D61">
         <v>2552</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <v>16903</v>
       </c>
-      <c r="F60">
+      <c r="F61">
         <v>11739</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <v>3618</v>
       </c>
-      <c r="H60">
+      <c r="H61">
         <v>48304</v>
       </c>
-      <c r="I60" t="s">
-        <v>144</v>
-      </c>
-      <c r="J60" s="9" t="s">
+      <c r="I61" t="s">
+        <v>144</v>
+      </c>
+      <c r="J61" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="K60">
+      <c r="K61">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7457650505748228E-3</v>
       </c>
-      <c r="L60">
+      <c r="L61">
         <f t="shared" si="0"/>
         <v>0.34992961245445514</v>
       </c>
-      <c r="M60">
+      <c r="M61">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.1373219749940796E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I61" t="s">
-        <v>143</v>
-      </c>
-      <c r="K61" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M61" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="I62" t="s">
+        <v>143</v>
+      </c>
+      <c r="K62" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M62" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F62">
-        <v>25577</v>
-      </c>
-      <c r="G62">
-        <v>8555</v>
-      </c>
-      <c r="H62">
-        <v>10940561</v>
-      </c>
-      <c r="I62" t="s">
-        <v>143</v>
-      </c>
-      <c r="K62" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M62">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9999996572388065E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>74</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F63">
         <v>25577</v>
       </c>
       <c r="G63">
+        <v>8555</v>
+      </c>
+      <c r="H63">
+        <v>10940561</v>
+      </c>
+      <c r="I63" t="s">
+        <v>143</v>
+      </c>
+      <c r="K63" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M63">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>4.9999996572388065E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64">
+        <v>25577</v>
+      </c>
+      <c r="G64">
         <v>53</v>
       </c>
-      <c r="H63">
+      <c r="H64">
         <v>64221</v>
       </c>
-      <c r="I63" t="s">
-        <v>143</v>
-      </c>
-      <c r="K63" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M63">
+      <c r="I64" t="s">
+        <v>143</v>
+      </c>
+      <c r="K64" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M64">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>4.7375258284086307E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>2143</v>
       </c>
-      <c r="D64">
+      <c r="D65">
         <v>8183</v>
       </c>
-      <c r="E64">
+      <c r="E65">
         <v>17688</v>
       </c>
-      <c r="F64">
+      <c r="F65">
         <v>1577</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>7087</v>
       </c>
-      <c r="H64">
+      <c r="H65">
         <v>13759</v>
       </c>
-      <c r="I64" t="s">
-        <v>144</v>
-      </c>
-      <c r="K64">
+      <c r="I65" t="s">
+        <v>144</v>
+      </c>
+      <c r="K65">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.0086581624526999E-3</v>
       </c>
-      <c r="L64">
+      <c r="L65">
         <f t="shared" si="0"/>
         <v>1.2855585434988008</v>
       </c>
-      <c r="M64">
+      <c r="M65">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.2310983367422143E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>322</v>
       </c>
-      <c r="D65">
+      <c r="D66">
         <v>340</v>
       </c>
-      <c r="E65">
+      <c r="E66">
         <v>850</v>
       </c>
-      <c r="F65">
+      <c r="F66">
         <v>224</v>
       </c>
-      <c r="G65">
+      <c r="G66">
         <v>196</v>
       </c>
-      <c r="H65">
+      <c r="H66">
         <v>427</v>
       </c>
-      <c r="I65" t="s">
-        <v>144</v>
-      </c>
-      <c r="K65">
+      <c r="I66" t="s">
+        <v>144</v>
+      </c>
+      <c r="K66">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>7.763975155279503E-3</v>
       </c>
-      <c r="L65">
+      <c r="L66">
         <f t="shared" si="0"/>
         <v>1.9906323185011709</v>
       </c>
-      <c r="M65">
+      <c r="M66">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>9.7257653061224494E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>17954</v>
       </c>
-      <c r="D66">
+      <c r="D67">
         <v>4101</v>
       </c>
-      <c r="E66">
+      <c r="E67">
         <v>107157</v>
       </c>
-      <c r="F66">
+      <c r="F67">
         <v>6990</v>
       </c>
-      <c r="G66">
+      <c r="G67">
         <v>1978</v>
       </c>
-      <c r="H66">
+      <c r="H67">
         <v>18773</v>
       </c>
-      <c r="I66" t="s">
-        <v>144</v>
-      </c>
-      <c r="K66">
+      <c r="I67" t="s">
+        <v>144</v>
+      </c>
+      <c r="K67">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.4553570577299918E-3</v>
       </c>
-      <c r="L66">
+      <c r="L67">
         <f t="shared" si="0"/>
         <v>5.7080381398817455</v>
       </c>
-      <c r="M66">
+      <c r="M67">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.3577825320297233E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>80</v>
-      </c>
-      <c r="B67" t="s">
-        <v>81</v>
-      </c>
-      <c r="F67">
-        <v>12091</v>
-      </c>
-      <c r="G67">
-        <v>225</v>
-      </c>
-      <c r="H67">
-        <v>60246</v>
-      </c>
-      <c r="I67" t="s">
-        <v>144</v>
-      </c>
-      <c r="J67" t="s">
-        <v>158</v>
-      </c>
-      <c r="K67" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L67">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M67">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>2.2145397403027046E-2</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3566,16 +3532,16 @@
         <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F68">
-        <v>12652</v>
+        <v>12091</v>
       </c>
       <c r="G68">
-        <v>487</v>
+        <v>225</v>
       </c>
       <c r="H68">
-        <v>70482</v>
+        <v>60246</v>
       </c>
       <c r="I68" t="s">
         <v>144</v>
@@ -3588,640 +3554,651 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L68">
-        <f t="shared" ref="L68:L121" si="1">IF(COUNTA(E68),E68/H68,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M68">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>2.2145397403027046E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="F69">
+        <v>12652</v>
+      </c>
+      <c r="G69">
+        <v>487</v>
+      </c>
+      <c r="H69">
+        <v>70482</v>
+      </c>
+      <c r="I69" t="s">
+        <v>144</v>
+      </c>
+      <c r="J69" t="s">
+        <v>158</v>
+      </c>
+      <c r="K69" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L69">
+        <f t="shared" ref="L69:L122" si="1">IF(COUNTA(E69),E69/H69,1)</f>
+        <v>1</v>
+      </c>
+      <c r="M69">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.14390530654429E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>4251</v>
       </c>
-      <c r="D69">
+      <c r="D70">
         <v>9059</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <v>577116</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <v>3644</v>
       </c>
-      <c r="G69">
+      <c r="G70">
         <v>7841</v>
       </c>
-      <c r="H69">
+      <c r="H70">
         <v>415410</v>
       </c>
-      <c r="I69" t="s">
-        <v>144</v>
-      </c>
-      <c r="K69">
+      <c r="I70" t="s">
+        <v>144</v>
+      </c>
+      <c r="K70">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.4986207799680335E-2</v>
       </c>
-      <c r="L69">
+      <c r="L70">
         <f t="shared" si="1"/>
         <v>1.3892684335957246</v>
       </c>
-      <c r="M69">
+      <c r="M70">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.4538751875747831E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>1991</v>
       </c>
-      <c r="D70">
+      <c r="D71">
         <v>1991</v>
       </c>
-      <c r="E70">
+      <c r="E71">
         <v>9764</v>
       </c>
-      <c r="F70">
+      <c r="F71">
         <v>7669</v>
       </c>
-      <c r="G70">
+      <c r="G71">
         <v>7669</v>
       </c>
-      <c r="H70">
+      <c r="H71">
         <v>126176</v>
       </c>
-      <c r="I70" t="s">
-        <v>144</v>
-      </c>
-      <c r="J70" s="9" t="s">
+      <c r="I71" t="s">
+        <v>144</v>
+      </c>
+      <c r="J71" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="K70">
+      <c r="K71">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>2.4631181855264811E-3</v>
       </c>
-      <c r="L70" s="1">
+      <c r="L71" s="1">
         <f t="shared" si="1"/>
         <v>7.7383971595232054E-2</v>
       </c>
-      <c r="M70">
+      <c r="M71">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.1453555583889911E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>20471</v>
       </c>
-      <c r="D71">
+      <c r="D72">
         <v>3278</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <v>4245692</v>
       </c>
-      <c r="F71">
+      <c r="F72">
         <v>18535</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>2826</v>
       </c>
-      <c r="H71">
+      <c r="H72">
         <v>829693</v>
       </c>
-      <c r="I71" t="s">
-        <v>144</v>
-      </c>
-      <c r="K71">
+      <c r="I72" t="s">
+        <v>144</v>
+      </c>
+      <c r="K72">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>6.3270385115103078E-2</v>
       </c>
-      <c r="L71">
+      <c r="L72">
         <f t="shared" si="1"/>
         <v>5.1171843079307644</v>
       </c>
-      <c r="M71">
+      <c r="M72">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.5839908850549762E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>16712</v>
       </c>
-      <c r="D72">
+      <c r="D73">
         <v>5337</v>
       </c>
-      <c r="E72">
+      <c r="E73">
         <v>182402</v>
       </c>
-      <c r="F72">
+      <c r="F73">
         <v>13149</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>3679</v>
       </c>
-      <c r="H72">
+      <c r="H73">
         <v>52079</v>
       </c>
-      <c r="I72" t="s">
-        <v>144</v>
-      </c>
-      <c r="K72">
+      <c r="I73" t="s">
+        <v>144</v>
+      </c>
+      <c r="K73">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>2.0450501673110744E-3</v>
       </c>
-      <c r="L72">
+      <c r="L73">
         <f t="shared" si="1"/>
         <v>3.5024098004954012</v>
       </c>
-      <c r="M72">
+      <c r="M73">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>1.0765646699212701E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>20540</v>
       </c>
-      <c r="D73">
+      <c r="D74">
         <v>6696</v>
       </c>
-      <c r="E73">
+      <c r="E74">
         <v>7870084</v>
       </c>
-      <c r="F73">
+      <c r="F74">
         <v>18565</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <v>4098</v>
       </c>
-      <c r="H73">
+      <c r="H74">
         <v>434311</v>
       </c>
-      <c r="I73" t="s">
-        <v>144</v>
-      </c>
-      <c r="K73">
+      <c r="I74" t="s">
+        <v>144</v>
+      </c>
+      <c r="K74">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.7222059355583242E-2</v>
       </c>
-      <c r="L73">
+      <c r="L74">
         <f t="shared" si="1"/>
         <v>18.120848884785328</v>
       </c>
-      <c r="M73">
+      <c r="M74">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>5.7086566305688388E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>9767</v>
       </c>
-      <c r="D74">
+      <c r="D75">
         <v>9619</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>160162</v>
       </c>
-      <c r="F74">
+      <c r="F75">
         <v>7758</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <v>8639</v>
       </c>
-      <c r="H74">
+      <c r="H75">
         <v>134408</v>
       </c>
-      <c r="I74" t="s">
-        <v>144</v>
-      </c>
-      <c r="K74">
+      <c r="I75" t="s">
+        <v>144</v>
+      </c>
+      <c r="K75">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>1.7047801145843595E-3</v>
       </c>
-      <c r="L74">
+      <c r="L75">
         <f t="shared" si="1"/>
         <v>1.1916106184155706</v>
       </c>
-      <c r="M74">
+      <c r="M75">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.0054501428962306E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>21859</v>
       </c>
-      <c r="D75">
+      <c r="D76">
         <v>3737</v>
       </c>
-      <c r="E75">
+      <c r="E76">
         <v>421067</v>
       </c>
-      <c r="F75">
+      <c r="F76">
         <v>15575</v>
       </c>
-      <c r="G75">
+      <c r="G76">
         <v>3551</v>
       </c>
-      <c r="H75">
+      <c r="H76">
         <v>417884</v>
       </c>
-      <c r="I75" t="s">
-        <v>144</v>
-      </c>
-      <c r="K75">
+      <c r="I76" t="s">
+        <v>144</v>
+      </c>
+      <c r="K76">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.1546338115660223E-3</v>
       </c>
-      <c r="L75">
+      <c r="L76">
         <f t="shared" si="1"/>
         <v>1.0076169463296034</v>
       </c>
-      <c r="M75">
+      <c r="M76">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>7.5557401821565425E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>4067</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D77" s="5">
         <v>3823</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E77" s="5">
         <v>7641</v>
       </c>
-      <c r="K76">
+      <c r="K77">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.9144138839492127E-4</v>
       </c>
-      <c r="L76" t="e">
+      <c r="L77" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M76" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+      <c r="M77" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>10957</v>
       </c>
-      <c r="D77">
+      <c r="D78">
         <v>23737</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E78" s="5">
         <v>146627</v>
       </c>
-      <c r="F77">
+      <c r="F78">
         <v>11164</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <v>51319</v>
       </c>
-      <c r="H77">
+      <c r="H78">
         <v>1257932</v>
       </c>
-      <c r="I77" t="s">
-        <v>144</v>
-      </c>
-      <c r="K77">
+      <c r="I78" t="s">
+        <v>144</v>
+      </c>
+      <c r="K78">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>5.6376285458378361E-4</v>
       </c>
-      <c r="L77" s="1">
+      <c r="L78" s="1">
         <f t="shared" si="1"/>
         <v>0.11656194452482328</v>
       </c>
-      <c r="M77">
+      <c r="M78">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>2.1956299798070017E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>16396</v>
       </c>
-      <c r="D78">
+      <c r="D79">
         <v>18180</v>
       </c>
-      <c r="E78">
+      <c r="E79">
         <v>1093028</v>
       </c>
-      <c r="F78">
+      <c r="F79">
         <v>16291</v>
       </c>
-      <c r="G78">
+      <c r="G79">
         <v>18511</v>
       </c>
-      <c r="H78">
+      <c r="H79">
         <v>1125042</v>
       </c>
-      <c r="I78" t="s">
-        <v>144</v>
-      </c>
-      <c r="K78">
+      <c r="I79" t="s">
+        <v>144</v>
+      </c>
+      <c r="K79">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>3.6669036505992633E-3</v>
       </c>
-      <c r="L78">
+      <c r="L79">
         <f t="shared" si="1"/>
         <v>0.97154417346196853</v>
       </c>
-      <c r="M78">
+      <c r="M79">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>3.7307067361755722E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>95</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>95</v>
       </c>
-      <c r="F79">
+      <c r="F80">
         <v>2716</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I80" t="s">
         <v>145</v>
       </c>
-      <c r="K79" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L79">
+      <c r="K80" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L80">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M79" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+      <c r="M80" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>13894</v>
       </c>
-      <c r="D80">
+      <c r="D81">
         <v>3000</v>
       </c>
-      <c r="E80">
+      <c r="E81">
         <v>188518</v>
       </c>
-      <c r="I80" t="s">
-        <v>144</v>
-      </c>
-      <c r="K80">
+      <c r="I81" t="s">
+        <v>144</v>
+      </c>
+      <c r="K81">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.5227676215152824E-3</v>
       </c>
-      <c r="L80" t="e">
+      <c r="L81" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M80" t="e">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="M81" t="e">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>10601</v>
       </c>
-      <c r="D81">
+      <c r="D82">
         <v>2333</v>
       </c>
-      <c r="E81">
+      <c r="E82">
         <v>113787</v>
       </c>
-      <c r="F81">
+      <c r="F82">
         <v>10237</v>
       </c>
-      <c r="G81">
+      <c r="G82">
         <v>1887</v>
       </c>
-      <c r="H81">
+      <c r="H82">
         <v>105556</v>
       </c>
-      <c r="I81" t="s">
-        <v>144</v>
-      </c>
-      <c r="K81">
+      <c r="I82" t="s">
+        <v>144</v>
+      </c>
+      <c r="K82">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>4.6007758408868329E-3</v>
       </c>
-      <c r="L81">
+      <c r="L82">
         <f t="shared" si="1"/>
         <v>1.0779775664102467</v>
       </c>
-      <c r="M81">
+      <c r="M82">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>5.4643476372038856E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>97</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F82">
+      <c r="C83">
+        <v>18240</v>
+      </c>
+      <c r="D83">
+        <v>57</v>
+      </c>
+      <c r="E83">
+        <v>51770</v>
+      </c>
+      <c r="F83">
         <v>18375</v>
       </c>
-      <c r="G82">
+      <c r="G83">
         <v>57</v>
       </c>
-      <c r="H82">
+      <c r="H83">
         <v>209475</v>
       </c>
-      <c r="I82" t="s">
-        <v>143</v>
-      </c>
-      <c r="K82" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L82">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M82">
-        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83">
-        <v>18218</v>
-      </c>
-      <c r="D83">
-        <v>4543</v>
-      </c>
-      <c r="E83">
-        <v>15151173</v>
-      </c>
-      <c r="F83">
-        <v>18028</v>
-      </c>
-      <c r="G83">
-        <v>2318</v>
-      </c>
-      <c r="H83">
-        <v>5898446</v>
-      </c>
       <c r="I83" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K83">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>0.1830639472969372</v>
+        <v>4.9794167436134192E-2</v>
       </c>
       <c r="L83">
         <f t="shared" si="1"/>
-        <v>2.5686719858077876</v>
+        <v>0.24714166368301707</v>
       </c>
       <c r="M83">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.14114861686729088</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>100</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>101</v>
+      <c r="A84" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84">
+        <v>18218</v>
+      </c>
+      <c r="D84">
+        <v>4543</v>
+      </c>
+      <c r="E84">
+        <v>15151173</v>
       </c>
       <c r="F84">
-        <v>18423</v>
+        <v>18028</v>
       </c>
       <c r="G84">
-        <v>79</v>
+        <v>2318</v>
       </c>
       <c r="H84">
-        <v>72970</v>
+        <v>5898446</v>
       </c>
       <c r="I84" t="s">
-        <v>143</v>
-      </c>
-      <c r="J84" s="7"/>
-      <c r="K84" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>144</v>
+      </c>
+      <c r="K84">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>0.1830639472969372</v>
       </c>
       <c r="L84">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5686719858077876</v>
       </c>
       <c r="M84">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0136833635995734E-2</v>
+        <v>0.14114861686729088</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>102</v>
+      <c r="B85" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="F85">
-        <v>18549</v>
+        <v>18423</v>
       </c>
       <c r="G85">
-        <v>430</v>
+        <v>79</v>
       </c>
       <c r="H85">
-        <v>398197</v>
+        <v>72970</v>
       </c>
       <c r="I85" t="s">
         <v>143</v>
       </c>
-      <c r="J85" s="7"/>
+      <c r="J85" s="6"/>
       <c r="K85" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4232,29 +4209,29 @@
       </c>
       <c r="M85">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9923960045486063E-2</v>
+        <v>5.0136833635995734E-2</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>103</v>
+      <c r="B86" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="F86">
-        <v>18480</v>
+        <v>18549</v>
       </c>
       <c r="G86">
-        <v>530</v>
+        <v>430</v>
       </c>
       <c r="H86">
-        <v>489769</v>
+        <v>398197</v>
       </c>
       <c r="I86" t="s">
         <v>143</v>
       </c>
-      <c r="J86" s="7"/>
+      <c r="J86" s="6"/>
       <c r="K86" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4265,29 +4242,29 @@
       </c>
       <c r="M86">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0005002858776446E-2</v>
+        <v>4.9923960045486063E-2</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>104</v>
+      <c r="B87" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="F87">
-        <v>18511</v>
+        <v>18480</v>
       </c>
       <c r="G87">
-        <v>1215</v>
+        <v>530</v>
       </c>
       <c r="H87">
-        <v>1124480</v>
+        <v>489769</v>
       </c>
       <c r="I87" t="s">
         <v>143</v>
       </c>
-      <c r="J87" s="7"/>
+      <c r="J87" s="6"/>
       <c r="K87" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4298,29 +4275,29 @@
       </c>
       <c r="M87">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9997187747114216E-2</v>
+        <v>5.0005002858776446E-2</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B88" s="6" t="s">
-        <v>105</v>
+      <c r="B88" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="F88">
-        <v>18478</v>
+        <v>18511</v>
       </c>
       <c r="G88">
-        <v>309</v>
+        <v>1215</v>
       </c>
       <c r="H88">
-        <v>284538</v>
+        <v>1124480</v>
       </c>
       <c r="I88" t="s">
         <v>143</v>
       </c>
-      <c r="J88" s="7"/>
+      <c r="J88" s="6"/>
       <c r="K88" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4331,29 +4308,29 @@
       </c>
       <c r="M88">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9834124442921887E-2</v>
+        <v>4.9997187747114216E-2</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>106</v>
+      <c r="B89" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="F89">
-        <v>18589</v>
+        <v>18478</v>
       </c>
       <c r="G89">
-        <v>45</v>
+        <v>309</v>
       </c>
       <c r="H89">
-        <v>41743</v>
+        <v>284538</v>
       </c>
       <c r="I89" t="s">
         <v>143</v>
       </c>
-      <c r="J89" s="7"/>
+      <c r="J89" s="6"/>
       <c r="K89" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4364,29 +4341,29 @@
       </c>
       <c r="M89">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9901674227888652E-2</v>
+        <v>4.9834124442921887E-2</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>107</v>
+      <c r="B90" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="F90">
-        <v>18340</v>
+        <v>18589</v>
       </c>
       <c r="G90">
-        <v>501</v>
+        <v>45</v>
       </c>
       <c r="H90">
-        <v>459393</v>
+        <v>41743</v>
       </c>
       <c r="I90" t="s">
         <v>143</v>
       </c>
-      <c r="J90" s="7"/>
+      <c r="J90" s="6"/>
       <c r="K90" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4397,29 +4374,29 @@
       </c>
       <c r="M90">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9997387993914025E-2</v>
+        <v>4.9901674227888652E-2</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>108</v>
+      <c r="B91" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F91">
-        <v>18875</v>
+        <v>18340</v>
       </c>
       <c r="G91">
-        <v>198</v>
+        <v>501</v>
       </c>
       <c r="H91">
-        <v>186087</v>
+        <v>459393</v>
       </c>
       <c r="I91" t="s">
         <v>143</v>
       </c>
-      <c r="J91" s="7"/>
+      <c r="J91" s="6"/>
       <c r="K91" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4430,29 +4407,29 @@
       </c>
       <c r="M91">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9792494481236203E-2</v>
+        <v>4.9997387993914025E-2</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>109</v>
+      <c r="B92" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F92">
-        <v>18471</v>
+        <v>18875</v>
       </c>
       <c r="G92">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="H92">
-        <v>159910</v>
+        <v>186087</v>
       </c>
       <c r="I92" t="s">
         <v>143</v>
       </c>
-      <c r="J92" s="7"/>
+      <c r="J92" s="6"/>
       <c r="K92" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4463,29 +4440,29 @@
       </c>
       <c r="M92">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.004251313494705E-2</v>
+        <v>4.9792494481236203E-2</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>110</v>
+      <c r="B93" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="F93">
-        <v>18648</v>
+        <v>18471</v>
       </c>
       <c r="G93">
-        <v>566</v>
+        <v>173</v>
       </c>
       <c r="H93">
-        <v>527943</v>
+        <v>159910</v>
       </c>
       <c r="I93" t="s">
         <v>143</v>
       </c>
-      <c r="J93" s="7"/>
+      <c r="J93" s="6"/>
       <c r="K93" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4496,29 +4473,29 @@
       </c>
       <c r="M93">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.001938460419026E-2</v>
+        <v>5.004251313494705E-2</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B94" s="6" t="s">
-        <v>111</v>
+      <c r="B94" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="F94">
-        <v>18540</v>
+        <v>18648</v>
       </c>
       <c r="G94">
-        <v>91</v>
+        <v>566</v>
       </c>
       <c r="H94">
-        <v>84676</v>
+        <v>527943</v>
       </c>
       <c r="I94" t="s">
         <v>143</v>
       </c>
-      <c r="J94" s="7"/>
+      <c r="J94" s="6"/>
       <c r="K94" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4529,29 +4506,29 @@
       </c>
       <c r="M94">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0189077373543396E-2</v>
+        <v>5.001938460419026E-2</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>112</v>
+      <c r="B95" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="F95">
-        <v>18665</v>
+        <v>18540</v>
       </c>
       <c r="G95">
-        <v>606</v>
+        <v>91</v>
       </c>
       <c r="H95">
-        <v>565628</v>
+        <v>84676</v>
       </c>
       <c r="I95" t="s">
         <v>143</v>
       </c>
-      <c r="J95" s="7"/>
+      <c r="J95" s="6"/>
       <c r="K95" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4562,29 +4539,29 @@
       </c>
       <c r="M95">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.000694015289555E-2</v>
+        <v>5.0189077373543396E-2</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="6" t="s">
-        <v>113</v>
+      <c r="B96" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F96">
-        <v>18546</v>
+        <v>18665</v>
       </c>
       <c r="G96">
-        <v>323</v>
+        <v>606</v>
       </c>
       <c r="H96">
-        <v>299781</v>
+        <v>565628</v>
       </c>
       <c r="I96" t="s">
         <v>143</v>
       </c>
-      <c r="J96" s="7"/>
+      <c r="J96" s="6"/>
       <c r="K96" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4595,29 +4572,29 @@
       </c>
       <c r="M96">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0043920580372658E-2</v>
+        <v>5.000694015289555E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B97" s="6" t="s">
-        <v>114</v>
+      <c r="B97" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="F97">
-        <v>18339</v>
+        <v>18546</v>
       </c>
       <c r="G97">
-        <v>423</v>
+        <v>323</v>
       </c>
       <c r="H97">
-        <v>387737</v>
+        <v>299781</v>
       </c>
       <c r="I97" t="s">
         <v>143</v>
       </c>
-      <c r="J97" s="7"/>
+      <c r="J97" s="6"/>
       <c r="K97" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4628,29 +4605,29 @@
       </c>
       <c r="M97">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9982874410063063E-2</v>
+        <v>5.0043920580372658E-2</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B98" s="6" t="s">
-        <v>115</v>
+      <c r="B98" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="F98">
-        <v>18508</v>
+        <v>18339</v>
       </c>
       <c r="G98">
-        <v>577</v>
+        <v>423</v>
       </c>
       <c r="H98">
-        <v>533911</v>
+        <v>387737</v>
       </c>
       <c r="I98" t="s">
         <v>143</v>
       </c>
-      <c r="J98" s="7"/>
+      <c r="J98" s="6"/>
       <c r="K98" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4661,29 +4638,29 @@
       </c>
       <c r="M98">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9995804896210513E-2</v>
+        <v>4.9982874410063063E-2</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>116</v>
+      <c r="B99" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="F99">
-        <v>18608</v>
+        <v>18508</v>
       </c>
       <c r="G99">
-        <v>552</v>
+        <v>577</v>
       </c>
       <c r="H99">
-        <v>513287</v>
+        <v>533911</v>
       </c>
       <c r="I99" t="s">
         <v>143</v>
       </c>
-      <c r="J99" s="7"/>
+      <c r="J99" s="6"/>
       <c r="K99" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4694,29 +4671,29 @@
       </c>
       <c r="M99">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9971396905803329E-2</v>
+        <v>4.9995804896210513E-2</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>117</v>
+      <c r="B100" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="F100">
-        <v>18967</v>
+        <v>18608</v>
       </c>
       <c r="G100">
-        <v>48</v>
+        <v>552</v>
       </c>
       <c r="H100">
-        <v>42973</v>
+        <v>513287</v>
       </c>
       <c r="I100" t="s">
         <v>143</v>
       </c>
-      <c r="J100" s="7"/>
+      <c r="J100" s="6"/>
       <c r="K100" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4727,29 +4704,29 @@
       </c>
       <c r="M100">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.7201499094919247E-2</v>
+        <v>4.9971396905803329E-2</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>118</v>
+      <c r="B101" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="F101">
-        <v>18545</v>
+        <v>18967</v>
       </c>
       <c r="G101">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="H101">
-        <v>81072</v>
+        <v>42973</v>
       </c>
       <c r="I101" t="s">
         <v>143</v>
       </c>
-      <c r="J101" s="7"/>
+      <c r="J101" s="6"/>
       <c r="K101" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4760,29 +4737,29 @@
       </c>
       <c r="M101">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0248696088731046E-2</v>
+        <v>4.7201499094919247E-2</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>119</v>
+      <c r="B102" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="F102">
-        <v>18621</v>
+        <v>18545</v>
       </c>
       <c r="G102">
-        <v>429</v>
+        <v>87</v>
       </c>
       <c r="H102">
-        <v>399505</v>
+        <v>81072</v>
       </c>
       <c r="I102" t="s">
         <v>143</v>
       </c>
-      <c r="J102" s="7"/>
+      <c r="J102" s="6"/>
       <c r="K102" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4793,29 +4770,29 @@
       </c>
       <c r="M102">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0010584085016178E-2</v>
+        <v>5.0248696088731046E-2</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>120</v>
+      <c r="B103" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F103">
-        <v>18493</v>
+        <v>18621</v>
       </c>
       <c r="G103">
-        <v>183</v>
+        <v>429</v>
       </c>
       <c r="H103">
-        <v>169642</v>
+        <v>399505</v>
       </c>
       <c r="I103" t="s">
         <v>143</v>
       </c>
-      <c r="J103" s="7"/>
+      <c r="J103" s="6"/>
       <c r="K103" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4826,29 +4803,29 @@
       </c>
       <c r="M103">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0127370598652153E-2</v>
+        <v>5.0010584085016178E-2</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B104" s="6" t="s">
-        <v>121</v>
+      <c r="B104" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="F104">
-        <v>18370</v>
+        <v>18493</v>
       </c>
       <c r="G104">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H104">
-        <v>172133</v>
+        <v>169642</v>
       </c>
       <c r="I104" t="s">
         <v>143</v>
       </c>
-      <c r="J104" s="7"/>
+      <c r="J104" s="6"/>
       <c r="K104" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4859,29 +4836,29 @@
       </c>
       <c r="M104">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0108727610408743E-2</v>
+        <v>5.0127370598652153E-2</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B105" s="6" t="s">
-        <v>122</v>
+      <c r="B105" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="F105">
-        <v>18528</v>
+        <v>18370</v>
       </c>
       <c r="G105">
-        <v>550</v>
+        <v>187</v>
       </c>
       <c r="H105">
-        <v>509464</v>
+        <v>172133</v>
       </c>
       <c r="I105" t="s">
         <v>143</v>
       </c>
-      <c r="J105" s="7"/>
+      <c r="J105" s="6"/>
       <c r="K105" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4892,29 +4869,29 @@
       </c>
       <c r="M105">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9994504631810328E-2</v>
+        <v>5.0108727610408743E-2</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B106" s="6" t="s">
-        <v>123</v>
+      <c r="B106" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="F106">
-        <v>18335</v>
+        <v>18528</v>
       </c>
       <c r="G106">
-        <v>177</v>
+        <v>550</v>
       </c>
       <c r="H106">
-        <v>162528</v>
+        <v>509464</v>
       </c>
       <c r="I106" t="s">
         <v>143</v>
       </c>
-      <c r="J106" s="7"/>
+      <c r="J106" s="6"/>
       <c r="K106" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4925,29 +4902,29 @@
       </c>
       <c r="M106">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0081117433083897E-2</v>
+        <v>4.9994504631810328E-2</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B107" s="6" t="s">
-        <v>124</v>
+      <c r="B107" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="F107">
-        <v>18584</v>
+        <v>18335</v>
       </c>
       <c r="G107">
-        <v>265</v>
+        <v>177</v>
       </c>
       <c r="H107">
-        <v>245886</v>
+        <v>162528</v>
       </c>
       <c r="I107" t="s">
         <v>143</v>
       </c>
-      <c r="J107" s="7"/>
+      <c r="J107" s="6"/>
       <c r="K107" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4958,29 +4935,29 @@
       </c>
       <c r="M107">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9928524435708541E-2</v>
+        <v>5.0081117433083897E-2</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B108" s="6" t="s">
-        <v>125</v>
+      <c r="B108" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F108">
-        <v>18612</v>
+        <v>18584</v>
       </c>
       <c r="G108">
-        <v>473</v>
+        <v>265</v>
       </c>
       <c r="H108">
-        <v>439949</v>
+        <v>245886</v>
       </c>
       <c r="I108" t="s">
         <v>143</v>
       </c>
-      <c r="J108" s="7"/>
+      <c r="J108" s="6"/>
       <c r="K108" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -4991,29 +4968,29 @@
       </c>
       <c r="M108">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9974464631924932E-2</v>
+        <v>4.9928524435708541E-2</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="6" t="s">
-        <v>126</v>
+      <c r="B109" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="F109">
-        <v>18917</v>
+        <v>18612</v>
       </c>
       <c r="G109">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="H109">
-        <v>428467</v>
+        <v>439949</v>
       </c>
       <c r="I109" t="s">
         <v>143</v>
       </c>
-      <c r="J109" s="7"/>
+      <c r="J109" s="6"/>
       <c r="K109" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5024,29 +5001,29 @@
       </c>
       <c r="M109">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9999644082474377E-2</v>
+        <v>4.9974464631924932E-2</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B110" s="6" t="s">
-        <v>127</v>
+      <c r="B110" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F110">
-        <v>18742</v>
+        <v>18917</v>
       </c>
       <c r="G110">
-        <v>156</v>
+        <v>453</v>
       </c>
       <c r="H110">
-        <v>145048</v>
+        <v>428467</v>
       </c>
       <c r="I110" t="s">
         <v>143</v>
       </c>
-      <c r="J110" s="7"/>
+      <c r="J110" s="6"/>
       <c r="K110" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5057,29 +5034,29 @@
       </c>
       <c r="M110">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9610226859186417E-2</v>
+        <v>4.9999644082474377E-2</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B111" s="6" t="s">
-        <v>128</v>
+      <c r="B111" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="F111">
-        <v>18514</v>
+        <v>18742</v>
       </c>
       <c r="G111">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="H111">
-        <v>112695</v>
+        <v>145048</v>
       </c>
       <c r="I111" t="s">
         <v>143</v>
       </c>
-      <c r="J111" s="7"/>
+      <c r="J111" s="6"/>
       <c r="K111" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5090,29 +5067,29 @@
       </c>
       <c r="M111">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9893567473086382E-2</v>
+        <v>4.9610226859186417E-2</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B112" s="6" t="s">
-        <v>129</v>
+      <c r="B112" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="F112">
-        <v>18371</v>
+        <v>18514</v>
       </c>
       <c r="G112">
-        <v>572</v>
+        <v>122</v>
       </c>
       <c r="H112">
-        <v>525419</v>
+        <v>112695</v>
       </c>
       <c r="I112" t="s">
         <v>143</v>
       </c>
-      <c r="J112" s="7"/>
+      <c r="J112" s="6"/>
       <c r="K112" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5123,29 +5100,29 @@
       </c>
       <c r="M112">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0000799374812763E-2</v>
+        <v>4.9893567473086382E-2</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B113" s="6" t="s">
-        <v>130</v>
+      <c r="B113" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F113">
-        <v>18821</v>
+        <v>18371</v>
       </c>
       <c r="G113">
-        <v>57</v>
+        <v>572</v>
       </c>
       <c r="H113">
-        <v>56384</v>
+        <v>525419</v>
       </c>
       <c r="I113" t="s">
         <v>143</v>
       </c>
-      <c r="J113" s="7"/>
+      <c r="J113" s="6"/>
       <c r="K113" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5156,29 +5133,29 @@
       </c>
       <c r="M113">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.2557939666125091E-2</v>
+        <v>5.0000799374812763E-2</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B114" s="6" t="s">
-        <v>131</v>
+      <c r="B114" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="F114">
-        <v>18689</v>
+        <v>18821</v>
       </c>
       <c r="G114">
-        <v>581</v>
+        <v>57</v>
       </c>
       <c r="H114">
-        <v>542785</v>
+        <v>56384</v>
       </c>
       <c r="I114" t="s">
         <v>143</v>
       </c>
-      <c r="J114" s="7"/>
+      <c r="J114" s="6"/>
       <c r="K114" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5189,29 +5166,29 @@
       </c>
       <c r="M114">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>4.9987986158802442E-2</v>
+        <v>5.2557939666125091E-2</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>132</v>
+      <c r="B115" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="F115">
-        <v>18136</v>
+        <v>18689</v>
       </c>
       <c r="G115">
-        <v>80</v>
+        <v>581</v>
       </c>
       <c r="H115">
-        <v>73121</v>
+        <v>542785</v>
       </c>
       <c r="I115" t="s">
         <v>143</v>
       </c>
-      <c r="J115" s="7"/>
+      <c r="J115" s="6"/>
       <c r="K115" t="e">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
         <v>#DIV/0!</v>
@@ -5222,252 +5199,285 @@
       </c>
       <c r="M115">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>5.0397689677988529E-2</v>
+        <v>4.9987986158802442E-2</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C116">
-        <v>5213</v>
-      </c>
-      <c r="D116">
-        <v>24504</v>
-      </c>
-      <c r="E116">
-        <v>850425</v>
+      <c r="A116" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="F116">
-        <v>5309</v>
+        <v>18136</v>
       </c>
       <c r="G116">
-        <v>22128</v>
+        <v>80</v>
       </c>
       <c r="H116">
-        <v>848829</v>
+        <v>73121</v>
       </c>
       <c r="I116" t="s">
-        <v>144</v>
-      </c>
-      <c r="K116">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>6.657502067178171E-3</v>
+        <v>143</v>
+      </c>
+      <c r="J116" s="6"/>
+      <c r="K116" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L116">
         <f t="shared" si="1"/>
-        <v>1.0018802373622955</v>
+        <v>1</v>
       </c>
       <c r="M116">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>7.2254569962438443E-3</v>
+        <v>5.0397689677988529E-2</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>136</v>
+      <c r="A117" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C117">
-        <v>18025</v>
+        <v>5213</v>
       </c>
       <c r="D117">
-        <v>64</v>
+        <v>24504</v>
       </c>
       <c r="E117">
-        <v>58693</v>
+        <v>850425</v>
       </c>
       <c r="F117">
-        <v>17661</v>
+        <v>5309</v>
       </c>
       <c r="G117">
-        <v>56</v>
+        <v>22128</v>
       </c>
       <c r="H117">
-        <v>197848</v>
+        <v>848829</v>
       </c>
       <c r="I117" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K117">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>5.0878120665742023E-2</v>
+        <v>6.657502067178171E-3</v>
       </c>
       <c r="L117">
         <f t="shared" si="1"/>
-        <v>0.29665702963891472</v>
+        <v>1.0018802373622955</v>
       </c>
       <c r="M117">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.20004529754827019</v>
+        <v>7.2254569962438443E-3</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="s">
+      <c r="A118" s="9" t="s">
         <v>135</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C118">
-        <v>9702</v>
+        <v>18025</v>
       </c>
       <c r="D118">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="E118">
-        <v>118293</v>
+        <v>58693</v>
       </c>
       <c r="F118">
-        <v>9490</v>
+        <v>17661</v>
       </c>
       <c r="G118">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="H118">
-        <v>117708</v>
+        <v>197848</v>
       </c>
       <c r="I118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K118">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>8.9651769798828621E-2</v>
+        <v>5.0878120665742023E-2</v>
       </c>
       <c r="L118">
         <f t="shared" si="1"/>
-        <v>1.0049699255785502</v>
+        <v>0.29665702963891472</v>
       </c>
       <c r="M118">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.11484603676384499</v>
+        <v>0.20004529754827019</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
+      <c r="A119" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>138</v>
+      <c r="B119" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="C119">
-        <v>18362</v>
+        <v>9702</v>
       </c>
       <c r="D119">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="E119">
-        <v>56832</v>
+        <v>118293</v>
       </c>
       <c r="F119">
-        <v>18200</v>
+        <v>9490</v>
       </c>
       <c r="G119">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="H119">
-        <v>134717</v>
+        <v>117708</v>
       </c>
       <c r="I119" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K119">
         <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>4.9920769049685364E-2</v>
+        <v>8.9651769798828621E-2</v>
       </c>
       <c r="L119">
         <f t="shared" si="1"/>
-        <v>0.42186212578961824</v>
+        <v>1.0049699255785502</v>
       </c>
       <c r="M119">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>0.20005494505494506</v>
+        <v>0.11484603676384499</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>139</v>
-      </c>
-      <c r="B120" t="s">
-        <v>140</v>
+      <c r="A120" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C120">
+        <v>18362</v>
+      </c>
+      <c r="D120">
+        <v>62</v>
+      </c>
+      <c r="E120">
+        <v>56832</v>
       </c>
       <c r="F120">
-        <v>1212</v>
+        <v>18200</v>
       </c>
       <c r="G120">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H120">
-        <v>2338</v>
+        <v>134717</v>
       </c>
       <c r="I120" t="s">
-        <v>149</v>
-      </c>
-      <c r="J120" t="s">
-        <v>157</v>
-      </c>
-      <c r="K120" t="e">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>#DIV/0!</v>
+        <v>143</v>
+      </c>
+      <c r="K120">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>4.9920769049685364E-2</v>
       </c>
       <c r="L120">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.42186212578961824</v>
       </c>
       <c r="M120">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
-        <v>9.6452145214521445E-2</v>
+        <v>0.20005494505494506</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A121" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C121">
-        <v>7183</v>
-      </c>
-      <c r="D121">
-        <v>621</v>
-      </c>
-      <c r="E121">
-        <v>26332</v>
+      <c r="A121" t="s">
+        <v>139</v>
+      </c>
+      <c r="B121" t="s">
+        <v>140</v>
       </c>
       <c r="F121">
-        <v>5388</v>
+        <v>1212</v>
       </c>
       <c r="G121">
-        <v>372</v>
+        <v>20</v>
       </c>
       <c r="H121">
-        <v>15503</v>
+        <v>2338</v>
       </c>
       <c r="I121" t="s">
-        <v>144</v>
-      </c>
-      <c r="K121">
-        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
-        <v>5.9031848099029673E-3</v>
+        <v>149</v>
+      </c>
+      <c r="J121" t="s">
+        <v>157</v>
+      </c>
+      <c r="K121" t="e">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="L121">
         <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M121">
+        <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
+        <v>9.6452145214521445E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C122">
+        <v>7183</v>
+      </c>
+      <c r="D122">
+        <v>621</v>
+      </c>
+      <c r="E122">
+        <v>26332</v>
+      </c>
+      <c r="F122">
+        <v>5388</v>
+      </c>
+      <c r="G122">
+        <v>372</v>
+      </c>
+      <c r="H122">
+        <v>15503</v>
+      </c>
+      <c r="I122" t="s">
+        <v>144</v>
+      </c>
+      <c r="K122">
+        <f>Table1[[#This Row],[Statistical]]/Table1[[#This Row],[Genes]]/Table1[[#This Row],[Attributes]]</f>
+        <v>5.9031848099029673E-3</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="1"/>
         <v>1.6985099658130685</v>
       </c>
-      <c r="M121">
+      <c r="M122">
         <f>Table1[[#This Row],[Number Of Statistically Significant Associations]]/(Table1[[#This Row],[Number Of Genes]]*Table1[[#This Row],[Number Of Attributes]])</f>
         <v>7.7347311029687636E-3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="L2:L121">
+  <conditionalFormatting sqref="L2:L122">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>1.05</formula>
     </cfRule>

</xml_diff>

<commit_message>
revised ClinVar-DSigDB, added disclaimer sentence in others
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059E7BDF-6E1E-474F-BC3F-91C188D17B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7C30CC-48F2-4E26-B9EF-FEE48E13EE39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,8 +2442,15 @@
       <c r="B39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="C39">
+        <v>17883</v>
+      </c>
+      <c r="D39">
+        <v>48</v>
+      </c>
+      <c r="E39" s="5">
+        <v>132898</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">

</xml_diff>

<commit_message>
changed url format, revised rest of appyters
</commit_message>
<xml_diff>
--- a/Updated Scripts.xlsx
+++ b/Updated Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\charlesdai\Projects\Harmonizome-Data-Processing-Appyters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960C5424-7254-42D8-B0F6-8BBB75AE690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6755CC88-8864-43FA-A43C-1B2523ECC300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CC157D8-2979-47DE-93ED-2C75C5E1B133}"/>
   </bookViews>
@@ -1028,8 +1028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524E01FC-6AC0-4B00-8398-68BEEE66F31D}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2429,11 +2429,18 @@
       <c r="A38" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="C38">
+        <v>7983</v>
+      </c>
+      <c r="D38">
+        <v>13763</v>
+      </c>
+      <c r="E38" s="5">
+        <v>5484617</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">

</xml_diff>